<commit_message>
Fix wrong phone format in excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/법인 회원 업로드.xlsx
+++ b/src/main/resources/법인 회원 업로드.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A33E91-5CFA-48AA-82A6-E2052996E08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -34,31 +43,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -69,38 +79,48 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -290,29 +310,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H13:H14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="12.63"/>
-    <col customWidth="1" min="3" max="3" width="23.75"/>
-    <col customWidth="1" min="4" max="4" width="22.25"/>
-    <col customWidth="1" min="5" max="5" width="29.75"/>
-    <col customWidth="1" min="6" max="6" width="22.25"/>
+    <col min="1" max="2" width="12.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="22.21875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="29.77734375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="22.21875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -321,3456 +345,3454 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="D2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="D3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="D4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="D5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="D6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="D7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="D8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="D9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="D10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="D11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="D12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="D13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="D14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="D15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="D16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="D17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="D18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="D19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="D20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="D21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="D22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="D23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="D25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="D26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="D27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="D28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="D30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="D31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="D32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="D33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="D34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="D35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="D36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
       <c r="D37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
       <c r="D38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="D39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
       <c r="D40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
       <c r="D41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="D42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="D43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
       <c r="D44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
       <c r="D45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="D46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="D47" s="4"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
       <c r="D48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
       <c r="D49" s="4"/>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="D50" s="4"/>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
       <c r="D51" s="4"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="D52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
       <c r="D53" s="4"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
       <c r="D54" s="4"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="D55" s="4"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
       <c r="D56" s="4"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
       <c r="D57" s="4"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
       <c r="D58" s="4"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
       <c r="D59" s="4"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="D60" s="4"/>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
       <c r="D61" s="4"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
       <c r="D62" s="4"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="D63" s="4"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
       <c r="D64" s="4"/>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="5"/>
       <c r="D65" s="4"/>
       <c r="F65" s="4"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="5"/>
       <c r="D66" s="4"/>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="5"/>
       <c r="D67" s="4"/>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="5"/>
       <c r="D68" s="4"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="5"/>
       <c r="D69" s="4"/>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="5"/>
       <c r="D70" s="4"/>
       <c r="F70" s="4"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
       <c r="D71" s="4"/>
       <c r="F71" s="4"/>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="5"/>
       <c r="D72" s="4"/>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
       <c r="D73" s="4"/>
       <c r="F73" s="4"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
       <c r="D74" s="4"/>
       <c r="F74" s="4"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
       <c r="D75" s="4"/>
       <c r="F75" s="4"/>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
+    <row r="76" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
       <c r="D76" s="4"/>
       <c r="F76" s="4"/>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
+    <row r="77" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="5"/>
       <c r="D77" s="4"/>
       <c r="F77" s="4"/>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
+    <row r="78" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
       <c r="D78" s="4"/>
       <c r="F78" s="4"/>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
+    <row r="79" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
       <c r="D79" s="4"/>
       <c r="F79" s="4"/>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
+    <row r="80" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
       <c r="D80" s="4"/>
       <c r="F80" s="4"/>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
+    <row r="81" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
       <c r="D81" s="4"/>
       <c r="F81" s="4"/>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
+    <row r="82" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="5"/>
       <c r="D82" s="4"/>
       <c r="F82" s="4"/>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
+    <row r="83" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="5"/>
       <c r="D83" s="4"/>
       <c r="F83" s="4"/>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
+    <row r="84" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="5"/>
       <c r="D84" s="4"/>
       <c r="F84" s="4"/>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="5"/>
       <c r="D85" s="4"/>
       <c r="F85" s="4"/>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="5"/>
       <c r="D86" s="4"/>
       <c r="F86" s="4"/>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
+    <row r="87" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="5"/>
       <c r="D87" s="4"/>
       <c r="F87" s="4"/>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
+    <row r="88" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="5"/>
       <c r="D88" s="4"/>
       <c r="F88" s="4"/>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
+    <row r="89" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="5"/>
       <c r="D89" s="4"/>
       <c r="F89" s="4"/>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
+    <row r="90" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="5"/>
       <c r="D90" s="4"/>
       <c r="F90" s="4"/>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
+    <row r="91" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="5"/>
       <c r="D91" s="4"/>
       <c r="F91" s="4"/>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
+    <row r="92" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="5"/>
       <c r="D92" s="4"/>
       <c r="F92" s="4"/>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
+    <row r="93" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="5"/>
       <c r="D93" s="4"/>
       <c r="F93" s="4"/>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
+    <row r="94" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="5"/>
       <c r="D94" s="4"/>
       <c r="F94" s="4"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
+    <row r="95" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="5"/>
       <c r="D95" s="4"/>
       <c r="F95" s="4"/>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
+    <row r="96" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="5"/>
       <c r="D96" s="4"/>
       <c r="F96" s="4"/>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
+    <row r="97" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="5"/>
       <c r="D97" s="4"/>
       <c r="F97" s="4"/>
     </row>
-    <row r="98" ht="15.75" customHeight="1">
+    <row r="98" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="5"/>
       <c r="D98" s="4"/>
       <c r="F98" s="4"/>
     </row>
-    <row r="99" ht="15.75" customHeight="1">
+    <row r="99" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="5"/>
       <c r="D99" s="4"/>
       <c r="F99" s="4"/>
     </row>
-    <row r="100" ht="15.75" customHeight="1">
+    <row r="100" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="5"/>
       <c r="D100" s="4"/>
       <c r="F100" s="4"/>
     </row>
-    <row r="101" ht="15.75" customHeight="1">
+    <row r="101" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="5"/>
       <c r="D101" s="4"/>
       <c r="F101" s="4"/>
     </row>
-    <row r="102" ht="15.75" customHeight="1">
+    <row r="102" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="5"/>
       <c r="D102" s="4"/>
       <c r="F102" s="4"/>
     </row>
-    <row r="103" ht="15.75" customHeight="1">
+    <row r="103" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="5"/>
       <c r="D103" s="4"/>
       <c r="F103" s="4"/>
     </row>
-    <row r="104" ht="15.75" customHeight="1">
+    <row r="104" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="5"/>
       <c r="D104" s="4"/>
       <c r="F104" s="4"/>
     </row>
-    <row r="105" ht="15.75" customHeight="1">
+    <row r="105" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="5"/>
       <c r="D105" s="4"/>
       <c r="F105" s="4"/>
     </row>
-    <row r="106" ht="15.75" customHeight="1">
+    <row r="106" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="5"/>
       <c r="D106" s="4"/>
       <c r="F106" s="4"/>
     </row>
-    <row r="107" ht="15.75" customHeight="1">
+    <row r="107" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="5"/>
       <c r="D107" s="4"/>
       <c r="F107" s="4"/>
     </row>
-    <row r="108" ht="15.75" customHeight="1">
+    <row r="108" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="5"/>
       <c r="D108" s="4"/>
       <c r="F108" s="4"/>
     </row>
-    <row r="109" ht="15.75" customHeight="1">
+    <row r="109" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="5"/>
       <c r="D109" s="4"/>
       <c r="F109" s="4"/>
     </row>
-    <row r="110" ht="15.75" customHeight="1">
+    <row r="110" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="5"/>
       <c r="D110" s="4"/>
       <c r="F110" s="4"/>
     </row>
-    <row r="111" ht="15.75" customHeight="1">
+    <row r="111" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="5"/>
       <c r="D111" s="4"/>
       <c r="F111" s="4"/>
     </row>
-    <row r="112" ht="15.75" customHeight="1">
+    <row r="112" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="5"/>
       <c r="D112" s="4"/>
       <c r="F112" s="4"/>
     </row>
-    <row r="113" ht="15.75" customHeight="1">
+    <row r="113" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="5"/>
       <c r="D113" s="4"/>
       <c r="F113" s="4"/>
     </row>
-    <row r="114" ht="15.75" customHeight="1">
+    <row r="114" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="5"/>
       <c r="D114" s="4"/>
       <c r="F114" s="4"/>
     </row>
-    <row r="115" ht="15.75" customHeight="1">
+    <row r="115" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="5"/>
       <c r="D115" s="4"/>
       <c r="F115" s="4"/>
     </row>
-    <row r="116" ht="15.75" customHeight="1">
+    <row r="116" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="5"/>
       <c r="D116" s="4"/>
       <c r="F116" s="4"/>
     </row>
-    <row r="117" ht="15.75" customHeight="1">
+    <row r="117" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="5"/>
       <c r="D117" s="4"/>
       <c r="F117" s="4"/>
     </row>
-    <row r="118" ht="15.75" customHeight="1">
+    <row r="118" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="5"/>
       <c r="D118" s="4"/>
       <c r="F118" s="4"/>
     </row>
-    <row r="119" ht="15.75" customHeight="1">
+    <row r="119" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="5"/>
       <c r="D119" s="4"/>
       <c r="F119" s="4"/>
     </row>
-    <row r="120" ht="15.75" customHeight="1">
+    <row r="120" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="5"/>
       <c r="D120" s="4"/>
       <c r="F120" s="4"/>
     </row>
-    <row r="121" ht="15.75" customHeight="1">
+    <row r="121" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="5"/>
       <c r="D121" s="4"/>
       <c r="F121" s="4"/>
     </row>
-    <row r="122" ht="15.75" customHeight="1">
+    <row r="122" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="5"/>
       <c r="D122" s="4"/>
       <c r="F122" s="4"/>
     </row>
-    <row r="123" ht="15.75" customHeight="1">
+    <row r="123" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="5"/>
       <c r="D123" s="4"/>
       <c r="F123" s="4"/>
     </row>
-    <row r="124" ht="15.75" customHeight="1">
+    <row r="124" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="5"/>
       <c r="D124" s="4"/>
       <c r="F124" s="4"/>
     </row>
-    <row r="125" ht="15.75" customHeight="1">
+    <row r="125" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="5"/>
       <c r="D125" s="4"/>
       <c r="F125" s="4"/>
     </row>
-    <row r="126" ht="15.75" customHeight="1">
+    <row r="126" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="5"/>
       <c r="D126" s="4"/>
       <c r="F126" s="4"/>
     </row>
-    <row r="127" ht="15.75" customHeight="1">
+    <row r="127" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="5"/>
       <c r="D127" s="4"/>
       <c r="F127" s="4"/>
     </row>
-    <row r="128" ht="15.75" customHeight="1">
+    <row r="128" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="5"/>
       <c r="D128" s="4"/>
       <c r="F128" s="4"/>
     </row>
-    <row r="129" ht="15.75" customHeight="1">
+    <row r="129" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="5"/>
       <c r="D129" s="4"/>
       <c r="F129" s="4"/>
     </row>
-    <row r="130" ht="15.75" customHeight="1">
+    <row r="130" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="5"/>
       <c r="D130" s="4"/>
       <c r="F130" s="4"/>
     </row>
-    <row r="131" ht="15.75" customHeight="1">
+    <row r="131" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="5"/>
       <c r="D131" s="4"/>
       <c r="F131" s="4"/>
     </row>
-    <row r="132" ht="15.75" customHeight="1">
+    <row r="132" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="5"/>
       <c r="D132" s="4"/>
       <c r="F132" s="4"/>
     </row>
-    <row r="133" ht="15.75" customHeight="1">
+    <row r="133" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="5"/>
       <c r="D133" s="4"/>
       <c r="F133" s="4"/>
     </row>
-    <row r="134" ht="15.75" customHeight="1">
+    <row r="134" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="5"/>
       <c r="D134" s="4"/>
       <c r="F134" s="4"/>
     </row>
-    <row r="135" ht="15.75" customHeight="1">
+    <row r="135" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="5"/>
       <c r="D135" s="4"/>
       <c r="F135" s="4"/>
     </row>
-    <row r="136" ht="15.75" customHeight="1">
+    <row r="136" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="5"/>
       <c r="D136" s="4"/>
       <c r="F136" s="4"/>
     </row>
-    <row r="137" ht="15.75" customHeight="1">
+    <row r="137" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="5"/>
       <c r="D137" s="4"/>
       <c r="F137" s="4"/>
     </row>
-    <row r="138" ht="15.75" customHeight="1">
+    <row r="138" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="5"/>
       <c r="D138" s="4"/>
       <c r="F138" s="4"/>
     </row>
-    <row r="139" ht="15.75" customHeight="1">
+    <row r="139" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="5"/>
       <c r="D139" s="4"/>
       <c r="F139" s="4"/>
     </row>
-    <row r="140" ht="15.75" customHeight="1">
+    <row r="140" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="5"/>
       <c r="D140" s="4"/>
       <c r="F140" s="4"/>
     </row>
-    <row r="141" ht="15.75" customHeight="1">
+    <row r="141" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" s="5"/>
       <c r="D141" s="4"/>
       <c r="F141" s="4"/>
     </row>
-    <row r="142" ht="15.75" customHeight="1">
+    <row r="142" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B142" s="5"/>
       <c r="D142" s="4"/>
       <c r="F142" s="4"/>
     </row>
-    <row r="143" ht="15.75" customHeight="1">
+    <row r="143" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" s="5"/>
       <c r="D143" s="4"/>
       <c r="F143" s="4"/>
     </row>
-    <row r="144" ht="15.75" customHeight="1">
+    <row r="144" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="5"/>
       <c r="D144" s="4"/>
       <c r="F144" s="4"/>
     </row>
-    <row r="145" ht="15.75" customHeight="1">
+    <row r="145" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="5"/>
       <c r="D145" s="4"/>
       <c r="F145" s="4"/>
     </row>
-    <row r="146" ht="15.75" customHeight="1">
+    <row r="146" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="5"/>
       <c r="D146" s="4"/>
       <c r="F146" s="4"/>
     </row>
-    <row r="147" ht="15.75" customHeight="1">
+    <row r="147" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="5"/>
       <c r="D147" s="4"/>
       <c r="F147" s="4"/>
     </row>
-    <row r="148" ht="15.75" customHeight="1">
+    <row r="148" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="5"/>
       <c r="D148" s="4"/>
       <c r="F148" s="4"/>
     </row>
-    <row r="149" ht="15.75" customHeight="1">
+    <row r="149" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="5"/>
       <c r="D149" s="4"/>
       <c r="F149" s="4"/>
     </row>
-    <row r="150" ht="15.75" customHeight="1">
+    <row r="150" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="5"/>
       <c r="D150" s="4"/>
       <c r="F150" s="4"/>
     </row>
-    <row r="151" ht="15.75" customHeight="1">
+    <row r="151" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="5"/>
       <c r="D151" s="4"/>
       <c r="F151" s="4"/>
     </row>
-    <row r="152" ht="15.75" customHeight="1">
+    <row r="152" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="5"/>
       <c r="D152" s="4"/>
       <c r="F152" s="4"/>
     </row>
-    <row r="153" ht="15.75" customHeight="1">
+    <row r="153" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="5"/>
       <c r="D153" s="4"/>
       <c r="F153" s="4"/>
     </row>
-    <row r="154" ht="15.75" customHeight="1">
+    <row r="154" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="5"/>
       <c r="D154" s="4"/>
       <c r="F154" s="4"/>
     </row>
-    <row r="155" ht="15.75" customHeight="1">
+    <row r="155" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="5"/>
       <c r="D155" s="4"/>
       <c r="F155" s="4"/>
     </row>
-    <row r="156" ht="15.75" customHeight="1">
+    <row r="156" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="5"/>
       <c r="D156" s="4"/>
       <c r="F156" s="4"/>
     </row>
-    <row r="157" ht="15.75" customHeight="1">
+    <row r="157" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="5"/>
       <c r="D157" s="4"/>
       <c r="F157" s="4"/>
     </row>
-    <row r="158" ht="15.75" customHeight="1">
+    <row r="158" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="5"/>
       <c r="D158" s="4"/>
       <c r="F158" s="4"/>
     </row>
-    <row r="159" ht="15.75" customHeight="1">
+    <row r="159" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="5"/>
       <c r="D159" s="4"/>
       <c r="F159" s="4"/>
     </row>
-    <row r="160" ht="15.75" customHeight="1">
+    <row r="160" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" s="5"/>
       <c r="D160" s="4"/>
       <c r="F160" s="4"/>
     </row>
-    <row r="161" ht="15.75" customHeight="1">
+    <row r="161" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" s="5"/>
       <c r="D161" s="4"/>
       <c r="F161" s="4"/>
     </row>
-    <row r="162" ht="15.75" customHeight="1">
+    <row r="162" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" s="5"/>
       <c r="D162" s="4"/>
       <c r="F162" s="4"/>
     </row>
-    <row r="163" ht="15.75" customHeight="1">
+    <row r="163" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="5"/>
       <c r="D163" s="4"/>
       <c r="F163" s="4"/>
     </row>
-    <row r="164" ht="15.75" customHeight="1">
+    <row r="164" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" s="5"/>
       <c r="D164" s="4"/>
       <c r="F164" s="4"/>
     </row>
-    <row r="165" ht="15.75" customHeight="1">
+    <row r="165" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="5"/>
       <c r="D165" s="4"/>
       <c r="F165" s="4"/>
     </row>
-    <row r="166" ht="15.75" customHeight="1">
+    <row r="166" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="5"/>
       <c r="D166" s="4"/>
       <c r="F166" s="4"/>
     </row>
-    <row r="167" ht="15.75" customHeight="1">
+    <row r="167" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="5"/>
       <c r="D167" s="4"/>
       <c r="F167" s="4"/>
     </row>
-    <row r="168" ht="15.75" customHeight="1">
+    <row r="168" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" s="5"/>
       <c r="D168" s="4"/>
       <c r="F168" s="4"/>
     </row>
-    <row r="169" ht="15.75" customHeight="1">
+    <row r="169" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="5"/>
       <c r="D169" s="4"/>
       <c r="F169" s="4"/>
     </row>
-    <row r="170" ht="15.75" customHeight="1">
+    <row r="170" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="5"/>
       <c r="D170" s="4"/>
       <c r="F170" s="4"/>
     </row>
-    <row r="171" ht="15.75" customHeight="1">
+    <row r="171" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="5"/>
       <c r="D171" s="4"/>
       <c r="F171" s="4"/>
     </row>
-    <row r="172" ht="15.75" customHeight="1">
+    <row r="172" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="5"/>
       <c r="D172" s="4"/>
       <c r="F172" s="4"/>
     </row>
-    <row r="173" ht="15.75" customHeight="1">
+    <row r="173" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="5"/>
       <c r="D173" s="4"/>
       <c r="F173" s="4"/>
     </row>
-    <row r="174" ht="15.75" customHeight="1">
+    <row r="174" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" s="5"/>
       <c r="D174" s="4"/>
       <c r="F174" s="4"/>
     </row>
-    <row r="175" ht="15.75" customHeight="1">
+    <row r="175" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="5"/>
       <c r="D175" s="4"/>
       <c r="F175" s="4"/>
     </row>
-    <row r="176" ht="15.75" customHeight="1">
+    <row r="176" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="5"/>
       <c r="D176" s="4"/>
       <c r="F176" s="4"/>
     </row>
-    <row r="177" ht="15.75" customHeight="1">
+    <row r="177" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="5"/>
       <c r="D177" s="4"/>
       <c r="F177" s="4"/>
     </row>
-    <row r="178" ht="15.75" customHeight="1">
+    <row r="178" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" s="5"/>
       <c r="D178" s="4"/>
       <c r="F178" s="4"/>
     </row>
-    <row r="179" ht="15.75" customHeight="1">
+    <row r="179" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="5"/>
       <c r="D179" s="4"/>
       <c r="F179" s="4"/>
     </row>
-    <row r="180" ht="15.75" customHeight="1">
+    <row r="180" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="5"/>
       <c r="D180" s="4"/>
       <c r="F180" s="4"/>
     </row>
-    <row r="181" ht="15.75" customHeight="1">
+    <row r="181" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" s="5"/>
       <c r="D181" s="4"/>
       <c r="F181" s="4"/>
     </row>
-    <row r="182" ht="15.75" customHeight="1">
+    <row r="182" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="5"/>
       <c r="D182" s="4"/>
       <c r="F182" s="4"/>
     </row>
-    <row r="183" ht="15.75" customHeight="1">
+    <row r="183" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="5"/>
       <c r="D183" s="4"/>
       <c r="F183" s="4"/>
     </row>
-    <row r="184" ht="15.75" customHeight="1">
+    <row r="184" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="5"/>
       <c r="D184" s="4"/>
       <c r="F184" s="4"/>
     </row>
-    <row r="185" ht="15.75" customHeight="1">
+    <row r="185" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185" s="5"/>
       <c r="D185" s="4"/>
       <c r="F185" s="4"/>
     </row>
-    <row r="186" ht="15.75" customHeight="1">
+    <row r="186" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" s="5"/>
       <c r="D186" s="4"/>
       <c r="F186" s="4"/>
     </row>
-    <row r="187" ht="15.75" customHeight="1">
+    <row r="187" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" s="5"/>
       <c r="D187" s="4"/>
       <c r="F187" s="4"/>
     </row>
-    <row r="188" ht="15.75" customHeight="1">
+    <row r="188" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" s="5"/>
       <c r="D188" s="4"/>
       <c r="F188" s="4"/>
     </row>
-    <row r="189" ht="15.75" customHeight="1">
+    <row r="189" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" s="5"/>
       <c r="D189" s="4"/>
       <c r="F189" s="4"/>
     </row>
-    <row r="190" ht="15.75" customHeight="1">
+    <row r="190" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="5"/>
       <c r="D190" s="4"/>
       <c r="F190" s="4"/>
     </row>
-    <row r="191" ht="15.75" customHeight="1">
+    <row r="191" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" s="5"/>
       <c r="D191" s="4"/>
       <c r="F191" s="4"/>
     </row>
-    <row r="192" ht="15.75" customHeight="1">
+    <row r="192" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="5"/>
       <c r="D192" s="4"/>
       <c r="F192" s="4"/>
     </row>
-    <row r="193" ht="15.75" customHeight="1">
+    <row r="193" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" s="5"/>
       <c r="D193" s="4"/>
       <c r="F193" s="4"/>
     </row>
-    <row r="194" ht="15.75" customHeight="1">
+    <row r="194" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="5"/>
       <c r="D194" s="4"/>
       <c r="F194" s="4"/>
     </row>
-    <row r="195" ht="15.75" customHeight="1">
+    <row r="195" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="5"/>
       <c r="D195" s="4"/>
       <c r="F195" s="4"/>
     </row>
-    <row r="196" ht="15.75" customHeight="1">
+    <row r="196" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="5"/>
       <c r="D196" s="4"/>
       <c r="F196" s="4"/>
     </row>
-    <row r="197" ht="15.75" customHeight="1">
+    <row r="197" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="5"/>
       <c r="D197" s="4"/>
       <c r="F197" s="4"/>
     </row>
-    <row r="198" ht="15.75" customHeight="1">
+    <row r="198" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="5"/>
       <c r="D198" s="4"/>
       <c r="F198" s="4"/>
     </row>
-    <row r="199" ht="15.75" customHeight="1">
+    <row r="199" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B199" s="5"/>
       <c r="D199" s="4"/>
       <c r="F199" s="4"/>
     </row>
-    <row r="200" ht="15.75" customHeight="1">
+    <row r="200" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200" s="5"/>
       <c r="D200" s="4"/>
       <c r="F200" s="4"/>
     </row>
-    <row r="201" ht="15.75" customHeight="1">
+    <row r="201" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B201" s="5"/>
       <c r="D201" s="4"/>
       <c r="F201" s="4"/>
     </row>
-    <row r="202" ht="15.75" customHeight="1">
+    <row r="202" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B202" s="5"/>
       <c r="D202" s="4"/>
       <c r="F202" s="4"/>
     </row>
-    <row r="203" ht="15.75" customHeight="1">
+    <row r="203" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B203" s="5"/>
       <c r="D203" s="4"/>
       <c r="F203" s="4"/>
     </row>
-    <row r="204" ht="15.75" customHeight="1">
+    <row r="204" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B204" s="5"/>
       <c r="D204" s="4"/>
       <c r="F204" s="4"/>
     </row>
-    <row r="205" ht="15.75" customHeight="1">
+    <row r="205" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B205" s="5"/>
       <c r="D205" s="4"/>
       <c r="F205" s="4"/>
     </row>
-    <row r="206" ht="15.75" customHeight="1">
+    <row r="206" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B206" s="5"/>
       <c r="D206" s="4"/>
       <c r="F206" s="4"/>
     </row>
-    <row r="207" ht="15.75" customHeight="1">
+    <row r="207" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B207" s="5"/>
       <c r="D207" s="4"/>
       <c r="F207" s="4"/>
     </row>
-    <row r="208" ht="15.75" customHeight="1">
+    <row r="208" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B208" s="5"/>
       <c r="D208" s="4"/>
       <c r="F208" s="4"/>
     </row>
-    <row r="209" ht="15.75" customHeight="1">
+    <row r="209" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B209" s="5"/>
       <c r="D209" s="4"/>
       <c r="F209" s="4"/>
     </row>
-    <row r="210" ht="15.75" customHeight="1">
+    <row r="210" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B210" s="5"/>
       <c r="D210" s="4"/>
       <c r="F210" s="4"/>
     </row>
-    <row r="211" ht="15.75" customHeight="1">
+    <row r="211" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B211" s="5"/>
       <c r="D211" s="4"/>
       <c r="F211" s="4"/>
     </row>
-    <row r="212" ht="15.75" customHeight="1">
+    <row r="212" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B212" s="5"/>
       <c r="D212" s="4"/>
       <c r="F212" s="4"/>
     </row>
-    <row r="213" ht="15.75" customHeight="1">
+    <row r="213" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B213" s="5"/>
       <c r="D213" s="4"/>
       <c r="F213" s="4"/>
     </row>
-    <row r="214" ht="15.75" customHeight="1">
+    <row r="214" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B214" s="5"/>
       <c r="D214" s="4"/>
       <c r="F214" s="4"/>
     </row>
-    <row r="215" ht="15.75" customHeight="1">
+    <row r="215" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B215" s="5"/>
       <c r="D215" s="4"/>
       <c r="F215" s="4"/>
     </row>
-    <row r="216" ht="15.75" customHeight="1">
+    <row r="216" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B216" s="5"/>
       <c r="D216" s="4"/>
       <c r="F216" s="4"/>
     </row>
-    <row r="217" ht="15.75" customHeight="1">
+    <row r="217" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B217" s="5"/>
       <c r="D217" s="4"/>
       <c r="F217" s="4"/>
     </row>
-    <row r="218" ht="15.75" customHeight="1">
+    <row r="218" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B218" s="5"/>
       <c r="D218" s="4"/>
       <c r="F218" s="4"/>
     </row>
-    <row r="219" ht="15.75" customHeight="1">
+    <row r="219" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B219" s="5"/>
       <c r="D219" s="4"/>
       <c r="F219" s="4"/>
     </row>
-    <row r="220" ht="15.75" customHeight="1">
+    <row r="220" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B220" s="5"/>
       <c r="D220" s="4"/>
       <c r="F220" s="4"/>
     </row>
-    <row r="221" ht="15.75" customHeight="1">
+    <row r="221" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B221" s="5"/>
     </row>
-    <row r="222" ht="15.75" customHeight="1">
+    <row r="222" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B222" s="5"/>
     </row>
-    <row r="223" ht="15.75" customHeight="1">
+    <row r="223" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B223" s="5"/>
     </row>
-    <row r="224" ht="15.75" customHeight="1">
+    <row r="224" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B224" s="5"/>
     </row>
-    <row r="225" ht="15.75" customHeight="1">
+    <row r="225" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B225" s="5"/>
     </row>
-    <row r="226" ht="15.75" customHeight="1">
+    <row r="226" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B226" s="5"/>
     </row>
-    <row r="227" ht="15.75" customHeight="1">
+    <row r="227" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B227" s="5"/>
     </row>
-    <row r="228" ht="15.75" customHeight="1">
+    <row r="228" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B228" s="5"/>
     </row>
-    <row r="229" ht="15.75" customHeight="1">
+    <row r="229" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B229" s="5"/>
     </row>
-    <row r="230" ht="15.75" customHeight="1">
+    <row r="230" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B230" s="5"/>
     </row>
-    <row r="231" ht="15.75" customHeight="1">
+    <row r="231" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B231" s="5"/>
     </row>
-    <row r="232" ht="15.75" customHeight="1">
+    <row r="232" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B232" s="5"/>
     </row>
-    <row r="233" ht="15.75" customHeight="1">
+    <row r="233" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B233" s="5"/>
     </row>
-    <row r="234" ht="15.75" customHeight="1">
+    <row r="234" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B234" s="5"/>
     </row>
-    <row r="235" ht="15.75" customHeight="1">
+    <row r="235" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B235" s="5"/>
     </row>
-    <row r="236" ht="15.75" customHeight="1">
+    <row r="236" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B236" s="5"/>
     </row>
-    <row r="237" ht="15.75" customHeight="1">
+    <row r="237" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B237" s="5"/>
     </row>
-    <row r="238" ht="15.75" customHeight="1">
+    <row r="238" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B238" s="5"/>
     </row>
-    <row r="239" ht="15.75" customHeight="1">
+    <row r="239" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B239" s="5"/>
     </row>
-    <row r="240" ht="15.75" customHeight="1">
+    <row r="240" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B240" s="5"/>
     </row>
-    <row r="241" ht="15.75" customHeight="1">
+    <row r="241" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B241" s="5"/>
     </row>
-    <row r="242" ht="15.75" customHeight="1">
+    <row r="242" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B242" s="5"/>
     </row>
-    <row r="243" ht="15.75" customHeight="1">
+    <row r="243" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B243" s="5"/>
     </row>
-    <row r="244" ht="15.75" customHeight="1">
+    <row r="244" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B244" s="5"/>
     </row>
-    <row r="245" ht="15.75" customHeight="1">
+    <row r="245" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B245" s="5"/>
     </row>
-    <row r="246" ht="15.75" customHeight="1">
+    <row r="246" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B246" s="5"/>
     </row>
-    <row r="247" ht="15.75" customHeight="1">
+    <row r="247" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B247" s="5"/>
     </row>
-    <row r="248" ht="15.75" customHeight="1">
+    <row r="248" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B248" s="5"/>
     </row>
-    <row r="249" ht="15.75" customHeight="1">
+    <row r="249" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B249" s="5"/>
     </row>
-    <row r="250" ht="15.75" customHeight="1">
+    <row r="250" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B250" s="5"/>
     </row>
-    <row r="251" ht="15.75" customHeight="1">
+    <row r="251" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B251" s="5"/>
     </row>
-    <row r="252" ht="15.75" customHeight="1">
+    <row r="252" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B252" s="5"/>
     </row>
-    <row r="253" ht="15.75" customHeight="1">
+    <row r="253" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B253" s="5"/>
     </row>
-    <row r="254" ht="15.75" customHeight="1">
+    <row r="254" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B254" s="5"/>
     </row>
-    <row r="255" ht="15.75" customHeight="1">
+    <row r="255" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B255" s="5"/>
     </row>
-    <row r="256" ht="15.75" customHeight="1">
+    <row r="256" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B256" s="5"/>
     </row>
-    <row r="257" ht="15.75" customHeight="1">
+    <row r="257" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B257" s="5"/>
     </row>
-    <row r="258" ht="15.75" customHeight="1">
+    <row r="258" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B258" s="5"/>
     </row>
-    <row r="259" ht="15.75" customHeight="1">
+    <row r="259" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B259" s="5"/>
     </row>
-    <row r="260" ht="15.75" customHeight="1">
+    <row r="260" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B260" s="5"/>
     </row>
-    <row r="261" ht="15.75" customHeight="1">
+    <row r="261" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B261" s="5"/>
     </row>
-    <row r="262" ht="15.75" customHeight="1">
+    <row r="262" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B262" s="5"/>
     </row>
-    <row r="263" ht="15.75" customHeight="1">
+    <row r="263" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B263" s="5"/>
     </row>
-    <row r="264" ht="15.75" customHeight="1">
+    <row r="264" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B264" s="5"/>
     </row>
-    <row r="265" ht="15.75" customHeight="1">
+    <row r="265" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B265" s="5"/>
     </row>
-    <row r="266" ht="15.75" customHeight="1">
+    <row r="266" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B266" s="5"/>
     </row>
-    <row r="267" ht="15.75" customHeight="1">
+    <row r="267" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B267" s="5"/>
     </row>
-    <row r="268" ht="15.75" customHeight="1">
+    <row r="268" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B268" s="5"/>
     </row>
-    <row r="269" ht="15.75" customHeight="1">
+    <row r="269" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B269" s="5"/>
     </row>
-    <row r="270" ht="15.75" customHeight="1">
+    <row r="270" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B270" s="5"/>
     </row>
-    <row r="271" ht="15.75" customHeight="1">
+    <row r="271" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B271" s="5"/>
     </row>
-    <row r="272" ht="15.75" customHeight="1">
+    <row r="272" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B272" s="5"/>
     </row>
-    <row r="273" ht="15.75" customHeight="1">
+    <row r="273" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B273" s="5"/>
     </row>
-    <row r="274" ht="15.75" customHeight="1">
+    <row r="274" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B274" s="5"/>
     </row>
-    <row r="275" ht="15.75" customHeight="1">
+    <row r="275" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B275" s="5"/>
     </row>
-    <row r="276" ht="15.75" customHeight="1">
+    <row r="276" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B276" s="5"/>
     </row>
-    <row r="277" ht="15.75" customHeight="1">
+    <row r="277" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B277" s="5"/>
     </row>
-    <row r="278" ht="15.75" customHeight="1">
+    <row r="278" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B278" s="5"/>
     </row>
-    <row r="279" ht="15.75" customHeight="1">
+    <row r="279" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B279" s="5"/>
     </row>
-    <row r="280" ht="15.75" customHeight="1">
+    <row r="280" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B280" s="5"/>
     </row>
-    <row r="281" ht="15.75" customHeight="1">
+    <row r="281" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B281" s="5"/>
     </row>
-    <row r="282" ht="15.75" customHeight="1">
+    <row r="282" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B282" s="5"/>
     </row>
-    <row r="283" ht="15.75" customHeight="1">
+    <row r="283" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B283" s="5"/>
     </row>
-    <row r="284" ht="15.75" customHeight="1">
+    <row r="284" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B284" s="5"/>
     </row>
-    <row r="285" ht="15.75" customHeight="1">
+    <row r="285" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B285" s="5"/>
     </row>
-    <row r="286" ht="15.75" customHeight="1">
+    <row r="286" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B286" s="5"/>
     </row>
-    <row r="287" ht="15.75" customHeight="1">
+    <row r="287" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B287" s="5"/>
     </row>
-    <row r="288" ht="15.75" customHeight="1">
+    <row r="288" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B288" s="5"/>
     </row>
-    <row r="289" ht="15.75" customHeight="1">
+    <row r="289" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B289" s="5"/>
     </row>
-    <row r="290" ht="15.75" customHeight="1">
+    <row r="290" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B290" s="5"/>
     </row>
-    <row r="291" ht="15.75" customHeight="1">
+    <row r="291" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B291" s="5"/>
     </row>
-    <row r="292" ht="15.75" customHeight="1">
+    <row r="292" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B292" s="5"/>
     </row>
-    <row r="293" ht="15.75" customHeight="1">
+    <row r="293" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B293" s="5"/>
     </row>
-    <row r="294" ht="15.75" customHeight="1">
+    <row r="294" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B294" s="5"/>
     </row>
-    <row r="295" ht="15.75" customHeight="1">
+    <row r="295" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B295" s="5"/>
     </row>
-    <row r="296" ht="15.75" customHeight="1">
+    <row r="296" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B296" s="5"/>
     </row>
-    <row r="297" ht="15.75" customHeight="1">
+    <row r="297" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B297" s="5"/>
     </row>
-    <row r="298" ht="15.75" customHeight="1">
+    <row r="298" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B298" s="5"/>
     </row>
-    <row r="299" ht="15.75" customHeight="1">
+    <row r="299" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B299" s="5"/>
     </row>
-    <row r="300" ht="15.75" customHeight="1">
+    <row r="300" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B300" s="5"/>
     </row>
-    <row r="301" ht="15.75" customHeight="1">
+    <row r="301" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B301" s="5"/>
     </row>
-    <row r="302" ht="15.75" customHeight="1">
+    <row r="302" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B302" s="5"/>
     </row>
-    <row r="303" ht="15.75" customHeight="1">
+    <row r="303" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B303" s="5"/>
     </row>
-    <row r="304" ht="15.75" customHeight="1">
+    <row r="304" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B304" s="5"/>
     </row>
-    <row r="305" ht="15.75" customHeight="1">
+    <row r="305" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B305" s="5"/>
     </row>
-    <row r="306" ht="15.75" customHeight="1">
+    <row r="306" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B306" s="5"/>
     </row>
-    <row r="307" ht="15.75" customHeight="1">
+    <row r="307" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B307" s="5"/>
     </row>
-    <row r="308" ht="15.75" customHeight="1">
+    <row r="308" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B308" s="5"/>
     </row>
-    <row r="309" ht="15.75" customHeight="1">
+    <row r="309" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B309" s="5"/>
     </row>
-    <row r="310" ht="15.75" customHeight="1">
+    <row r="310" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B310" s="5"/>
     </row>
-    <row r="311" ht="15.75" customHeight="1">
+    <row r="311" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B311" s="5"/>
     </row>
-    <row r="312" ht="15.75" customHeight="1">
+    <row r="312" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B312" s="5"/>
     </row>
-    <row r="313" ht="15.75" customHeight="1">
+    <row r="313" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B313" s="5"/>
     </row>
-    <row r="314" ht="15.75" customHeight="1">
+    <row r="314" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B314" s="5"/>
     </row>
-    <row r="315" ht="15.75" customHeight="1">
+    <row r="315" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B315" s="5"/>
     </row>
-    <row r="316" ht="15.75" customHeight="1">
+    <row r="316" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B316" s="5"/>
     </row>
-    <row r="317" ht="15.75" customHeight="1">
+    <row r="317" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B317" s="5"/>
     </row>
-    <row r="318" ht="15.75" customHeight="1">
+    <row r="318" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B318" s="5"/>
     </row>
-    <row r="319" ht="15.75" customHeight="1">
+    <row r="319" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B319" s="5"/>
     </row>
-    <row r="320" ht="15.75" customHeight="1">
+    <row r="320" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B320" s="5"/>
     </row>
-    <row r="321" ht="15.75" customHeight="1">
+    <row r="321" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B321" s="5"/>
     </row>
-    <row r="322" ht="15.75" customHeight="1">
+    <row r="322" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B322" s="5"/>
     </row>
-    <row r="323" ht="15.75" customHeight="1">
+    <row r="323" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B323" s="5"/>
     </row>
-    <row r="324" ht="15.75" customHeight="1">
+    <row r="324" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B324" s="5"/>
     </row>
-    <row r="325" ht="15.75" customHeight="1">
+    <row r="325" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B325" s="5"/>
     </row>
-    <row r="326" ht="15.75" customHeight="1">
+    <row r="326" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B326" s="5"/>
     </row>
-    <row r="327" ht="15.75" customHeight="1">
+    <row r="327" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B327" s="5"/>
     </row>
-    <row r="328" ht="15.75" customHeight="1">
+    <row r="328" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B328" s="5"/>
     </row>
-    <row r="329" ht="15.75" customHeight="1">
+    <row r="329" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B329" s="5"/>
     </row>
-    <row r="330" ht="15.75" customHeight="1">
+    <row r="330" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B330" s="5"/>
     </row>
-    <row r="331" ht="15.75" customHeight="1">
+    <row r="331" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B331" s="5"/>
     </row>
-    <row r="332" ht="15.75" customHeight="1">
+    <row r="332" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B332" s="5"/>
     </row>
-    <row r="333" ht="15.75" customHeight="1">
+    <row r="333" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B333" s="5"/>
     </row>
-    <row r="334" ht="15.75" customHeight="1">
+    <row r="334" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B334" s="5"/>
     </row>
-    <row r="335" ht="15.75" customHeight="1">
+    <row r="335" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B335" s="5"/>
     </row>
-    <row r="336" ht="15.75" customHeight="1">
+    <row r="336" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B336" s="5"/>
     </row>
-    <row r="337" ht="15.75" customHeight="1">
+    <row r="337" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B337" s="5"/>
     </row>
-    <row r="338" ht="15.75" customHeight="1">
+    <row r="338" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B338" s="5"/>
     </row>
-    <row r="339" ht="15.75" customHeight="1">
+    <row r="339" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B339" s="5"/>
     </row>
-    <row r="340" ht="15.75" customHeight="1">
+    <row r="340" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B340" s="5"/>
     </row>
-    <row r="341" ht="15.75" customHeight="1">
+    <row r="341" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B341" s="5"/>
     </row>
-    <row r="342" ht="15.75" customHeight="1">
+    <row r="342" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B342" s="5"/>
     </row>
-    <row r="343" ht="15.75" customHeight="1">
+    <row r="343" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B343" s="5"/>
     </row>
-    <row r="344" ht="15.75" customHeight="1">
+    <row r="344" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B344" s="5"/>
     </row>
-    <row r="345" ht="15.75" customHeight="1">
+    <row r="345" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B345" s="5"/>
     </row>
-    <row r="346" ht="15.75" customHeight="1">
+    <row r="346" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B346" s="5"/>
     </row>
-    <row r="347" ht="15.75" customHeight="1">
+    <row r="347" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B347" s="5"/>
     </row>
-    <row r="348" ht="15.75" customHeight="1">
+    <row r="348" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B348" s="5"/>
     </row>
-    <row r="349" ht="15.75" customHeight="1">
+    <row r="349" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B349" s="5"/>
     </row>
-    <row r="350" ht="15.75" customHeight="1">
+    <row r="350" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B350" s="5"/>
     </row>
-    <row r="351" ht="15.75" customHeight="1">
+    <row r="351" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B351" s="5"/>
     </row>
-    <row r="352" ht="15.75" customHeight="1">
+    <row r="352" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B352" s="5"/>
     </row>
-    <row r="353" ht="15.75" customHeight="1">
+    <row r="353" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B353" s="5"/>
     </row>
-    <row r="354" ht="15.75" customHeight="1">
+    <row r="354" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B354" s="5"/>
     </row>
-    <row r="355" ht="15.75" customHeight="1">
+    <row r="355" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B355" s="5"/>
     </row>
-    <row r="356" ht="15.75" customHeight="1">
+    <row r="356" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B356" s="5"/>
     </row>
-    <row r="357" ht="15.75" customHeight="1">
+    <row r="357" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B357" s="5"/>
     </row>
-    <row r="358" ht="15.75" customHeight="1">
+    <row r="358" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B358" s="5"/>
     </row>
-    <row r="359" ht="15.75" customHeight="1">
+    <row r="359" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B359" s="5"/>
     </row>
-    <row r="360" ht="15.75" customHeight="1">
+    <row r="360" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B360" s="5"/>
     </row>
-    <row r="361" ht="15.75" customHeight="1">
+    <row r="361" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B361" s="5"/>
     </row>
-    <row r="362" ht="15.75" customHeight="1">
+    <row r="362" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B362" s="5"/>
     </row>
-    <row r="363" ht="15.75" customHeight="1">
+    <row r="363" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B363" s="5"/>
     </row>
-    <row r="364" ht="15.75" customHeight="1">
+    <row r="364" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B364" s="5"/>
     </row>
-    <row r="365" ht="15.75" customHeight="1">
+    <row r="365" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B365" s="5"/>
     </row>
-    <row r="366" ht="15.75" customHeight="1">
+    <row r="366" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B366" s="5"/>
     </row>
-    <row r="367" ht="15.75" customHeight="1">
+    <row r="367" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B367" s="5"/>
     </row>
-    <row r="368" ht="15.75" customHeight="1">
+    <row r="368" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B368" s="5"/>
     </row>
-    <row r="369" ht="15.75" customHeight="1">
+    <row r="369" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B369" s="5"/>
     </row>
-    <row r="370" ht="15.75" customHeight="1">
+    <row r="370" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B370" s="5"/>
     </row>
-    <row r="371" ht="15.75" customHeight="1">
+    <row r="371" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B371" s="5"/>
     </row>
-    <row r="372" ht="15.75" customHeight="1">
+    <row r="372" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B372" s="5"/>
     </row>
-    <row r="373" ht="15.75" customHeight="1">
+    <row r="373" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B373" s="5"/>
     </row>
-    <row r="374" ht="15.75" customHeight="1">
+    <row r="374" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B374" s="5"/>
     </row>
-    <row r="375" ht="15.75" customHeight="1">
+    <row r="375" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B375" s="5"/>
     </row>
-    <row r="376" ht="15.75" customHeight="1">
+    <row r="376" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B376" s="5"/>
     </row>
-    <row r="377" ht="15.75" customHeight="1">
+    <row r="377" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B377" s="5"/>
     </row>
-    <row r="378" ht="15.75" customHeight="1">
+    <row r="378" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B378" s="5"/>
     </row>
-    <row r="379" ht="15.75" customHeight="1">
+    <row r="379" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B379" s="5"/>
     </row>
-    <row r="380" ht="15.75" customHeight="1">
+    <row r="380" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B380" s="5"/>
     </row>
-    <row r="381" ht="15.75" customHeight="1">
+    <row r="381" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B381" s="5"/>
     </row>
-    <row r="382" ht="15.75" customHeight="1">
+    <row r="382" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B382" s="5"/>
     </row>
-    <row r="383" ht="15.75" customHeight="1">
+    <row r="383" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B383" s="5"/>
     </row>
-    <row r="384" ht="15.75" customHeight="1">
+    <row r="384" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B384" s="5"/>
     </row>
-    <row r="385" ht="15.75" customHeight="1">
+    <row r="385" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B385" s="5"/>
     </row>
-    <row r="386" ht="15.75" customHeight="1">
+    <row r="386" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B386" s="5"/>
     </row>
-    <row r="387" ht="15.75" customHeight="1">
+    <row r="387" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B387" s="5"/>
     </row>
-    <row r="388" ht="15.75" customHeight="1">
+    <row r="388" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B388" s="5"/>
     </row>
-    <row r="389" ht="15.75" customHeight="1">
+    <row r="389" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B389" s="5"/>
     </row>
-    <row r="390" ht="15.75" customHeight="1">
+    <row r="390" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B390" s="5"/>
     </row>
-    <row r="391" ht="15.75" customHeight="1">
+    <row r="391" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B391" s="5"/>
     </row>
-    <row r="392" ht="15.75" customHeight="1">
+    <row r="392" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B392" s="5"/>
     </row>
-    <row r="393" ht="15.75" customHeight="1">
+    <row r="393" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B393" s="5"/>
     </row>
-    <row r="394" ht="15.75" customHeight="1">
+    <row r="394" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B394" s="5"/>
     </row>
-    <row r="395" ht="15.75" customHeight="1">
+    <row r="395" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B395" s="5"/>
     </row>
-    <row r="396" ht="15.75" customHeight="1">
+    <row r="396" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B396" s="5"/>
     </row>
-    <row r="397" ht="15.75" customHeight="1">
+    <row r="397" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B397" s="5"/>
     </row>
-    <row r="398" ht="15.75" customHeight="1">
+    <row r="398" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B398" s="5"/>
     </row>
-    <row r="399" ht="15.75" customHeight="1">
+    <row r="399" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B399" s="5"/>
     </row>
-    <row r="400" ht="15.75" customHeight="1">
+    <row r="400" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B400" s="5"/>
     </row>
-    <row r="401" ht="15.75" customHeight="1">
+    <row r="401" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B401" s="5"/>
     </row>
-    <row r="402" ht="15.75" customHeight="1">
+    <row r="402" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B402" s="5"/>
     </row>
-    <row r="403" ht="15.75" customHeight="1">
+    <row r="403" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B403" s="5"/>
     </row>
-    <row r="404" ht="15.75" customHeight="1">
+    <row r="404" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B404" s="5"/>
     </row>
-    <row r="405" ht="15.75" customHeight="1">
+    <row r="405" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B405" s="5"/>
     </row>
-    <row r="406" ht="15.75" customHeight="1">
+    <row r="406" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B406" s="5"/>
     </row>
-    <row r="407" ht="15.75" customHeight="1">
+    <row r="407" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B407" s="5"/>
     </row>
-    <row r="408" ht="15.75" customHeight="1">
+    <row r="408" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B408" s="5"/>
     </row>
-    <row r="409" ht="15.75" customHeight="1">
+    <row r="409" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B409" s="5"/>
     </row>
-    <row r="410" ht="15.75" customHeight="1">
+    <row r="410" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B410" s="5"/>
     </row>
-    <row r="411" ht="15.75" customHeight="1">
+    <row r="411" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B411" s="5"/>
     </row>
-    <row r="412" ht="15.75" customHeight="1">
+    <row r="412" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B412" s="5"/>
     </row>
-    <row r="413" ht="15.75" customHeight="1">
+    <row r="413" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B413" s="5"/>
     </row>
-    <row r="414" ht="15.75" customHeight="1">
+    <row r="414" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B414" s="5"/>
     </row>
-    <row r="415" ht="15.75" customHeight="1">
+    <row r="415" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B415" s="5"/>
     </row>
-    <row r="416" ht="15.75" customHeight="1">
+    <row r="416" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B416" s="5"/>
     </row>
-    <row r="417" ht="15.75" customHeight="1">
+    <row r="417" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B417" s="5"/>
     </row>
-    <row r="418" ht="15.75" customHeight="1">
+    <row r="418" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B418" s="5"/>
     </row>
-    <row r="419" ht="15.75" customHeight="1">
+    <row r="419" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B419" s="5"/>
     </row>
-    <row r="420" ht="15.75" customHeight="1">
+    <row r="420" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B420" s="5"/>
     </row>
-    <row r="421" ht="15.75" customHeight="1">
+    <row r="421" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B421" s="5"/>
     </row>
-    <row r="422" ht="15.75" customHeight="1">
+    <row r="422" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B422" s="5"/>
     </row>
-    <row r="423" ht="15.75" customHeight="1">
+    <row r="423" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B423" s="5"/>
     </row>
-    <row r="424" ht="15.75" customHeight="1">
+    <row r="424" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B424" s="5"/>
     </row>
-    <row r="425" ht="15.75" customHeight="1">
+    <row r="425" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B425" s="5"/>
     </row>
-    <row r="426" ht="15.75" customHeight="1">
+    <row r="426" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B426" s="5"/>
     </row>
-    <row r="427" ht="15.75" customHeight="1">
+    <row r="427" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B427" s="5"/>
     </row>
-    <row r="428" ht="15.75" customHeight="1">
+    <row r="428" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B428" s="5"/>
     </row>
-    <row r="429" ht="15.75" customHeight="1">
+    <row r="429" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B429" s="5"/>
     </row>
-    <row r="430" ht="15.75" customHeight="1">
+    <row r="430" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B430" s="5"/>
     </row>
-    <row r="431" ht="15.75" customHeight="1">
+    <row r="431" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B431" s="5"/>
     </row>
-    <row r="432" ht="15.75" customHeight="1">
+    <row r="432" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B432" s="5"/>
     </row>
-    <row r="433" ht="15.75" customHeight="1">
+    <row r="433" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B433" s="5"/>
     </row>
-    <row r="434" ht="15.75" customHeight="1">
+    <row r="434" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B434" s="5"/>
     </row>
-    <row r="435" ht="15.75" customHeight="1">
+    <row r="435" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B435" s="5"/>
     </row>
-    <row r="436" ht="15.75" customHeight="1">
+    <row r="436" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B436" s="5"/>
     </row>
-    <row r="437" ht="15.75" customHeight="1">
+    <row r="437" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B437" s="5"/>
     </row>
-    <row r="438" ht="15.75" customHeight="1">
+    <row r="438" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B438" s="5"/>
     </row>
-    <row r="439" ht="15.75" customHeight="1">
+    <row r="439" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B439" s="5"/>
     </row>
-    <row r="440" ht="15.75" customHeight="1">
+    <row r="440" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B440" s="5"/>
     </row>
-    <row r="441" ht="15.75" customHeight="1">
+    <row r="441" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B441" s="5"/>
     </row>
-    <row r="442" ht="15.75" customHeight="1">
+    <row r="442" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B442" s="5"/>
     </row>
-    <row r="443" ht="15.75" customHeight="1">
+    <row r="443" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B443" s="5"/>
     </row>
-    <row r="444" ht="15.75" customHeight="1">
+    <row r="444" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B444" s="5"/>
     </row>
-    <row r="445" ht="15.75" customHeight="1">
+    <row r="445" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B445" s="5"/>
     </row>
-    <row r="446" ht="15.75" customHeight="1">
+    <row r="446" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B446" s="5"/>
     </row>
-    <row r="447" ht="15.75" customHeight="1">
+    <row r="447" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B447" s="5"/>
     </row>
-    <row r="448" ht="15.75" customHeight="1">
+    <row r="448" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B448" s="5"/>
     </row>
-    <row r="449" ht="15.75" customHeight="1">
+    <row r="449" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B449" s="5"/>
     </row>
-    <row r="450" ht="15.75" customHeight="1">
+    <row r="450" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B450" s="5"/>
     </row>
-    <row r="451" ht="15.75" customHeight="1">
+    <row r="451" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B451" s="5"/>
     </row>
-    <row r="452" ht="15.75" customHeight="1">
+    <row r="452" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B452" s="5"/>
     </row>
-    <row r="453" ht="15.75" customHeight="1">
+    <row r="453" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B453" s="5"/>
     </row>
-    <row r="454" ht="15.75" customHeight="1">
+    <row r="454" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B454" s="5"/>
     </row>
-    <row r="455" ht="15.75" customHeight="1">
+    <row r="455" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B455" s="5"/>
     </row>
-    <row r="456" ht="15.75" customHeight="1">
+    <row r="456" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B456" s="5"/>
     </row>
-    <row r="457" ht="15.75" customHeight="1">
+    <row r="457" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B457" s="5"/>
     </row>
-    <row r="458" ht="15.75" customHeight="1">
+    <row r="458" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B458" s="5"/>
     </row>
-    <row r="459" ht="15.75" customHeight="1">
+    <row r="459" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B459" s="5"/>
     </row>
-    <row r="460" ht="15.75" customHeight="1">
+    <row r="460" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B460" s="5"/>
     </row>
-    <row r="461" ht="15.75" customHeight="1">
+    <row r="461" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B461" s="5"/>
     </row>
-    <row r="462" ht="15.75" customHeight="1">
+    <row r="462" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B462" s="5"/>
     </row>
-    <row r="463" ht="15.75" customHeight="1">
+    <row r="463" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B463" s="5"/>
     </row>
-    <row r="464" ht="15.75" customHeight="1">
+    <row r="464" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B464" s="5"/>
     </row>
-    <row r="465" ht="15.75" customHeight="1">
+    <row r="465" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B465" s="5"/>
     </row>
-    <row r="466" ht="15.75" customHeight="1">
+    <row r="466" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B466" s="5"/>
     </row>
-    <row r="467" ht="15.75" customHeight="1">
+    <row r="467" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B467" s="5"/>
     </row>
-    <row r="468" ht="15.75" customHeight="1">
+    <row r="468" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B468" s="5"/>
     </row>
-    <row r="469" ht="15.75" customHeight="1">
+    <row r="469" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B469" s="5"/>
     </row>
-    <row r="470" ht="15.75" customHeight="1">
+    <row r="470" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B470" s="5"/>
     </row>
-    <row r="471" ht="15.75" customHeight="1">
+    <row r="471" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B471" s="5"/>
     </row>
-    <row r="472" ht="15.75" customHeight="1">
+    <row r="472" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B472" s="5"/>
     </row>
-    <row r="473" ht="15.75" customHeight="1">
+    <row r="473" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B473" s="5"/>
     </row>
-    <row r="474" ht="15.75" customHeight="1">
+    <row r="474" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B474" s="5"/>
     </row>
-    <row r="475" ht="15.75" customHeight="1">
+    <row r="475" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B475" s="5"/>
     </row>
-    <row r="476" ht="15.75" customHeight="1">
+    <row r="476" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B476" s="5"/>
     </row>
-    <row r="477" ht="15.75" customHeight="1">
+    <row r="477" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B477" s="5"/>
     </row>
-    <row r="478" ht="15.75" customHeight="1">
+    <row r="478" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B478" s="5"/>
     </row>
-    <row r="479" ht="15.75" customHeight="1">
+    <row r="479" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B479" s="5"/>
     </row>
-    <row r="480" ht="15.75" customHeight="1">
+    <row r="480" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B480" s="5"/>
     </row>
-    <row r="481" ht="15.75" customHeight="1">
+    <row r="481" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B481" s="5"/>
     </row>
-    <row r="482" ht="15.75" customHeight="1">
+    <row r="482" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B482" s="5"/>
     </row>
-    <row r="483" ht="15.75" customHeight="1">
+    <row r="483" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B483" s="5"/>
     </row>
-    <row r="484" ht="15.75" customHeight="1">
+    <row r="484" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B484" s="5"/>
     </row>
-    <row r="485" ht="15.75" customHeight="1">
+    <row r="485" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B485" s="5"/>
     </row>
-    <row r="486" ht="15.75" customHeight="1">
+    <row r="486" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B486" s="5"/>
     </row>
-    <row r="487" ht="15.75" customHeight="1">
+    <row r="487" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B487" s="5"/>
     </row>
-    <row r="488" ht="15.75" customHeight="1">
+    <row r="488" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B488" s="5"/>
     </row>
-    <row r="489" ht="15.75" customHeight="1">
+    <row r="489" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B489" s="5"/>
     </row>
-    <row r="490" ht="15.75" customHeight="1">
+    <row r="490" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B490" s="5"/>
     </row>
-    <row r="491" ht="15.75" customHeight="1">
+    <row r="491" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B491" s="5"/>
     </row>
-    <row r="492" ht="15.75" customHeight="1">
+    <row r="492" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B492" s="5"/>
     </row>
-    <row r="493" ht="15.75" customHeight="1">
+    <row r="493" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B493" s="5"/>
     </row>
-    <row r="494" ht="15.75" customHeight="1">
+    <row r="494" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B494" s="5"/>
     </row>
-    <row r="495" ht="15.75" customHeight="1">
+    <row r="495" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B495" s="5"/>
     </row>
-    <row r="496" ht="15.75" customHeight="1">
+    <row r="496" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B496" s="5"/>
     </row>
-    <row r="497" ht="15.75" customHeight="1">
+    <row r="497" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B497" s="5"/>
     </row>
-    <row r="498" ht="15.75" customHeight="1">
+    <row r="498" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B498" s="5"/>
     </row>
-    <row r="499" ht="15.75" customHeight="1">
+    <row r="499" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B499" s="5"/>
     </row>
-    <row r="500" ht="15.75" customHeight="1">
+    <row r="500" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B500" s="5"/>
     </row>
-    <row r="501" ht="15.75" customHeight="1">
+    <row r="501" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B501" s="5"/>
     </row>
-    <row r="502" ht="15.75" customHeight="1">
+    <row r="502" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B502" s="5"/>
     </row>
-    <row r="503" ht="15.75" customHeight="1">
+    <row r="503" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B503" s="5"/>
     </row>
-    <row r="504" ht="15.75" customHeight="1">
+    <row r="504" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B504" s="5"/>
     </row>
-    <row r="505" ht="15.75" customHeight="1">
+    <row r="505" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B505" s="5"/>
     </row>
-    <row r="506" ht="15.75" customHeight="1">
+    <row r="506" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B506" s="5"/>
     </row>
-    <row r="507" ht="15.75" customHeight="1">
+    <row r="507" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B507" s="5"/>
     </row>
-    <row r="508" ht="15.75" customHeight="1">
+    <row r="508" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B508" s="5"/>
     </row>
-    <row r="509" ht="15.75" customHeight="1">
+    <row r="509" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B509" s="5"/>
     </row>
-    <row r="510" ht="15.75" customHeight="1">
+    <row r="510" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B510" s="5"/>
     </row>
-    <row r="511" ht="15.75" customHeight="1">
+    <row r="511" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B511" s="5"/>
     </row>
-    <row r="512" ht="15.75" customHeight="1">
+    <row r="512" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B512" s="5"/>
     </row>
-    <row r="513" ht="15.75" customHeight="1">
+    <row r="513" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B513" s="5"/>
     </row>
-    <row r="514" ht="15.75" customHeight="1">
+    <row r="514" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B514" s="5"/>
     </row>
-    <row r="515" ht="15.75" customHeight="1">
+    <row r="515" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B515" s="5"/>
     </row>
-    <row r="516" ht="15.75" customHeight="1">
+    <row r="516" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B516" s="5"/>
     </row>
-    <row r="517" ht="15.75" customHeight="1">
+    <row r="517" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B517" s="5"/>
     </row>
-    <row r="518" ht="15.75" customHeight="1">
+    <row r="518" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B518" s="5"/>
     </row>
-    <row r="519" ht="15.75" customHeight="1">
+    <row r="519" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B519" s="5"/>
     </row>
-    <row r="520" ht="15.75" customHeight="1">
+    <row r="520" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B520" s="5"/>
     </row>
-    <row r="521" ht="15.75" customHeight="1">
+    <row r="521" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B521" s="5"/>
     </row>
-    <row r="522" ht="15.75" customHeight="1">
+    <row r="522" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B522" s="5"/>
     </row>
-    <row r="523" ht="15.75" customHeight="1">
+    <row r="523" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B523" s="5"/>
     </row>
-    <row r="524" ht="15.75" customHeight="1">
+    <row r="524" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B524" s="5"/>
     </row>
-    <row r="525" ht="15.75" customHeight="1">
+    <row r="525" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B525" s="5"/>
     </row>
-    <row r="526" ht="15.75" customHeight="1">
+    <row r="526" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B526" s="5"/>
     </row>
-    <row r="527" ht="15.75" customHeight="1">
+    <row r="527" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B527" s="5"/>
     </row>
-    <row r="528" ht="15.75" customHeight="1">
+    <row r="528" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B528" s="5"/>
     </row>
-    <row r="529" ht="15.75" customHeight="1">
+    <row r="529" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B529" s="5"/>
     </row>
-    <row r="530" ht="15.75" customHeight="1">
+    <row r="530" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B530" s="5"/>
     </row>
-    <row r="531" ht="15.75" customHeight="1">
+    <row r="531" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B531" s="5"/>
     </row>
-    <row r="532" ht="15.75" customHeight="1">
+    <row r="532" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B532" s="5"/>
     </row>
-    <row r="533" ht="15.75" customHeight="1">
+    <row r="533" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B533" s="5"/>
     </row>
-    <row r="534" ht="15.75" customHeight="1">
+    <row r="534" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B534" s="5"/>
     </row>
-    <row r="535" ht="15.75" customHeight="1">
+    <row r="535" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B535" s="5"/>
     </row>
-    <row r="536" ht="15.75" customHeight="1">
+    <row r="536" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B536" s="5"/>
     </row>
-    <row r="537" ht="15.75" customHeight="1">
+    <row r="537" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B537" s="5"/>
     </row>
-    <row r="538" ht="15.75" customHeight="1">
+    <row r="538" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B538" s="5"/>
     </row>
-    <row r="539" ht="15.75" customHeight="1">
+    <row r="539" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B539" s="5"/>
     </row>
-    <row r="540" ht="15.75" customHeight="1">
+    <row r="540" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B540" s="5"/>
     </row>
-    <row r="541" ht="15.75" customHeight="1">
+    <row r="541" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B541" s="5"/>
     </row>
-    <row r="542" ht="15.75" customHeight="1">
+    <row r="542" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B542" s="5"/>
     </row>
-    <row r="543" ht="15.75" customHeight="1">
+    <row r="543" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B543" s="5"/>
     </row>
-    <row r="544" ht="15.75" customHeight="1">
+    <row r="544" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B544" s="5"/>
     </row>
-    <row r="545" ht="15.75" customHeight="1">
+    <row r="545" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B545" s="5"/>
     </row>
-    <row r="546" ht="15.75" customHeight="1">
+    <row r="546" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B546" s="5"/>
     </row>
-    <row r="547" ht="15.75" customHeight="1">
+    <row r="547" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B547" s="5"/>
     </row>
-    <row r="548" ht="15.75" customHeight="1">
+    <row r="548" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B548" s="5"/>
     </row>
-    <row r="549" ht="15.75" customHeight="1">
+    <row r="549" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B549" s="5"/>
     </row>
-    <row r="550" ht="15.75" customHeight="1">
+    <row r="550" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B550" s="5"/>
     </row>
-    <row r="551" ht="15.75" customHeight="1">
+    <row r="551" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B551" s="5"/>
     </row>
-    <row r="552" ht="15.75" customHeight="1">
+    <row r="552" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B552" s="5"/>
     </row>
-    <row r="553" ht="15.75" customHeight="1">
+    <row r="553" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B553" s="5"/>
     </row>
-    <row r="554" ht="15.75" customHeight="1">
+    <row r="554" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B554" s="5"/>
     </row>
-    <row r="555" ht="15.75" customHeight="1">
+    <row r="555" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B555" s="5"/>
     </row>
-    <row r="556" ht="15.75" customHeight="1">
+    <row r="556" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B556" s="5"/>
     </row>
-    <row r="557" ht="15.75" customHeight="1">
+    <row r="557" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B557" s="5"/>
     </row>
-    <row r="558" ht="15.75" customHeight="1">
+    <row r="558" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B558" s="5"/>
     </row>
-    <row r="559" ht="15.75" customHeight="1">
+    <row r="559" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B559" s="5"/>
     </row>
-    <row r="560" ht="15.75" customHeight="1">
+    <row r="560" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B560" s="5"/>
     </row>
-    <row r="561" ht="15.75" customHeight="1">
+    <row r="561" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B561" s="5"/>
     </row>
-    <row r="562" ht="15.75" customHeight="1">
+    <row r="562" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B562" s="5"/>
     </row>
-    <row r="563" ht="15.75" customHeight="1">
+    <row r="563" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B563" s="5"/>
     </row>
-    <row r="564" ht="15.75" customHeight="1">
+    <row r="564" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B564" s="5"/>
     </row>
-    <row r="565" ht="15.75" customHeight="1">
+    <row r="565" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B565" s="5"/>
     </row>
-    <row r="566" ht="15.75" customHeight="1">
+    <row r="566" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B566" s="5"/>
     </row>
-    <row r="567" ht="15.75" customHeight="1">
+    <row r="567" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B567" s="5"/>
     </row>
-    <row r="568" ht="15.75" customHeight="1">
+    <row r="568" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B568" s="5"/>
     </row>
-    <row r="569" ht="15.75" customHeight="1">
+    <row r="569" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B569" s="5"/>
     </row>
-    <row r="570" ht="15.75" customHeight="1">
+    <row r="570" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B570" s="5"/>
     </row>
-    <row r="571" ht="15.75" customHeight="1">
+    <row r="571" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B571" s="5"/>
     </row>
-    <row r="572" ht="15.75" customHeight="1">
+    <row r="572" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B572" s="5"/>
     </row>
-    <row r="573" ht="15.75" customHeight="1">
+    <row r="573" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B573" s="5"/>
     </row>
-    <row r="574" ht="15.75" customHeight="1">
+    <row r="574" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B574" s="5"/>
     </row>
-    <row r="575" ht="15.75" customHeight="1">
+    <row r="575" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B575" s="5"/>
     </row>
-    <row r="576" ht="15.75" customHeight="1">
+    <row r="576" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B576" s="5"/>
     </row>
-    <row r="577" ht="15.75" customHeight="1">
+    <row r="577" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B577" s="5"/>
     </row>
-    <row r="578" ht="15.75" customHeight="1">
+    <row r="578" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B578" s="5"/>
     </row>
-    <row r="579" ht="15.75" customHeight="1">
+    <row r="579" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B579" s="5"/>
     </row>
-    <row r="580" ht="15.75" customHeight="1">
+    <row r="580" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B580" s="5"/>
     </row>
-    <row r="581" ht="15.75" customHeight="1">
+    <row r="581" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B581" s="5"/>
     </row>
-    <row r="582" ht="15.75" customHeight="1">
+    <row r="582" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B582" s="5"/>
     </row>
-    <row r="583" ht="15.75" customHeight="1">
+    <row r="583" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B583" s="5"/>
     </row>
-    <row r="584" ht="15.75" customHeight="1">
+    <row r="584" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B584" s="5"/>
     </row>
-    <row r="585" ht="15.75" customHeight="1">
+    <row r="585" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B585" s="5"/>
     </row>
-    <row r="586" ht="15.75" customHeight="1">
+    <row r="586" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B586" s="5"/>
     </row>
-    <row r="587" ht="15.75" customHeight="1">
+    <row r="587" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B587" s="5"/>
     </row>
-    <row r="588" ht="15.75" customHeight="1">
+    <row r="588" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B588" s="5"/>
     </row>
-    <row r="589" ht="15.75" customHeight="1">
+    <row r="589" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B589" s="5"/>
     </row>
-    <row r="590" ht="15.75" customHeight="1">
+    <row r="590" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B590" s="5"/>
     </row>
-    <row r="591" ht="15.75" customHeight="1">
+    <row r="591" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B591" s="5"/>
     </row>
-    <row r="592" ht="15.75" customHeight="1">
+    <row r="592" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B592" s="5"/>
     </row>
-    <row r="593" ht="15.75" customHeight="1">
+    <row r="593" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B593" s="5"/>
     </row>
-    <row r="594" ht="15.75" customHeight="1">
+    <row r="594" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B594" s="5"/>
     </row>
-    <row r="595" ht="15.75" customHeight="1">
+    <row r="595" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B595" s="5"/>
     </row>
-    <row r="596" ht="15.75" customHeight="1">
+    <row r="596" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B596" s="5"/>
     </row>
-    <row r="597" ht="15.75" customHeight="1">
+    <row r="597" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B597" s="5"/>
     </row>
-    <row r="598" ht="15.75" customHeight="1">
+    <row r="598" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B598" s="5"/>
     </row>
-    <row r="599" ht="15.75" customHeight="1">
+    <row r="599" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B599" s="5"/>
     </row>
-    <row r="600" ht="15.75" customHeight="1">
+    <row r="600" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B600" s="5"/>
     </row>
-    <row r="601" ht="15.75" customHeight="1">
+    <row r="601" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B601" s="5"/>
     </row>
-    <row r="602" ht="15.75" customHeight="1">
+    <row r="602" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B602" s="5"/>
     </row>
-    <row r="603" ht="15.75" customHeight="1">
+    <row r="603" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B603" s="5"/>
     </row>
-    <row r="604" ht="15.75" customHeight="1">
+    <row r="604" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B604" s="5"/>
     </row>
-    <row r="605" ht="15.75" customHeight="1">
+    <row r="605" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B605" s="5"/>
     </row>
-    <row r="606" ht="15.75" customHeight="1">
+    <row r="606" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B606" s="5"/>
     </row>
-    <row r="607" ht="15.75" customHeight="1">
+    <row r="607" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B607" s="5"/>
     </row>
-    <row r="608" ht="15.75" customHeight="1">
+    <row r="608" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B608" s="5"/>
     </row>
-    <row r="609" ht="15.75" customHeight="1">
+    <row r="609" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B609" s="5"/>
     </row>
-    <row r="610" ht="15.75" customHeight="1">
+    <row r="610" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B610" s="5"/>
     </row>
-    <row r="611" ht="15.75" customHeight="1">
+    <row r="611" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B611" s="5"/>
     </row>
-    <row r="612" ht="15.75" customHeight="1">
+    <row r="612" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B612" s="5"/>
     </row>
-    <row r="613" ht="15.75" customHeight="1">
+    <row r="613" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B613" s="5"/>
     </row>
-    <row r="614" ht="15.75" customHeight="1">
+    <row r="614" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B614" s="5"/>
     </row>
-    <row r="615" ht="15.75" customHeight="1">
+    <row r="615" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B615" s="5"/>
     </row>
-    <row r="616" ht="15.75" customHeight="1">
+    <row r="616" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B616" s="5"/>
     </row>
-    <row r="617" ht="15.75" customHeight="1">
+    <row r="617" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B617" s="5"/>
     </row>
-    <row r="618" ht="15.75" customHeight="1">
+    <row r="618" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B618" s="5"/>
     </row>
-    <row r="619" ht="15.75" customHeight="1">
+    <row r="619" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B619" s="5"/>
     </row>
-    <row r="620" ht="15.75" customHeight="1">
+    <row r="620" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B620" s="5"/>
     </row>
-    <row r="621" ht="15.75" customHeight="1">
+    <row r="621" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B621" s="5"/>
     </row>
-    <row r="622" ht="15.75" customHeight="1">
+    <row r="622" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B622" s="5"/>
     </row>
-    <row r="623" ht="15.75" customHeight="1">
+    <row r="623" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B623" s="5"/>
     </row>
-    <row r="624" ht="15.75" customHeight="1">
+    <row r="624" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B624" s="5"/>
     </row>
-    <row r="625" ht="15.75" customHeight="1">
+    <row r="625" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B625" s="5"/>
     </row>
-    <row r="626" ht="15.75" customHeight="1">
+    <row r="626" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B626" s="5"/>
     </row>
-    <row r="627" ht="15.75" customHeight="1">
+    <row r="627" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B627" s="5"/>
     </row>
-    <row r="628" ht="15.75" customHeight="1">
+    <row r="628" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B628" s="5"/>
     </row>
-    <row r="629" ht="15.75" customHeight="1">
+    <row r="629" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B629" s="5"/>
     </row>
-    <row r="630" ht="15.75" customHeight="1">
+    <row r="630" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B630" s="5"/>
     </row>
-    <row r="631" ht="15.75" customHeight="1">
+    <row r="631" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B631" s="5"/>
     </row>
-    <row r="632" ht="15.75" customHeight="1">
+    <row r="632" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B632" s="5"/>
     </row>
-    <row r="633" ht="15.75" customHeight="1">
+    <row r="633" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B633" s="5"/>
     </row>
-    <row r="634" ht="15.75" customHeight="1">
+    <row r="634" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B634" s="5"/>
     </row>
-    <row r="635" ht="15.75" customHeight="1">
+    <row r="635" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B635" s="5"/>
     </row>
-    <row r="636" ht="15.75" customHeight="1">
+    <row r="636" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B636" s="5"/>
     </row>
-    <row r="637" ht="15.75" customHeight="1">
+    <row r="637" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B637" s="5"/>
     </row>
-    <row r="638" ht="15.75" customHeight="1">
+    <row r="638" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B638" s="5"/>
     </row>
-    <row r="639" ht="15.75" customHeight="1">
+    <row r="639" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B639" s="5"/>
     </row>
-    <row r="640" ht="15.75" customHeight="1">
+    <row r="640" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B640" s="5"/>
     </row>
-    <row r="641" ht="15.75" customHeight="1">
+    <row r="641" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B641" s="5"/>
     </row>
-    <row r="642" ht="15.75" customHeight="1">
+    <row r="642" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B642" s="5"/>
     </row>
-    <row r="643" ht="15.75" customHeight="1">
+    <row r="643" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B643" s="5"/>
     </row>
-    <row r="644" ht="15.75" customHeight="1">
+    <row r="644" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B644" s="5"/>
     </row>
-    <row r="645" ht="15.75" customHeight="1">
+    <row r="645" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B645" s="5"/>
     </row>
-    <row r="646" ht="15.75" customHeight="1">
+    <row r="646" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B646" s="5"/>
     </row>
-    <row r="647" ht="15.75" customHeight="1">
+    <row r="647" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B647" s="5"/>
     </row>
-    <row r="648" ht="15.75" customHeight="1">
+    <row r="648" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B648" s="5"/>
     </row>
-    <row r="649" ht="15.75" customHeight="1">
+    <row r="649" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B649" s="5"/>
     </row>
-    <row r="650" ht="15.75" customHeight="1">
+    <row r="650" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B650" s="5"/>
     </row>
-    <row r="651" ht="15.75" customHeight="1">
+    <row r="651" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B651" s="5"/>
     </row>
-    <row r="652" ht="15.75" customHeight="1">
+    <row r="652" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B652" s="5"/>
     </row>
-    <row r="653" ht="15.75" customHeight="1">
+    <row r="653" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B653" s="5"/>
     </row>
-    <row r="654" ht="15.75" customHeight="1">
+    <row r="654" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B654" s="5"/>
     </row>
-    <row r="655" ht="15.75" customHeight="1">
+    <row r="655" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B655" s="5"/>
     </row>
-    <row r="656" ht="15.75" customHeight="1">
+    <row r="656" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B656" s="5"/>
     </row>
-    <row r="657" ht="15.75" customHeight="1">
+    <row r="657" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B657" s="5"/>
     </row>
-    <row r="658" ht="15.75" customHeight="1">
+    <row r="658" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B658" s="5"/>
     </row>
-    <row r="659" ht="15.75" customHeight="1">
+    <row r="659" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B659" s="5"/>
     </row>
-    <row r="660" ht="15.75" customHeight="1">
+    <row r="660" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B660" s="5"/>
     </row>
-    <row r="661" ht="15.75" customHeight="1">
+    <row r="661" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B661" s="5"/>
     </row>
-    <row r="662" ht="15.75" customHeight="1">
+    <row r="662" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B662" s="5"/>
     </row>
-    <row r="663" ht="15.75" customHeight="1">
+    <row r="663" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B663" s="5"/>
     </row>
-    <row r="664" ht="15.75" customHeight="1">
+    <row r="664" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B664" s="5"/>
     </row>
-    <row r="665" ht="15.75" customHeight="1">
+    <row r="665" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B665" s="5"/>
     </row>
-    <row r="666" ht="15.75" customHeight="1">
+    <row r="666" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B666" s="5"/>
     </row>
-    <row r="667" ht="15.75" customHeight="1">
+    <row r="667" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B667" s="5"/>
     </row>
-    <row r="668" ht="15.75" customHeight="1">
+    <row r="668" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B668" s="5"/>
     </row>
-    <row r="669" ht="15.75" customHeight="1">
+    <row r="669" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B669" s="5"/>
     </row>
-    <row r="670" ht="15.75" customHeight="1">
+    <row r="670" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B670" s="5"/>
     </row>
-    <row r="671" ht="15.75" customHeight="1">
+    <row r="671" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B671" s="5"/>
     </row>
-    <row r="672" ht="15.75" customHeight="1">
+    <row r="672" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B672" s="5"/>
     </row>
-    <row r="673" ht="15.75" customHeight="1">
+    <row r="673" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B673" s="5"/>
     </row>
-    <row r="674" ht="15.75" customHeight="1">
+    <row r="674" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B674" s="5"/>
     </row>
-    <row r="675" ht="15.75" customHeight="1">
+    <row r="675" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B675" s="5"/>
     </row>
-    <row r="676" ht="15.75" customHeight="1">
+    <row r="676" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B676" s="5"/>
     </row>
-    <row r="677" ht="15.75" customHeight="1">
+    <row r="677" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B677" s="5"/>
     </row>
-    <row r="678" ht="15.75" customHeight="1">
+    <row r="678" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B678" s="5"/>
     </row>
-    <row r="679" ht="15.75" customHeight="1">
+    <row r="679" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B679" s="5"/>
     </row>
-    <row r="680" ht="15.75" customHeight="1">
+    <row r="680" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B680" s="5"/>
     </row>
-    <row r="681" ht="15.75" customHeight="1">
+    <row r="681" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B681" s="5"/>
     </row>
-    <row r="682" ht="15.75" customHeight="1">
+    <row r="682" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B682" s="5"/>
     </row>
-    <row r="683" ht="15.75" customHeight="1">
+    <row r="683" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B683" s="5"/>
     </row>
-    <row r="684" ht="15.75" customHeight="1">
+    <row r="684" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B684" s="5"/>
     </row>
-    <row r="685" ht="15.75" customHeight="1">
+    <row r="685" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B685" s="5"/>
     </row>
-    <row r="686" ht="15.75" customHeight="1">
+    <row r="686" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B686" s="5"/>
     </row>
-    <row r="687" ht="15.75" customHeight="1">
+    <row r="687" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B687" s="5"/>
     </row>
-    <row r="688" ht="15.75" customHeight="1">
+    <row r="688" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B688" s="5"/>
     </row>
-    <row r="689" ht="15.75" customHeight="1">
+    <row r="689" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B689" s="5"/>
     </row>
-    <row r="690" ht="15.75" customHeight="1">
+    <row r="690" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B690" s="5"/>
     </row>
-    <row r="691" ht="15.75" customHeight="1">
+    <row r="691" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B691" s="5"/>
     </row>
-    <row r="692" ht="15.75" customHeight="1">
+    <row r="692" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B692" s="5"/>
     </row>
-    <row r="693" ht="15.75" customHeight="1">
+    <row r="693" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B693" s="5"/>
     </row>
-    <row r="694" ht="15.75" customHeight="1">
+    <row r="694" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B694" s="5"/>
     </row>
-    <row r="695" ht="15.75" customHeight="1">
+    <row r="695" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B695" s="5"/>
     </row>
-    <row r="696" ht="15.75" customHeight="1">
+    <row r="696" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B696" s="5"/>
     </row>
-    <row r="697" ht="15.75" customHeight="1">
+    <row r="697" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B697" s="5"/>
     </row>
-    <row r="698" ht="15.75" customHeight="1">
+    <row r="698" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B698" s="5"/>
     </row>
-    <row r="699" ht="15.75" customHeight="1">
+    <row r="699" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B699" s="5"/>
     </row>
-    <row r="700" ht="15.75" customHeight="1">
+    <row r="700" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B700" s="5"/>
     </row>
-    <row r="701" ht="15.75" customHeight="1">
+    <row r="701" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B701" s="5"/>
     </row>
-    <row r="702" ht="15.75" customHeight="1">
+    <row r="702" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B702" s="5"/>
     </row>
-    <row r="703" ht="15.75" customHeight="1">
+    <row r="703" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B703" s="5"/>
     </row>
-    <row r="704" ht="15.75" customHeight="1">
+    <row r="704" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B704" s="5"/>
     </row>
-    <row r="705" ht="15.75" customHeight="1">
+    <row r="705" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B705" s="5"/>
     </row>
-    <row r="706" ht="15.75" customHeight="1">
+    <row r="706" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B706" s="5"/>
     </row>
-    <row r="707" ht="15.75" customHeight="1">
+    <row r="707" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B707" s="5"/>
     </row>
-    <row r="708" ht="15.75" customHeight="1">
+    <row r="708" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B708" s="5"/>
     </row>
-    <row r="709" ht="15.75" customHeight="1">
+    <row r="709" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B709" s="5"/>
     </row>
-    <row r="710" ht="15.75" customHeight="1">
+    <row r="710" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B710" s="5"/>
     </row>
-    <row r="711" ht="15.75" customHeight="1">
+    <row r="711" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B711" s="5"/>
     </row>
-    <row r="712" ht="15.75" customHeight="1">
+    <row r="712" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B712" s="5"/>
     </row>
-    <row r="713" ht="15.75" customHeight="1">
+    <row r="713" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B713" s="5"/>
     </row>
-    <row r="714" ht="15.75" customHeight="1">
+    <row r="714" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B714" s="5"/>
     </row>
-    <row r="715" ht="15.75" customHeight="1">
+    <row r="715" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B715" s="5"/>
     </row>
-    <row r="716" ht="15.75" customHeight="1">
+    <row r="716" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B716" s="5"/>
     </row>
-    <row r="717" ht="15.75" customHeight="1">
+    <row r="717" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B717" s="5"/>
     </row>
-    <row r="718" ht="15.75" customHeight="1">
+    <row r="718" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B718" s="5"/>
     </row>
-    <row r="719" ht="15.75" customHeight="1">
+    <row r="719" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B719" s="5"/>
     </row>
-    <row r="720" ht="15.75" customHeight="1">
+    <row r="720" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B720" s="5"/>
     </row>
-    <row r="721" ht="15.75" customHeight="1">
+    <row r="721" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B721" s="5"/>
     </row>
-    <row r="722" ht="15.75" customHeight="1">
+    <row r="722" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B722" s="5"/>
     </row>
-    <row r="723" ht="15.75" customHeight="1">
+    <row r="723" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B723" s="5"/>
     </row>
-    <row r="724" ht="15.75" customHeight="1">
+    <row r="724" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B724" s="5"/>
     </row>
-    <row r="725" ht="15.75" customHeight="1">
+    <row r="725" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B725" s="5"/>
     </row>
-    <row r="726" ht="15.75" customHeight="1">
+    <row r="726" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B726" s="5"/>
     </row>
-    <row r="727" ht="15.75" customHeight="1">
+    <row r="727" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B727" s="5"/>
     </row>
-    <row r="728" ht="15.75" customHeight="1">
+    <row r="728" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B728" s="5"/>
     </row>
-    <row r="729" ht="15.75" customHeight="1">
+    <row r="729" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B729" s="5"/>
     </row>
-    <row r="730" ht="15.75" customHeight="1">
+    <row r="730" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B730" s="5"/>
     </row>
-    <row r="731" ht="15.75" customHeight="1">
+    <row r="731" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B731" s="5"/>
     </row>
-    <row r="732" ht="15.75" customHeight="1">
+    <row r="732" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B732" s="5"/>
     </row>
-    <row r="733" ht="15.75" customHeight="1">
+    <row r="733" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B733" s="5"/>
     </row>
-    <row r="734" ht="15.75" customHeight="1">
+    <row r="734" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B734" s="5"/>
     </row>
-    <row r="735" ht="15.75" customHeight="1">
+    <row r="735" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B735" s="5"/>
     </row>
-    <row r="736" ht="15.75" customHeight="1">
+    <row r="736" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B736" s="5"/>
     </row>
-    <row r="737" ht="15.75" customHeight="1">
+    <row r="737" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B737" s="5"/>
     </row>
-    <row r="738" ht="15.75" customHeight="1">
+    <row r="738" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B738" s="5"/>
     </row>
-    <row r="739" ht="15.75" customHeight="1">
+    <row r="739" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B739" s="5"/>
     </row>
-    <row r="740" ht="15.75" customHeight="1">
+    <row r="740" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B740" s="5"/>
     </row>
-    <row r="741" ht="15.75" customHeight="1">
+    <row r="741" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B741" s="5"/>
     </row>
-    <row r="742" ht="15.75" customHeight="1">
+    <row r="742" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B742" s="5"/>
     </row>
-    <row r="743" ht="15.75" customHeight="1">
+    <row r="743" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B743" s="5"/>
     </row>
-    <row r="744" ht="15.75" customHeight="1">
+    <row r="744" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B744" s="5"/>
     </row>
-    <row r="745" ht="15.75" customHeight="1">
+    <row r="745" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B745" s="5"/>
     </row>
-    <row r="746" ht="15.75" customHeight="1">
+    <row r="746" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B746" s="5"/>
     </row>
-    <row r="747" ht="15.75" customHeight="1">
+    <row r="747" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B747" s="5"/>
     </row>
-    <row r="748" ht="15.75" customHeight="1">
+    <row r="748" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B748" s="5"/>
     </row>
-    <row r="749" ht="15.75" customHeight="1">
+    <row r="749" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B749" s="5"/>
     </row>
-    <row r="750" ht="15.75" customHeight="1">
+    <row r="750" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B750" s="5"/>
     </row>
-    <row r="751" ht="15.75" customHeight="1">
+    <row r="751" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B751" s="5"/>
     </row>
-    <row r="752" ht="15.75" customHeight="1">
+    <row r="752" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B752" s="5"/>
     </row>
-    <row r="753" ht="15.75" customHeight="1">
+    <row r="753" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B753" s="5"/>
     </row>
-    <row r="754" ht="15.75" customHeight="1">
+    <row r="754" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B754" s="5"/>
     </row>
-    <row r="755" ht="15.75" customHeight="1">
+    <row r="755" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B755" s="5"/>
     </row>
-    <row r="756" ht="15.75" customHeight="1">
+    <row r="756" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B756" s="5"/>
     </row>
-    <row r="757" ht="15.75" customHeight="1">
+    <row r="757" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B757" s="5"/>
     </row>
-    <row r="758" ht="15.75" customHeight="1">
+    <row r="758" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B758" s="5"/>
     </row>
-    <row r="759" ht="15.75" customHeight="1">
+    <row r="759" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B759" s="5"/>
     </row>
-    <row r="760" ht="15.75" customHeight="1">
+    <row r="760" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B760" s="5"/>
     </row>
-    <row r="761" ht="15.75" customHeight="1">
+    <row r="761" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B761" s="5"/>
     </row>
-    <row r="762" ht="15.75" customHeight="1">
+    <row r="762" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B762" s="5"/>
     </row>
-    <row r="763" ht="15.75" customHeight="1">
+    <row r="763" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B763" s="5"/>
     </row>
-    <row r="764" ht="15.75" customHeight="1">
+    <row r="764" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B764" s="5"/>
     </row>
-    <row r="765" ht="15.75" customHeight="1">
+    <row r="765" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B765" s="5"/>
     </row>
-    <row r="766" ht="15.75" customHeight="1">
+    <row r="766" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B766" s="5"/>
     </row>
-    <row r="767" ht="15.75" customHeight="1">
+    <row r="767" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B767" s="5"/>
     </row>
-    <row r="768" ht="15.75" customHeight="1">
+    <row r="768" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B768" s="5"/>
     </row>
-    <row r="769" ht="15.75" customHeight="1">
+    <row r="769" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B769" s="5"/>
     </row>
-    <row r="770" ht="15.75" customHeight="1">
+    <row r="770" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B770" s="5"/>
     </row>
-    <row r="771" ht="15.75" customHeight="1">
+    <row r="771" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B771" s="5"/>
     </row>
-    <row r="772" ht="15.75" customHeight="1">
+    <row r="772" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B772" s="5"/>
     </row>
-    <row r="773" ht="15.75" customHeight="1">
+    <row r="773" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B773" s="5"/>
     </row>
-    <row r="774" ht="15.75" customHeight="1">
+    <row r="774" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B774" s="5"/>
     </row>
-    <row r="775" ht="15.75" customHeight="1">
+    <row r="775" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B775" s="5"/>
     </row>
-    <row r="776" ht="15.75" customHeight="1">
+    <row r="776" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B776" s="5"/>
     </row>
-    <row r="777" ht="15.75" customHeight="1">
+    <row r="777" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B777" s="5"/>
     </row>
-    <row r="778" ht="15.75" customHeight="1">
+    <row r="778" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B778" s="5"/>
     </row>
-    <row r="779" ht="15.75" customHeight="1">
+    <row r="779" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B779" s="5"/>
     </row>
-    <row r="780" ht="15.75" customHeight="1">
+    <row r="780" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B780" s="5"/>
     </row>
-    <row r="781" ht="15.75" customHeight="1">
+    <row r="781" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B781" s="5"/>
     </row>
-    <row r="782" ht="15.75" customHeight="1">
+    <row r="782" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B782" s="5"/>
     </row>
-    <row r="783" ht="15.75" customHeight="1">
+    <row r="783" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B783" s="5"/>
     </row>
-    <row r="784" ht="15.75" customHeight="1">
+    <row r="784" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B784" s="5"/>
     </row>
-    <row r="785" ht="15.75" customHeight="1">
+    <row r="785" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B785" s="5"/>
     </row>
-    <row r="786" ht="15.75" customHeight="1">
+    <row r="786" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B786" s="5"/>
     </row>
-    <row r="787" ht="15.75" customHeight="1">
+    <row r="787" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B787" s="5"/>
     </row>
-    <row r="788" ht="15.75" customHeight="1">
+    <row r="788" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B788" s="5"/>
     </row>
-    <row r="789" ht="15.75" customHeight="1">
+    <row r="789" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B789" s="5"/>
     </row>
-    <row r="790" ht="15.75" customHeight="1">
+    <row r="790" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B790" s="5"/>
     </row>
-    <row r="791" ht="15.75" customHeight="1">
+    <row r="791" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B791" s="5"/>
     </row>
-    <row r="792" ht="15.75" customHeight="1">
+    <row r="792" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B792" s="5"/>
     </row>
-    <row r="793" ht="15.75" customHeight="1">
+    <row r="793" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B793" s="5"/>
     </row>
-    <row r="794" ht="15.75" customHeight="1">
+    <row r="794" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B794" s="5"/>
     </row>
-    <row r="795" ht="15.75" customHeight="1">
+    <row r="795" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B795" s="5"/>
     </row>
-    <row r="796" ht="15.75" customHeight="1">
+    <row r="796" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B796" s="5"/>
     </row>
-    <row r="797" ht="15.75" customHeight="1">
+    <row r="797" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B797" s="5"/>
     </row>
-    <row r="798" ht="15.75" customHeight="1">
+    <row r="798" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B798" s="5"/>
     </row>
-    <row r="799" ht="15.75" customHeight="1">
+    <row r="799" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B799" s="5"/>
     </row>
-    <row r="800" ht="15.75" customHeight="1">
+    <row r="800" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B800" s="5"/>
     </row>
-    <row r="801" ht="15.75" customHeight="1">
+    <row r="801" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B801" s="5"/>
     </row>
-    <row r="802" ht="15.75" customHeight="1">
+    <row r="802" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B802" s="5"/>
     </row>
-    <row r="803" ht="15.75" customHeight="1">
+    <row r="803" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B803" s="5"/>
     </row>
-    <row r="804" ht="15.75" customHeight="1">
+    <row r="804" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B804" s="5"/>
     </row>
-    <row r="805" ht="15.75" customHeight="1">
+    <row r="805" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B805" s="5"/>
     </row>
-    <row r="806" ht="15.75" customHeight="1">
+    <row r="806" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B806" s="5"/>
     </row>
-    <row r="807" ht="15.75" customHeight="1">
+    <row r="807" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B807" s="5"/>
     </row>
-    <row r="808" ht="15.75" customHeight="1">
+    <row r="808" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B808" s="5"/>
     </row>
-    <row r="809" ht="15.75" customHeight="1">
+    <row r="809" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B809" s="5"/>
     </row>
-    <row r="810" ht="15.75" customHeight="1">
+    <row r="810" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B810" s="5"/>
     </row>
-    <row r="811" ht="15.75" customHeight="1">
+    <row r="811" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B811" s="5"/>
     </row>
-    <row r="812" ht="15.75" customHeight="1">
+    <row r="812" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B812" s="5"/>
     </row>
-    <row r="813" ht="15.75" customHeight="1">
+    <row r="813" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B813" s="5"/>
     </row>
-    <row r="814" ht="15.75" customHeight="1">
+    <row r="814" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B814" s="5"/>
     </row>
-    <row r="815" ht="15.75" customHeight="1">
+    <row r="815" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B815" s="5"/>
     </row>
-    <row r="816" ht="15.75" customHeight="1">
+    <row r="816" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B816" s="5"/>
     </row>
-    <row r="817" ht="15.75" customHeight="1">
+    <row r="817" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B817" s="5"/>
     </row>
-    <row r="818" ht="15.75" customHeight="1">
+    <row r="818" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B818" s="5"/>
     </row>
-    <row r="819" ht="15.75" customHeight="1">
+    <row r="819" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B819" s="5"/>
     </row>
-    <row r="820" ht="15.75" customHeight="1">
+    <row r="820" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B820" s="5"/>
     </row>
-    <row r="821" ht="15.75" customHeight="1">
+    <row r="821" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B821" s="5"/>
     </row>
-    <row r="822" ht="15.75" customHeight="1">
+    <row r="822" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B822" s="5"/>
     </row>
-    <row r="823" ht="15.75" customHeight="1">
+    <row r="823" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B823" s="5"/>
     </row>
-    <row r="824" ht="15.75" customHeight="1">
+    <row r="824" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B824" s="5"/>
     </row>
-    <row r="825" ht="15.75" customHeight="1">
+    <row r="825" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B825" s="5"/>
     </row>
-    <row r="826" ht="15.75" customHeight="1">
+    <row r="826" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B826" s="5"/>
     </row>
-    <row r="827" ht="15.75" customHeight="1">
+    <row r="827" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B827" s="5"/>
     </row>
-    <row r="828" ht="15.75" customHeight="1">
+    <row r="828" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B828" s="5"/>
     </row>
-    <row r="829" ht="15.75" customHeight="1">
+    <row r="829" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B829" s="5"/>
     </row>
-    <row r="830" ht="15.75" customHeight="1">
+    <row r="830" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B830" s="5"/>
     </row>
-    <row r="831" ht="15.75" customHeight="1">
+    <row r="831" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B831" s="5"/>
     </row>
-    <row r="832" ht="15.75" customHeight="1">
+    <row r="832" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B832" s="5"/>
     </row>
-    <row r="833" ht="15.75" customHeight="1">
+    <row r="833" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B833" s="5"/>
     </row>
-    <row r="834" ht="15.75" customHeight="1">
+    <row r="834" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B834" s="5"/>
     </row>
-    <row r="835" ht="15.75" customHeight="1">
+    <row r="835" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B835" s="5"/>
     </row>
-    <row r="836" ht="15.75" customHeight="1">
+    <row r="836" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B836" s="5"/>
     </row>
-    <row r="837" ht="15.75" customHeight="1">
+    <row r="837" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B837" s="5"/>
     </row>
-    <row r="838" ht="15.75" customHeight="1">
+    <row r="838" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B838" s="5"/>
     </row>
-    <row r="839" ht="15.75" customHeight="1">
+    <row r="839" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B839" s="5"/>
     </row>
-    <row r="840" ht="15.75" customHeight="1">
+    <row r="840" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B840" s="5"/>
     </row>
-    <row r="841" ht="15.75" customHeight="1">
+    <row r="841" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B841" s="5"/>
     </row>
-    <row r="842" ht="15.75" customHeight="1">
+    <row r="842" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B842" s="5"/>
     </row>
-    <row r="843" ht="15.75" customHeight="1">
+    <row r="843" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B843" s="5"/>
     </row>
-    <row r="844" ht="15.75" customHeight="1">
+    <row r="844" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B844" s="5"/>
     </row>
-    <row r="845" ht="15.75" customHeight="1">
+    <row r="845" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B845" s="5"/>
     </row>
-    <row r="846" ht="15.75" customHeight="1">
+    <row r="846" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B846" s="5"/>
     </row>
-    <row r="847" ht="15.75" customHeight="1">
+    <row r="847" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B847" s="5"/>
     </row>
-    <row r="848" ht="15.75" customHeight="1">
+    <row r="848" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B848" s="5"/>
     </row>
-    <row r="849" ht="15.75" customHeight="1">
+    <row r="849" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B849" s="5"/>
     </row>
-    <row r="850" ht="15.75" customHeight="1">
+    <row r="850" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B850" s="5"/>
     </row>
-    <row r="851" ht="15.75" customHeight="1">
+    <row r="851" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B851" s="5"/>
     </row>
-    <row r="852" ht="15.75" customHeight="1">
+    <row r="852" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B852" s="5"/>
     </row>
-    <row r="853" ht="15.75" customHeight="1">
+    <row r="853" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B853" s="5"/>
     </row>
-    <row r="854" ht="15.75" customHeight="1">
+    <row r="854" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B854" s="5"/>
     </row>
-    <row r="855" ht="15.75" customHeight="1">
+    <row r="855" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B855" s="5"/>
     </row>
-    <row r="856" ht="15.75" customHeight="1">
+    <row r="856" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B856" s="5"/>
     </row>
-    <row r="857" ht="15.75" customHeight="1">
+    <row r="857" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B857" s="5"/>
     </row>
-    <row r="858" ht="15.75" customHeight="1">
+    <row r="858" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B858" s="5"/>
     </row>
-    <row r="859" ht="15.75" customHeight="1">
+    <row r="859" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B859" s="5"/>
     </row>
-    <row r="860" ht="15.75" customHeight="1">
+    <row r="860" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B860" s="5"/>
     </row>
-    <row r="861" ht="15.75" customHeight="1">
+    <row r="861" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B861" s="5"/>
     </row>
-    <row r="862" ht="15.75" customHeight="1">
+    <row r="862" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B862" s="5"/>
     </row>
-    <row r="863" ht="15.75" customHeight="1">
+    <row r="863" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B863" s="5"/>
     </row>
-    <row r="864" ht="15.75" customHeight="1">
+    <row r="864" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B864" s="5"/>
     </row>
-    <row r="865" ht="15.75" customHeight="1">
+    <row r="865" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B865" s="5"/>
     </row>
-    <row r="866" ht="15.75" customHeight="1">
+    <row r="866" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B866" s="5"/>
     </row>
-    <row r="867" ht="15.75" customHeight="1">
+    <row r="867" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B867" s="5"/>
     </row>
-    <row r="868" ht="15.75" customHeight="1">
+    <row r="868" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B868" s="5"/>
     </row>
-    <row r="869" ht="15.75" customHeight="1">
+    <row r="869" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B869" s="5"/>
     </row>
-    <row r="870" ht="15.75" customHeight="1">
+    <row r="870" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B870" s="5"/>
     </row>
-    <row r="871" ht="15.75" customHeight="1">
+    <row r="871" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B871" s="5"/>
     </row>
-    <row r="872" ht="15.75" customHeight="1">
+    <row r="872" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B872" s="5"/>
     </row>
-    <row r="873" ht="15.75" customHeight="1">
+    <row r="873" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B873" s="5"/>
     </row>
-    <row r="874" ht="15.75" customHeight="1">
+    <row r="874" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B874" s="5"/>
     </row>
-    <row r="875" ht="15.75" customHeight="1">
+    <row r="875" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B875" s="5"/>
     </row>
-    <row r="876" ht="15.75" customHeight="1">
+    <row r="876" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B876" s="5"/>
     </row>
-    <row r="877" ht="15.75" customHeight="1">
+    <row r="877" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B877" s="5"/>
     </row>
-    <row r="878" ht="15.75" customHeight="1">
+    <row r="878" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B878" s="5"/>
     </row>
-    <row r="879" ht="15.75" customHeight="1">
+    <row r="879" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B879" s="5"/>
     </row>
-    <row r="880" ht="15.75" customHeight="1">
+    <row r="880" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B880" s="5"/>
     </row>
-    <row r="881" ht="15.75" customHeight="1">
+    <row r="881" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B881" s="5"/>
     </row>
-    <row r="882" ht="15.75" customHeight="1">
+    <row r="882" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B882" s="5"/>
     </row>
-    <row r="883" ht="15.75" customHeight="1">
+    <row r="883" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B883" s="5"/>
     </row>
-    <row r="884" ht="15.75" customHeight="1">
+    <row r="884" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B884" s="5"/>
     </row>
-    <row r="885" ht="15.75" customHeight="1">
+    <row r="885" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B885" s="5"/>
     </row>
-    <row r="886" ht="15.75" customHeight="1">
+    <row r="886" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B886" s="5"/>
     </row>
-    <row r="887" ht="15.75" customHeight="1">
+    <row r="887" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B887" s="5"/>
     </row>
-    <row r="888" ht="15.75" customHeight="1">
+    <row r="888" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B888" s="5"/>
     </row>
-    <row r="889" ht="15.75" customHeight="1">
+    <row r="889" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B889" s="5"/>
     </row>
-    <row r="890" ht="15.75" customHeight="1">
+    <row r="890" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B890" s="5"/>
     </row>
-    <row r="891" ht="15.75" customHeight="1">
+    <row r="891" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B891" s="5"/>
     </row>
-    <row r="892" ht="15.75" customHeight="1">
+    <row r="892" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B892" s="5"/>
     </row>
-    <row r="893" ht="15.75" customHeight="1">
+    <row r="893" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B893" s="5"/>
     </row>
-    <row r="894" ht="15.75" customHeight="1">
+    <row r="894" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B894" s="5"/>
     </row>
-    <row r="895" ht="15.75" customHeight="1">
+    <row r="895" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B895" s="5"/>
     </row>
-    <row r="896" ht="15.75" customHeight="1">
+    <row r="896" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B896" s="5"/>
     </row>
-    <row r="897" ht="15.75" customHeight="1">
+    <row r="897" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B897" s="5"/>
     </row>
-    <row r="898" ht="15.75" customHeight="1">
+    <row r="898" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B898" s="5"/>
     </row>
-    <row r="899" ht="15.75" customHeight="1">
+    <row r="899" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B899" s="5"/>
     </row>
-    <row r="900" ht="15.75" customHeight="1">
+    <row r="900" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B900" s="5"/>
     </row>
-    <row r="901" ht="15.75" customHeight="1">
+    <row r="901" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B901" s="5"/>
     </row>
-    <row r="902" ht="15.75" customHeight="1">
+    <row r="902" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B902" s="5"/>
     </row>
-    <row r="903" ht="15.75" customHeight="1">
+    <row r="903" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B903" s="5"/>
     </row>
-    <row r="904" ht="15.75" customHeight="1">
+    <row r="904" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B904" s="5"/>
     </row>
-    <row r="905" ht="15.75" customHeight="1">
+    <row r="905" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B905" s="5"/>
     </row>
-    <row r="906" ht="15.75" customHeight="1">
+    <row r="906" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B906" s="5"/>
     </row>
-    <row r="907" ht="15.75" customHeight="1">
+    <row r="907" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B907" s="5"/>
     </row>
-    <row r="908" ht="15.75" customHeight="1">
+    <row r="908" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B908" s="5"/>
     </row>
-    <row r="909" ht="15.75" customHeight="1">
+    <row r="909" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B909" s="5"/>
     </row>
-    <row r="910" ht="15.75" customHeight="1">
+    <row r="910" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B910" s="5"/>
     </row>
-    <row r="911" ht="15.75" customHeight="1">
+    <row r="911" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B911" s="5"/>
     </row>
-    <row r="912" ht="15.75" customHeight="1">
+    <row r="912" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B912" s="5"/>
     </row>
-    <row r="913" ht="15.75" customHeight="1">
+    <row r="913" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B913" s="5"/>
     </row>
-    <row r="914" ht="15.75" customHeight="1">
+    <row r="914" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B914" s="5"/>
     </row>
-    <row r="915" ht="15.75" customHeight="1">
+    <row r="915" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B915" s="5"/>
     </row>
-    <row r="916" ht="15.75" customHeight="1">
+    <row r="916" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B916" s="5"/>
     </row>
-    <row r="917" ht="15.75" customHeight="1">
+    <row r="917" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B917" s="5"/>
     </row>
-    <row r="918" ht="15.75" customHeight="1">
+    <row r="918" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B918" s="5"/>
     </row>
-    <row r="919" ht="15.75" customHeight="1">
+    <row r="919" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B919" s="5"/>
     </row>
-    <row r="920" ht="15.75" customHeight="1">
+    <row r="920" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B920" s="5"/>
     </row>
-    <row r="921" ht="15.75" customHeight="1">
+    <row r="921" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B921" s="5"/>
     </row>
-    <row r="922" ht="15.75" customHeight="1">
+    <row r="922" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B922" s="5"/>
     </row>
-    <row r="923" ht="15.75" customHeight="1">
+    <row r="923" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B923" s="5"/>
     </row>
-    <row r="924" ht="15.75" customHeight="1">
+    <row r="924" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B924" s="5"/>
     </row>
-    <row r="925" ht="15.75" customHeight="1">
+    <row r="925" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B925" s="5"/>
     </row>
-    <row r="926" ht="15.75" customHeight="1">
+    <row r="926" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B926" s="5"/>
     </row>
-    <row r="927" ht="15.75" customHeight="1">
+    <row r="927" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B927" s="5"/>
     </row>
-    <row r="928" ht="15.75" customHeight="1">
+    <row r="928" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B928" s="5"/>
     </row>
-    <row r="929" ht="15.75" customHeight="1">
+    <row r="929" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B929" s="5"/>
     </row>
-    <row r="930" ht="15.75" customHeight="1">
+    <row r="930" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B930" s="5"/>
     </row>
-    <row r="931" ht="15.75" customHeight="1">
+    <row r="931" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B931" s="5"/>
     </row>
-    <row r="932" ht="15.75" customHeight="1">
+    <row r="932" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B932" s="5"/>
     </row>
-    <row r="933" ht="15.75" customHeight="1">
+    <row r="933" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B933" s="5"/>
     </row>
-    <row r="934" ht="15.75" customHeight="1">
+    <row r="934" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B934" s="5"/>
     </row>
-    <row r="935" ht="15.75" customHeight="1">
+    <row r="935" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B935" s="5"/>
     </row>
-    <row r="936" ht="15.75" customHeight="1">
+    <row r="936" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B936" s="5"/>
     </row>
-    <row r="937" ht="15.75" customHeight="1">
+    <row r="937" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B937" s="5"/>
     </row>
-    <row r="938" ht="15.75" customHeight="1">
+    <row r="938" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B938" s="5"/>
     </row>
-    <row r="939" ht="15.75" customHeight="1">
+    <row r="939" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B939" s="5"/>
     </row>
-    <row r="940" ht="15.75" customHeight="1">
+    <row r="940" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B940" s="5"/>
     </row>
-    <row r="941" ht="15.75" customHeight="1">
+    <row r="941" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B941" s="5"/>
     </row>
-    <row r="942" ht="15.75" customHeight="1">
+    <row r="942" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B942" s="5"/>
     </row>
-    <row r="943" ht="15.75" customHeight="1">
+    <row r="943" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B943" s="5"/>
     </row>
-    <row r="944" ht="15.75" customHeight="1">
+    <row r="944" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B944" s="5"/>
     </row>
-    <row r="945" ht="15.75" customHeight="1">
+    <row r="945" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B945" s="5"/>
     </row>
-    <row r="946" ht="15.75" customHeight="1">
+    <row r="946" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B946" s="5"/>
     </row>
-    <row r="947" ht="15.75" customHeight="1">
+    <row r="947" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B947" s="5"/>
     </row>
-    <row r="948" ht="15.75" customHeight="1">
+    <row r="948" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B948" s="5"/>
     </row>
-    <row r="949" ht="15.75" customHeight="1">
+    <row r="949" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B949" s="5"/>
     </row>
-    <row r="950" ht="15.75" customHeight="1">
+    <row r="950" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B950" s="5"/>
     </row>
-    <row r="951" ht="15.75" customHeight="1">
+    <row r="951" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B951" s="5"/>
     </row>
-    <row r="952" ht="15.75" customHeight="1">
+    <row r="952" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B952" s="5"/>
     </row>
-    <row r="953" ht="15.75" customHeight="1">
+    <row r="953" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B953" s="5"/>
     </row>
-    <row r="954" ht="15.75" customHeight="1">
+    <row r="954" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B954" s="5"/>
     </row>
-    <row r="955" ht="15.75" customHeight="1">
+    <row r="955" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B955" s="5"/>
     </row>
-    <row r="956" ht="15.75" customHeight="1">
+    <row r="956" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B956" s="5"/>
     </row>
-    <row r="957" ht="15.75" customHeight="1">
+    <row r="957" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B957" s="5"/>
     </row>
-    <row r="958" ht="15.75" customHeight="1">
+    <row r="958" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B958" s="5"/>
     </row>
-    <row r="959" ht="15.75" customHeight="1">
+    <row r="959" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B959" s="5"/>
     </row>
-    <row r="960" ht="15.75" customHeight="1">
+    <row r="960" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B960" s="5"/>
     </row>
-    <row r="961" ht="15.75" customHeight="1">
+    <row r="961" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B961" s="5"/>
     </row>
-    <row r="962" ht="15.75" customHeight="1">
+    <row r="962" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B962" s="5"/>
     </row>
-    <row r="963" ht="15.75" customHeight="1">
+    <row r="963" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B963" s="5"/>
     </row>
-    <row r="964" ht="15.75" customHeight="1">
+    <row r="964" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B964" s="5"/>
     </row>
-    <row r="965" ht="15.75" customHeight="1">
+    <row r="965" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B965" s="5"/>
     </row>
-    <row r="966" ht="15.75" customHeight="1">
+    <row r="966" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B966" s="5"/>
     </row>
-    <row r="967" ht="15.75" customHeight="1">
+    <row r="967" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B967" s="5"/>
     </row>
-    <row r="968" ht="15.75" customHeight="1">
+    <row r="968" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B968" s="5"/>
     </row>
-    <row r="969" ht="15.75" customHeight="1">
+    <row r="969" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B969" s="5"/>
     </row>
-    <row r="970" ht="15.75" customHeight="1">
+    <row r="970" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B970" s="5"/>
     </row>
-    <row r="971" ht="15.75" customHeight="1">
+    <row r="971" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B971" s="5"/>
     </row>
-    <row r="972" ht="15.75" customHeight="1">
+    <row r="972" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B972" s="5"/>
     </row>
-    <row r="973" ht="15.75" customHeight="1">
+    <row r="973" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B973" s="5"/>
     </row>
-    <row r="974" ht="15.75" customHeight="1">
+    <row r="974" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B974" s="5"/>
     </row>
-    <row r="975" ht="15.75" customHeight="1">
+    <row r="975" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B975" s="5"/>
     </row>
-    <row r="976" ht="15.75" customHeight="1">
+    <row r="976" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B976" s="5"/>
     </row>
-    <row r="977" ht="15.75" customHeight="1">
+    <row r="977" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B977" s="5"/>
     </row>
-    <row r="978" ht="15.75" customHeight="1">
+    <row r="978" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B978" s="5"/>
     </row>
-    <row r="979" ht="15.75" customHeight="1">
+    <row r="979" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B979" s="5"/>
     </row>
-    <row r="980" ht="15.75" customHeight="1">
+    <row r="980" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B980" s="5"/>
     </row>
-    <row r="981" ht="15.75" customHeight="1">
+    <row r="981" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B981" s="5"/>
     </row>
-    <row r="982" ht="15.75" customHeight="1">
+    <row r="982" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B982" s="5"/>
     </row>
-    <row r="983" ht="15.75" customHeight="1">
+    <row r="983" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B983" s="5"/>
     </row>
-    <row r="984" ht="15.75" customHeight="1">
+    <row r="984" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B984" s="5"/>
     </row>
-    <row r="985" ht="15.75" customHeight="1">
+    <row r="985" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B985" s="5"/>
     </row>
-    <row r="986" ht="15.75" customHeight="1">
+    <row r="986" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B986" s="5"/>
     </row>
-    <row r="987" ht="15.75" customHeight="1">
+    <row r="987" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B987" s="5"/>
     </row>
-    <row r="988" ht="15.75" customHeight="1">
+    <row r="988" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B988" s="5"/>
     </row>
-    <row r="989" ht="15.75" customHeight="1">
+    <row r="989" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B989" s="5"/>
     </row>
-    <row r="990" ht="15.75" customHeight="1">
+    <row r="990" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B990" s="5"/>
     </row>
-    <row r="991" ht="15.75" customHeight="1">
+    <row r="991" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B991" s="5"/>
     </row>
-    <row r="992" ht="15.75" customHeight="1">
+    <row r="992" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B992" s="5"/>
     </row>
-    <row r="993" ht="15.75" customHeight="1">
+    <row r="993" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B993" s="5"/>
     </row>
-    <row r="994" ht="15.75" customHeight="1">
+    <row r="994" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B994" s="5"/>
     </row>
-    <row r="995" ht="15.75" customHeight="1">
+    <row r="995" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B995" s="5"/>
     </row>
-    <row r="996" ht="15.75" customHeight="1">
+    <row r="996" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B996" s="5"/>
     </row>
-    <row r="997" ht="15.75" customHeight="1">
+    <row r="997" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B997" s="5"/>
     </row>
-    <row r="998" ht="15.75" customHeight="1">
+    <row r="998" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B998" s="5"/>
     </row>
-    <row r="999" ht="15.75" customHeight="1">
+    <row r="999" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B999" s="5"/>
     </row>
-    <row r="1000" ht="15.75" customHeight="1">
+    <row r="1000" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1000" s="5"/>
     </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IH-260 Update excel upload column headers
</commit_message>
<xml_diff>
--- a/src/main/resources/법인 회원 업로드.xlsx
+++ b/src/main/resources/법인 회원 업로드.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A33E91-5CFA-48AA-82A6-E2052996E08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A8A33E91-5CFA-48AA-82A6-E2052996E08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03391784-857C-4799-918B-B9E94EA43427}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,7 +41,7 @@
     <t>계정</t>
   </si>
   <si>
-    <t xml:space="preserve">핸드폰	</t>
+    <t>연락처(숫자만 표기)</t>
   </si>
   <si>
     <t>시작 날짜 (YYYY-MM-DD)</t>
@@ -44,7 +60,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -94,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -102,6 +118,9 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -323,23 +342,23 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H13:H14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="12.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="29.77734375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" style="6" customWidth="1"/>
+    <col min="1" max="2" width="12.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -356,3439 +375,3439 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="B2" s="3"/>
       <c r="D2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5"/>
       <c r="D3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="5"/>
       <c r="D4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5"/>
       <c r="D5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="B6" s="5"/>
       <c r="D6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="5"/>
       <c r="D7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5"/>
       <c r="D8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5"/>
       <c r="D9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="5"/>
       <c r="D10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5"/>
       <c r="D11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5"/>
       <c r="D12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5"/>
       <c r="D13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="B14" s="5"/>
       <c r="D14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5"/>
       <c r="D15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5"/>
       <c r="D16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="15.75" customHeight="1">
       <c r="B17" s="5"/>
       <c r="D17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="15.75" customHeight="1">
       <c r="B18" s="5"/>
       <c r="D18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="15.75" customHeight="1">
       <c r="B19" s="5"/>
       <c r="D19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="15.75" customHeight="1">
       <c r="B20" s="5"/>
       <c r="D20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="15.75" customHeight="1">
       <c r="B21" s="5"/>
       <c r="D21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="15.75" customHeight="1">
       <c r="B22" s="5"/>
       <c r="D22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="15.75" customHeight="1">
       <c r="B23" s="5"/>
       <c r="D23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="15.75" customHeight="1">
       <c r="B24" s="5"/>
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="15.75" customHeight="1">
       <c r="B25" s="5"/>
       <c r="D25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="15.75" customHeight="1">
       <c r="B26" s="5"/>
       <c r="D26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="15.75" customHeight="1">
       <c r="B27" s="5"/>
       <c r="D27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="15.75" customHeight="1">
       <c r="B28" s="5"/>
       <c r="D28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="15.75" customHeight="1">
       <c r="B29" s="5"/>
       <c r="D29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="15.75" customHeight="1">
       <c r="B30" s="5"/>
       <c r="D30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="15.75" customHeight="1">
       <c r="B31" s="5"/>
       <c r="D31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" ht="15.75" customHeight="1">
       <c r="B32" s="5"/>
       <c r="D32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" ht="15.75" customHeight="1">
       <c r="B33" s="5"/>
       <c r="D33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" ht="15.75" customHeight="1">
       <c r="B34" s="5"/>
       <c r="D34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" ht="15.75" customHeight="1">
       <c r="B35" s="5"/>
       <c r="D35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" ht="15.75" customHeight="1">
       <c r="B36" s="5"/>
       <c r="D36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" ht="15.75" customHeight="1">
       <c r="B37" s="5"/>
       <c r="D37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" ht="15.75" customHeight="1">
       <c r="B38" s="5"/>
       <c r="D38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" ht="15.75" customHeight="1">
       <c r="B39" s="5"/>
       <c r="D39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" ht="15.75" customHeight="1">
       <c r="B40" s="5"/>
       <c r="D40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" ht="15.75" customHeight="1">
       <c r="B41" s="5"/>
       <c r="D41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" ht="15.75" customHeight="1">
       <c r="B42" s="5"/>
       <c r="D42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" ht="15.75" customHeight="1">
       <c r="B43" s="5"/>
       <c r="D43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" ht="15.75" customHeight="1">
       <c r="B44" s="5"/>
       <c r="D44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6" ht="15.75" customHeight="1">
       <c r="B45" s="5"/>
       <c r="D45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6" ht="15.75" customHeight="1">
       <c r="B46" s="5"/>
       <c r="D46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" ht="15.75" customHeight="1">
       <c r="B47" s="5"/>
       <c r="D47" s="4"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" ht="15.75" customHeight="1">
       <c r="B48" s="5"/>
       <c r="D48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6" ht="15.75" customHeight="1">
       <c r="B49" s="5"/>
       <c r="D49" s="4"/>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:6" ht="15.75" customHeight="1">
       <c r="B50" s="5"/>
       <c r="D50" s="4"/>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:6" ht="15.75" customHeight="1">
       <c r="B51" s="5"/>
       <c r="D51" s="4"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6" ht="15.75" customHeight="1">
       <c r="B52" s="5"/>
       <c r="D52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:6" ht="15.75" customHeight="1">
       <c r="B53" s="5"/>
       <c r="D53" s="4"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6" ht="15.75" customHeight="1">
       <c r="B54" s="5"/>
       <c r="D54" s="4"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6" ht="15.75" customHeight="1">
       <c r="B55" s="5"/>
       <c r="D55" s="4"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6" ht="15.75" customHeight="1">
       <c r="B56" s="5"/>
       <c r="D56" s="4"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6" ht="15.75" customHeight="1">
       <c r="B57" s="5"/>
       <c r="D57" s="4"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:6" ht="15.75" customHeight="1">
       <c r="B58" s="5"/>
       <c r="D58" s="4"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:6" ht="15.75" customHeight="1">
       <c r="B59" s="5"/>
       <c r="D59" s="4"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:6" ht="15.75" customHeight="1">
       <c r="B60" s="5"/>
       <c r="D60" s="4"/>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:6" ht="15.75" customHeight="1">
       <c r="B61" s="5"/>
       <c r="D61" s="4"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:6" ht="15.75" customHeight="1">
       <c r="B62" s="5"/>
       <c r="D62" s="4"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:6" ht="15.75" customHeight="1">
       <c r="B63" s="5"/>
       <c r="D63" s="4"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:6" ht="15.75" customHeight="1">
       <c r="B64" s="5"/>
       <c r="D64" s="4"/>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:6" ht="15.75" customHeight="1">
       <c r="B65" s="5"/>
       <c r="D65" s="4"/>
       <c r="F65" s="4"/>
     </row>
-    <row r="66" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:6" ht="15.75" customHeight="1">
       <c r="B66" s="5"/>
       <c r="D66" s="4"/>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:6" ht="15.75" customHeight="1">
       <c r="B67" s="5"/>
       <c r="D67" s="4"/>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:6" ht="15.75" customHeight="1">
       <c r="B68" s="5"/>
       <c r="D68" s="4"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:6" ht="15.75" customHeight="1">
       <c r="B69" s="5"/>
       <c r="D69" s="4"/>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:6" ht="15.75" customHeight="1">
       <c r="B70" s="5"/>
       <c r="D70" s="4"/>
       <c r="F70" s="4"/>
     </row>
-    <row r="71" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:6" ht="15.75" customHeight="1">
       <c r="B71" s="5"/>
       <c r="D71" s="4"/>
       <c r="F71" s="4"/>
     </row>
-    <row r="72" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:6" ht="15.75" customHeight="1">
       <c r="B72" s="5"/>
       <c r="D72" s="4"/>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:6" ht="15.75" customHeight="1">
       <c r="B73" s="5"/>
       <c r="D73" s="4"/>
       <c r="F73" s="4"/>
     </row>
-    <row r="74" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:6" ht="15.75" customHeight="1">
       <c r="B74" s="5"/>
       <c r="D74" s="4"/>
       <c r="F74" s="4"/>
     </row>
-    <row r="75" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:6" ht="15.75" customHeight="1">
       <c r="B75" s="5"/>
       <c r="D75" s="4"/>
       <c r="F75" s="4"/>
     </row>
-    <row r="76" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:6" ht="15.75" customHeight="1">
       <c r="B76" s="5"/>
       <c r="D76" s="4"/>
       <c r="F76" s="4"/>
     </row>
-    <row r="77" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:6" ht="15.75" customHeight="1">
       <c r="B77" s="5"/>
       <c r="D77" s="4"/>
       <c r="F77" s="4"/>
     </row>
-    <row r="78" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:6" ht="15.75" customHeight="1">
       <c r="B78" s="5"/>
       <c r="D78" s="4"/>
       <c r="F78" s="4"/>
     </row>
-    <row r="79" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:6" ht="15.75" customHeight="1">
       <c r="B79" s="5"/>
       <c r="D79" s="4"/>
       <c r="F79" s="4"/>
     </row>
-    <row r="80" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:6" ht="15.75" customHeight="1">
       <c r="B80" s="5"/>
       <c r="D80" s="4"/>
       <c r="F80" s="4"/>
     </row>
-    <row r="81" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:6" ht="15.75" customHeight="1">
       <c r="B81" s="5"/>
       <c r="D81" s="4"/>
       <c r="F81" s="4"/>
     </row>
-    <row r="82" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:6" ht="15.75" customHeight="1">
       <c r="B82" s="5"/>
       <c r="D82" s="4"/>
       <c r="F82" s="4"/>
     </row>
-    <row r="83" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:6" ht="15.75" customHeight="1">
       <c r="B83" s="5"/>
       <c r="D83" s="4"/>
       <c r="F83" s="4"/>
     </row>
-    <row r="84" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:6" ht="15.75" customHeight="1">
       <c r="B84" s="5"/>
       <c r="D84" s="4"/>
       <c r="F84" s="4"/>
     </row>
-    <row r="85" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:6" ht="15.75" customHeight="1">
       <c r="B85" s="5"/>
       <c r="D85" s="4"/>
       <c r="F85" s="4"/>
     </row>
-    <row r="86" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:6" ht="15.75" customHeight="1">
       <c r="B86" s="5"/>
       <c r="D86" s="4"/>
       <c r="F86" s="4"/>
     </row>
-    <row r="87" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:6" ht="15.75" customHeight="1">
       <c r="B87" s="5"/>
       <c r="D87" s="4"/>
       <c r="F87" s="4"/>
     </row>
-    <row r="88" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:6" ht="15.75" customHeight="1">
       <c r="B88" s="5"/>
       <c r="D88" s="4"/>
       <c r="F88" s="4"/>
     </row>
-    <row r="89" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:6" ht="15.75" customHeight="1">
       <c r="B89" s="5"/>
       <c r="D89" s="4"/>
       <c r="F89" s="4"/>
     </row>
-    <row r="90" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:6" ht="15.75" customHeight="1">
       <c r="B90" s="5"/>
       <c r="D90" s="4"/>
       <c r="F90" s="4"/>
     </row>
-    <row r="91" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:6" ht="15.75" customHeight="1">
       <c r="B91" s="5"/>
       <c r="D91" s="4"/>
       <c r="F91" s="4"/>
     </row>
-    <row r="92" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:6" ht="15.75" customHeight="1">
       <c r="B92" s="5"/>
       <c r="D92" s="4"/>
       <c r="F92" s="4"/>
     </row>
-    <row r="93" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:6" ht="15.75" customHeight="1">
       <c r="B93" s="5"/>
       <c r="D93" s="4"/>
       <c r="F93" s="4"/>
     </row>
-    <row r="94" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:6" ht="15.75" customHeight="1">
       <c r="B94" s="5"/>
       <c r="D94" s="4"/>
       <c r="F94" s="4"/>
     </row>
-    <row r="95" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:6" ht="15.75" customHeight="1">
       <c r="B95" s="5"/>
       <c r="D95" s="4"/>
       <c r="F95" s="4"/>
     </row>
-    <row r="96" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:6" ht="15.75" customHeight="1">
       <c r="B96" s="5"/>
       <c r="D96" s="4"/>
       <c r="F96" s="4"/>
     </row>
-    <row r="97" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:6" ht="15.75" customHeight="1">
       <c r="B97" s="5"/>
       <c r="D97" s="4"/>
       <c r="F97" s="4"/>
     </row>
-    <row r="98" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:6" ht="15.75" customHeight="1">
       <c r="B98" s="5"/>
       <c r="D98" s="4"/>
       <c r="F98" s="4"/>
     </row>
-    <row r="99" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:6" ht="15.75" customHeight="1">
       <c r="B99" s="5"/>
       <c r="D99" s="4"/>
       <c r="F99" s="4"/>
     </row>
-    <row r="100" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:6" ht="15.75" customHeight="1">
       <c r="B100" s="5"/>
       <c r="D100" s="4"/>
       <c r="F100" s="4"/>
     </row>
-    <row r="101" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:6" ht="15.75" customHeight="1">
       <c r="B101" s="5"/>
       <c r="D101" s="4"/>
       <c r="F101" s="4"/>
     </row>
-    <row r="102" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:6" ht="15.75" customHeight="1">
       <c r="B102" s="5"/>
       <c r="D102" s="4"/>
       <c r="F102" s="4"/>
     </row>
-    <row r="103" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:6" ht="15.75" customHeight="1">
       <c r="B103" s="5"/>
       <c r="D103" s="4"/>
       <c r="F103" s="4"/>
     </row>
-    <row r="104" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:6" ht="15.75" customHeight="1">
       <c r="B104" s="5"/>
       <c r="D104" s="4"/>
       <c r="F104" s="4"/>
     </row>
-    <row r="105" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:6" ht="15.75" customHeight="1">
       <c r="B105" s="5"/>
       <c r="D105" s="4"/>
       <c r="F105" s="4"/>
     </row>
-    <row r="106" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:6" ht="15.75" customHeight="1">
       <c r="B106" s="5"/>
       <c r="D106" s="4"/>
       <c r="F106" s="4"/>
     </row>
-    <row r="107" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:6" ht="15.75" customHeight="1">
       <c r="B107" s="5"/>
       <c r="D107" s="4"/>
       <c r="F107" s="4"/>
     </row>
-    <row r="108" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:6" ht="15.75" customHeight="1">
       <c r="B108" s="5"/>
       <c r="D108" s="4"/>
       <c r="F108" s="4"/>
     </row>
-    <row r="109" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:6" ht="15.75" customHeight="1">
       <c r="B109" s="5"/>
       <c r="D109" s="4"/>
       <c r="F109" s="4"/>
     </row>
-    <row r="110" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:6" ht="15.75" customHeight="1">
       <c r="B110" s="5"/>
       <c r="D110" s="4"/>
       <c r="F110" s="4"/>
     </row>
-    <row r="111" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:6" ht="15.75" customHeight="1">
       <c r="B111" s="5"/>
       <c r="D111" s="4"/>
       <c r="F111" s="4"/>
     </row>
-    <row r="112" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:6" ht="15.75" customHeight="1">
       <c r="B112" s="5"/>
       <c r="D112" s="4"/>
       <c r="F112" s="4"/>
     </row>
-    <row r="113" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:6" ht="15.75" customHeight="1">
       <c r="B113" s="5"/>
       <c r="D113" s="4"/>
       <c r="F113" s="4"/>
     </row>
-    <row r="114" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:6" ht="15.75" customHeight="1">
       <c r="B114" s="5"/>
       <c r="D114" s="4"/>
       <c r="F114" s="4"/>
     </row>
-    <row r="115" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6" ht="15.75" customHeight="1">
       <c r="B115" s="5"/>
       <c r="D115" s="4"/>
       <c r="F115" s="4"/>
     </row>
-    <row r="116" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:6" ht="15.75" customHeight="1">
       <c r="B116" s="5"/>
       <c r="D116" s="4"/>
       <c r="F116" s="4"/>
     </row>
-    <row r="117" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:6" ht="15.75" customHeight="1">
       <c r="B117" s="5"/>
       <c r="D117" s="4"/>
       <c r="F117" s="4"/>
     </row>
-    <row r="118" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:6" ht="15.75" customHeight="1">
       <c r="B118" s="5"/>
       <c r="D118" s="4"/>
       <c r="F118" s="4"/>
     </row>
-    <row r="119" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:6" ht="15.75" customHeight="1">
       <c r="B119" s="5"/>
       <c r="D119" s="4"/>
       <c r="F119" s="4"/>
     </row>
-    <row r="120" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:6" ht="15.75" customHeight="1">
       <c r="B120" s="5"/>
       <c r="D120" s="4"/>
       <c r="F120" s="4"/>
     </row>
-    <row r="121" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:6" ht="15.75" customHeight="1">
       <c r="B121" s="5"/>
       <c r="D121" s="4"/>
       <c r="F121" s="4"/>
     </row>
-    <row r="122" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:6" ht="15.75" customHeight="1">
       <c r="B122" s="5"/>
       <c r="D122" s="4"/>
       <c r="F122" s="4"/>
     </row>
-    <row r="123" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:6" ht="15.75" customHeight="1">
       <c r="B123" s="5"/>
       <c r="D123" s="4"/>
       <c r="F123" s="4"/>
     </row>
-    <row r="124" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:6" ht="15.75" customHeight="1">
       <c r="B124" s="5"/>
       <c r="D124" s="4"/>
       <c r="F124" s="4"/>
     </row>
-    <row r="125" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:6" ht="15.75" customHeight="1">
       <c r="B125" s="5"/>
       <c r="D125" s="4"/>
       <c r="F125" s="4"/>
     </row>
-    <row r="126" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:6" ht="15.75" customHeight="1">
       <c r="B126" s="5"/>
       <c r="D126" s="4"/>
       <c r="F126" s="4"/>
     </row>
-    <row r="127" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:6" ht="15.75" customHeight="1">
       <c r="B127" s="5"/>
       <c r="D127" s="4"/>
       <c r="F127" s="4"/>
     </row>
-    <row r="128" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:6" ht="15.75" customHeight="1">
       <c r="B128" s="5"/>
       <c r="D128" s="4"/>
       <c r="F128" s="4"/>
     </row>
-    <row r="129" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:6" ht="15.75" customHeight="1">
       <c r="B129" s="5"/>
       <c r="D129" s="4"/>
       <c r="F129" s="4"/>
     </row>
-    <row r="130" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:6" ht="15.75" customHeight="1">
       <c r="B130" s="5"/>
       <c r="D130" s="4"/>
       <c r="F130" s="4"/>
     </row>
-    <row r="131" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:6" ht="15.75" customHeight="1">
       <c r="B131" s="5"/>
       <c r="D131" s="4"/>
       <c r="F131" s="4"/>
     </row>
-    <row r="132" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:6" ht="15.75" customHeight="1">
       <c r="B132" s="5"/>
       <c r="D132" s="4"/>
       <c r="F132" s="4"/>
     </row>
-    <row r="133" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:6" ht="15.75" customHeight="1">
       <c r="B133" s="5"/>
       <c r="D133" s="4"/>
       <c r="F133" s="4"/>
     </row>
-    <row r="134" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:6" ht="15.75" customHeight="1">
       <c r="B134" s="5"/>
       <c r="D134" s="4"/>
       <c r="F134" s="4"/>
     </row>
-    <row r="135" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:6" ht="15.75" customHeight="1">
       <c r="B135" s="5"/>
       <c r="D135" s="4"/>
       <c r="F135" s="4"/>
     </row>
-    <row r="136" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:6" ht="15.75" customHeight="1">
       <c r="B136" s="5"/>
       <c r="D136" s="4"/>
       <c r="F136" s="4"/>
     </row>
-    <row r="137" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:6" ht="15.75" customHeight="1">
       <c r="B137" s="5"/>
       <c r="D137" s="4"/>
       <c r="F137" s="4"/>
     </row>
-    <row r="138" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:6" ht="15.75" customHeight="1">
       <c r="B138" s="5"/>
       <c r="D138" s="4"/>
       <c r="F138" s="4"/>
     </row>
-    <row r="139" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:6" ht="15.75" customHeight="1">
       <c r="B139" s="5"/>
       <c r="D139" s="4"/>
       <c r="F139" s="4"/>
     </row>
-    <row r="140" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:6" ht="15.75" customHeight="1">
       <c r="B140" s="5"/>
       <c r="D140" s="4"/>
       <c r="F140" s="4"/>
     </row>
-    <row r="141" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:6" ht="15.75" customHeight="1">
       <c r="B141" s="5"/>
       <c r="D141" s="4"/>
       <c r="F141" s="4"/>
     </row>
-    <row r="142" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:6" ht="15.75" customHeight="1">
       <c r="B142" s="5"/>
       <c r="D142" s="4"/>
       <c r="F142" s="4"/>
     </row>
-    <row r="143" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:6" ht="15.75" customHeight="1">
       <c r="B143" s="5"/>
       <c r="D143" s="4"/>
       <c r="F143" s="4"/>
     </row>
-    <row r="144" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:6" ht="15.75" customHeight="1">
       <c r="B144" s="5"/>
       <c r="D144" s="4"/>
       <c r="F144" s="4"/>
     </row>
-    <row r="145" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:6" ht="15.75" customHeight="1">
       <c r="B145" s="5"/>
       <c r="D145" s="4"/>
       <c r="F145" s="4"/>
     </row>
-    <row r="146" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:6" ht="15.75" customHeight="1">
       <c r="B146" s="5"/>
       <c r="D146" s="4"/>
       <c r="F146" s="4"/>
     </row>
-    <row r="147" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:6" ht="15.75" customHeight="1">
       <c r="B147" s="5"/>
       <c r="D147" s="4"/>
       <c r="F147" s="4"/>
     </row>
-    <row r="148" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:6" ht="15.75" customHeight="1">
       <c r="B148" s="5"/>
       <c r="D148" s="4"/>
       <c r="F148" s="4"/>
     </row>
-    <row r="149" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:6" ht="15.75" customHeight="1">
       <c r="B149" s="5"/>
       <c r="D149" s="4"/>
       <c r="F149" s="4"/>
     </row>
-    <row r="150" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:6" ht="15.75" customHeight="1">
       <c r="B150" s="5"/>
       <c r="D150" s="4"/>
       <c r="F150" s="4"/>
     </row>
-    <row r="151" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:6" ht="15.75" customHeight="1">
       <c r="B151" s="5"/>
       <c r="D151" s="4"/>
       <c r="F151" s="4"/>
     </row>
-    <row r="152" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:6" ht="15.75" customHeight="1">
       <c r="B152" s="5"/>
       <c r="D152" s="4"/>
       <c r="F152" s="4"/>
     </row>
-    <row r="153" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:6" ht="15.75" customHeight="1">
       <c r="B153" s="5"/>
       <c r="D153" s="4"/>
       <c r="F153" s="4"/>
     </row>
-    <row r="154" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:6" ht="15.75" customHeight="1">
       <c r="B154" s="5"/>
       <c r="D154" s="4"/>
       <c r="F154" s="4"/>
     </row>
-    <row r="155" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:6" ht="15.75" customHeight="1">
       <c r="B155" s="5"/>
       <c r="D155" s="4"/>
       <c r="F155" s="4"/>
     </row>
-    <row r="156" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:6" ht="15.75" customHeight="1">
       <c r="B156" s="5"/>
       <c r="D156" s="4"/>
       <c r="F156" s="4"/>
     </row>
-    <row r="157" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:6" ht="15.75" customHeight="1">
       <c r="B157" s="5"/>
       <c r="D157" s="4"/>
       <c r="F157" s="4"/>
     </row>
-    <row r="158" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:6" ht="15.75" customHeight="1">
       <c r="B158" s="5"/>
       <c r="D158" s="4"/>
       <c r="F158" s="4"/>
     </row>
-    <row r="159" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:6" ht="15.75" customHeight="1">
       <c r="B159" s="5"/>
       <c r="D159" s="4"/>
       <c r="F159" s="4"/>
     </row>
-    <row r="160" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:6" ht="15.75" customHeight="1">
       <c r="B160" s="5"/>
       <c r="D160" s="4"/>
       <c r="F160" s="4"/>
     </row>
-    <row r="161" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:6" ht="15.75" customHeight="1">
       <c r="B161" s="5"/>
       <c r="D161" s="4"/>
       <c r="F161" s="4"/>
     </row>
-    <row r="162" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:6" ht="15.75" customHeight="1">
       <c r="B162" s="5"/>
       <c r="D162" s="4"/>
       <c r="F162" s="4"/>
     </row>
-    <row r="163" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:6" ht="15.75" customHeight="1">
       <c r="B163" s="5"/>
       <c r="D163" s="4"/>
       <c r="F163" s="4"/>
     </row>
-    <row r="164" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:6" ht="15.75" customHeight="1">
       <c r="B164" s="5"/>
       <c r="D164" s="4"/>
       <c r="F164" s="4"/>
     </row>
-    <row r="165" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:6" ht="15.75" customHeight="1">
       <c r="B165" s="5"/>
       <c r="D165" s="4"/>
       <c r="F165" s="4"/>
     </row>
-    <row r="166" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:6" ht="15.75" customHeight="1">
       <c r="B166" s="5"/>
       <c r="D166" s="4"/>
       <c r="F166" s="4"/>
     </row>
-    <row r="167" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:6" ht="15.75" customHeight="1">
       <c r="B167" s="5"/>
       <c r="D167" s="4"/>
       <c r="F167" s="4"/>
     </row>
-    <row r="168" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:6" ht="15.75" customHeight="1">
       <c r="B168" s="5"/>
       <c r="D168" s="4"/>
       <c r="F168" s="4"/>
     </row>
-    <row r="169" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:6" ht="15.75" customHeight="1">
       <c r="B169" s="5"/>
       <c r="D169" s="4"/>
       <c r="F169" s="4"/>
     </row>
-    <row r="170" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:6" ht="15.75" customHeight="1">
       <c r="B170" s="5"/>
       <c r="D170" s="4"/>
       <c r="F170" s="4"/>
     </row>
-    <row r="171" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:6" ht="15.75" customHeight="1">
       <c r="B171" s="5"/>
       <c r="D171" s="4"/>
       <c r="F171" s="4"/>
     </row>
-    <row r="172" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:6" ht="15.75" customHeight="1">
       <c r="B172" s="5"/>
       <c r="D172" s="4"/>
       <c r="F172" s="4"/>
     </row>
-    <row r="173" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:6" ht="15.75" customHeight="1">
       <c r="B173" s="5"/>
       <c r="D173" s="4"/>
       <c r="F173" s="4"/>
     </row>
-    <row r="174" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:6" ht="15.75" customHeight="1">
       <c r="B174" s="5"/>
       <c r="D174" s="4"/>
       <c r="F174" s="4"/>
     </row>
-    <row r="175" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:6" ht="15.75" customHeight="1">
       <c r="B175" s="5"/>
       <c r="D175" s="4"/>
       <c r="F175" s="4"/>
     </row>
-    <row r="176" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:6" ht="15.75" customHeight="1">
       <c r="B176" s="5"/>
       <c r="D176" s="4"/>
       <c r="F176" s="4"/>
     </row>
-    <row r="177" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:6" ht="15.75" customHeight="1">
       <c r="B177" s="5"/>
       <c r="D177" s="4"/>
       <c r="F177" s="4"/>
     </row>
-    <row r="178" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:6" ht="15.75" customHeight="1">
       <c r="B178" s="5"/>
       <c r="D178" s="4"/>
       <c r="F178" s="4"/>
     </row>
-    <row r="179" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:6" ht="15.75" customHeight="1">
       <c r="B179" s="5"/>
       <c r="D179" s="4"/>
       <c r="F179" s="4"/>
     </row>
-    <row r="180" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:6" ht="15.75" customHeight="1">
       <c r="B180" s="5"/>
       <c r="D180" s="4"/>
       <c r="F180" s="4"/>
     </row>
-    <row r="181" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:6" ht="15.75" customHeight="1">
       <c r="B181" s="5"/>
       <c r="D181" s="4"/>
       <c r="F181" s="4"/>
     </row>
-    <row r="182" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:6" ht="15.75" customHeight="1">
       <c r="B182" s="5"/>
       <c r="D182" s="4"/>
       <c r="F182" s="4"/>
     </row>
-    <row r="183" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:6" ht="15.75" customHeight="1">
       <c r="B183" s="5"/>
       <c r="D183" s="4"/>
       <c r="F183" s="4"/>
     </row>
-    <row r="184" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:6" ht="15.75" customHeight="1">
       <c r="B184" s="5"/>
       <c r="D184" s="4"/>
       <c r="F184" s="4"/>
     </row>
-    <row r="185" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:6" ht="15.75" customHeight="1">
       <c r="B185" s="5"/>
       <c r="D185" s="4"/>
       <c r="F185" s="4"/>
     </row>
-    <row r="186" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:6" ht="15.75" customHeight="1">
       <c r="B186" s="5"/>
       <c r="D186" s="4"/>
       <c r="F186" s="4"/>
     </row>
-    <row r="187" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:6" ht="15.75" customHeight="1">
       <c r="B187" s="5"/>
       <c r="D187" s="4"/>
       <c r="F187" s="4"/>
     </row>
-    <row r="188" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:6" ht="15.75" customHeight="1">
       <c r="B188" s="5"/>
       <c r="D188" s="4"/>
       <c r="F188" s="4"/>
     </row>
-    <row r="189" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:6" ht="15.75" customHeight="1">
       <c r="B189" s="5"/>
       <c r="D189" s="4"/>
       <c r="F189" s="4"/>
     </row>
-    <row r="190" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:6" ht="15.75" customHeight="1">
       <c r="B190" s="5"/>
       <c r="D190" s="4"/>
       <c r="F190" s="4"/>
     </row>
-    <row r="191" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:6" ht="15.75" customHeight="1">
       <c r="B191" s="5"/>
       <c r="D191" s="4"/>
       <c r="F191" s="4"/>
     </row>
-    <row r="192" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:6" ht="15.75" customHeight="1">
       <c r="B192" s="5"/>
       <c r="D192" s="4"/>
       <c r="F192" s="4"/>
     </row>
-    <row r="193" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:6" ht="15.75" customHeight="1">
       <c r="B193" s="5"/>
       <c r="D193" s="4"/>
       <c r="F193" s="4"/>
     </row>
-    <row r="194" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:6" ht="15.75" customHeight="1">
       <c r="B194" s="5"/>
       <c r="D194" s="4"/>
       <c r="F194" s="4"/>
     </row>
-    <row r="195" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:6" ht="15.75" customHeight="1">
       <c r="B195" s="5"/>
       <c r="D195" s="4"/>
       <c r="F195" s="4"/>
     </row>
-    <row r="196" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:6" ht="15.75" customHeight="1">
       <c r="B196" s="5"/>
       <c r="D196" s="4"/>
       <c r="F196" s="4"/>
     </row>
-    <row r="197" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:6" ht="15.75" customHeight="1">
       <c r="B197" s="5"/>
       <c r="D197" s="4"/>
       <c r="F197" s="4"/>
     </row>
-    <row r="198" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:6" ht="15.75" customHeight="1">
       <c r="B198" s="5"/>
       <c r="D198" s="4"/>
       <c r="F198" s="4"/>
     </row>
-    <row r="199" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:6" ht="15.75" customHeight="1">
       <c r="B199" s="5"/>
       <c r="D199" s="4"/>
       <c r="F199" s="4"/>
     </row>
-    <row r="200" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:6" ht="15.75" customHeight="1">
       <c r="B200" s="5"/>
       <c r="D200" s="4"/>
       <c r="F200" s="4"/>
     </row>
-    <row r="201" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:6" ht="15.75" customHeight="1">
       <c r="B201" s="5"/>
       <c r="D201" s="4"/>
       <c r="F201" s="4"/>
     </row>
-    <row r="202" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:6" ht="15.75" customHeight="1">
       <c r="B202" s="5"/>
       <c r="D202" s="4"/>
       <c r="F202" s="4"/>
     </row>
-    <row r="203" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:6" ht="15.75" customHeight="1">
       <c r="B203" s="5"/>
       <c r="D203" s="4"/>
       <c r="F203" s="4"/>
     </row>
-    <row r="204" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:6" ht="15.75" customHeight="1">
       <c r="B204" s="5"/>
       <c r="D204" s="4"/>
       <c r="F204" s="4"/>
     </row>
-    <row r="205" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:6" ht="15.75" customHeight="1">
       <c r="B205" s="5"/>
       <c r="D205" s="4"/>
       <c r="F205" s="4"/>
     </row>
-    <row r="206" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:6" ht="15.75" customHeight="1">
       <c r="B206" s="5"/>
       <c r="D206" s="4"/>
       <c r="F206" s="4"/>
     </row>
-    <row r="207" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:6" ht="15.75" customHeight="1">
       <c r="B207" s="5"/>
       <c r="D207" s="4"/>
       <c r="F207" s="4"/>
     </row>
-    <row r="208" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:6" ht="15.75" customHeight="1">
       <c r="B208" s="5"/>
       <c r="D208" s="4"/>
       <c r="F208" s="4"/>
     </row>
-    <row r="209" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:6" ht="15.75" customHeight="1">
       <c r="B209" s="5"/>
       <c r="D209" s="4"/>
       <c r="F209" s="4"/>
     </row>
-    <row r="210" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:6" ht="15.75" customHeight="1">
       <c r="B210" s="5"/>
       <c r="D210" s="4"/>
       <c r="F210" s="4"/>
     </row>
-    <row r="211" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:6" ht="15.75" customHeight="1">
       <c r="B211" s="5"/>
       <c r="D211" s="4"/>
       <c r="F211" s="4"/>
     </row>
-    <row r="212" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:6" ht="15.75" customHeight="1">
       <c r="B212" s="5"/>
       <c r="D212" s="4"/>
       <c r="F212" s="4"/>
     </row>
-    <row r="213" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:6" ht="15.75" customHeight="1">
       <c r="B213" s="5"/>
       <c r="D213" s="4"/>
       <c r="F213" s="4"/>
     </row>
-    <row r="214" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:6" ht="15.75" customHeight="1">
       <c r="B214" s="5"/>
       <c r="D214" s="4"/>
       <c r="F214" s="4"/>
     </row>
-    <row r="215" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:6" ht="15.75" customHeight="1">
       <c r="B215" s="5"/>
       <c r="D215" s="4"/>
       <c r="F215" s="4"/>
     </row>
-    <row r="216" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:6" ht="15.75" customHeight="1">
       <c r="B216" s="5"/>
       <c r="D216" s="4"/>
       <c r="F216" s="4"/>
     </row>
-    <row r="217" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:6" ht="15.75" customHeight="1">
       <c r="B217" s="5"/>
       <c r="D217" s="4"/>
       <c r="F217" s="4"/>
     </row>
-    <row r="218" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:6" ht="15.75" customHeight="1">
       <c r="B218" s="5"/>
       <c r="D218" s="4"/>
       <c r="F218" s="4"/>
     </row>
-    <row r="219" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:6" ht="15.75" customHeight="1">
       <c r="B219" s="5"/>
       <c r="D219" s="4"/>
       <c r="F219" s="4"/>
     </row>
-    <row r="220" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:6" ht="15.75" customHeight="1">
       <c r="B220" s="5"/>
       <c r="D220" s="4"/>
       <c r="F220" s="4"/>
     </row>
-    <row r="221" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:6" ht="15.75" customHeight="1">
       <c r="B221" s="5"/>
     </row>
-    <row r="222" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:6" ht="15.75" customHeight="1">
       <c r="B222" s="5"/>
     </row>
-    <row r="223" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:6" ht="15.75" customHeight="1">
       <c r="B223" s="5"/>
     </row>
-    <row r="224" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:6" ht="15.75" customHeight="1">
       <c r="B224" s="5"/>
     </row>
-    <row r="225" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:2" ht="15.75" customHeight="1">
       <c r="B225" s="5"/>
     </row>
-    <row r="226" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:2" ht="15.75" customHeight="1">
       <c r="B226" s="5"/>
     </row>
-    <row r="227" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:2" ht="15.75" customHeight="1">
       <c r="B227" s="5"/>
     </row>
-    <row r="228" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:2" ht="15.75" customHeight="1">
       <c r="B228" s="5"/>
     </row>
-    <row r="229" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:2" ht="15.75" customHeight="1">
       <c r="B229" s="5"/>
     </row>
-    <row r="230" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:2" ht="15.75" customHeight="1">
       <c r="B230" s="5"/>
     </row>
-    <row r="231" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:2" ht="15.75" customHeight="1">
       <c r="B231" s="5"/>
     </row>
-    <row r="232" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:2" ht="15.75" customHeight="1">
       <c r="B232" s="5"/>
     </row>
-    <row r="233" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:2" ht="15.75" customHeight="1">
       <c r="B233" s="5"/>
     </row>
-    <row r="234" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:2" ht="15.75" customHeight="1">
       <c r="B234" s="5"/>
     </row>
-    <row r="235" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:2" ht="15.75" customHeight="1">
       <c r="B235" s="5"/>
     </row>
-    <row r="236" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:2" ht="15.75" customHeight="1">
       <c r="B236" s="5"/>
     </row>
-    <row r="237" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:2" ht="15.75" customHeight="1">
       <c r="B237" s="5"/>
     </row>
-    <row r="238" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:2" ht="15.75" customHeight="1">
       <c r="B238" s="5"/>
     </row>
-    <row r="239" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:2" ht="15.75" customHeight="1">
       <c r="B239" s="5"/>
     </row>
-    <row r="240" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:2" ht="15.75" customHeight="1">
       <c r="B240" s="5"/>
     </row>
-    <row r="241" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:2" ht="15.75" customHeight="1">
       <c r="B241" s="5"/>
     </row>
-    <row r="242" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:2" ht="15.75" customHeight="1">
       <c r="B242" s="5"/>
     </row>
-    <row r="243" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:2" ht="15.75" customHeight="1">
       <c r="B243" s="5"/>
     </row>
-    <row r="244" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:2" ht="15.75" customHeight="1">
       <c r="B244" s="5"/>
     </row>
-    <row r="245" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:2" ht="15.75" customHeight="1">
       <c r="B245" s="5"/>
     </row>
-    <row r="246" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:2" ht="15.75" customHeight="1">
       <c r="B246" s="5"/>
     </row>
-    <row r="247" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:2" ht="15.75" customHeight="1">
       <c r="B247" s="5"/>
     </row>
-    <row r="248" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:2" ht="15.75" customHeight="1">
       <c r="B248" s="5"/>
     </row>
-    <row r="249" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:2" ht="15.75" customHeight="1">
       <c r="B249" s="5"/>
     </row>
-    <row r="250" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:2" ht="15.75" customHeight="1">
       <c r="B250" s="5"/>
     </row>
-    <row r="251" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:2" ht="15.75" customHeight="1">
       <c r="B251" s="5"/>
     </row>
-    <row r="252" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:2" ht="15.75" customHeight="1">
       <c r="B252" s="5"/>
     </row>
-    <row r="253" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:2" ht="15.75" customHeight="1">
       <c r="B253" s="5"/>
     </row>
-    <row r="254" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:2" ht="15.75" customHeight="1">
       <c r="B254" s="5"/>
     </row>
-    <row r="255" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:2" ht="15.75" customHeight="1">
       <c r="B255" s="5"/>
     </row>
-    <row r="256" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:2" ht="15.75" customHeight="1">
       <c r="B256" s="5"/>
     </row>
-    <row r="257" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:2" ht="15.75" customHeight="1">
       <c r="B257" s="5"/>
     </row>
-    <row r="258" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:2" ht="15.75" customHeight="1">
       <c r="B258" s="5"/>
     </row>
-    <row r="259" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:2" ht="15.75" customHeight="1">
       <c r="B259" s="5"/>
     </row>
-    <row r="260" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:2" ht="15.75" customHeight="1">
       <c r="B260" s="5"/>
     </row>
-    <row r="261" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:2" ht="15.75" customHeight="1">
       <c r="B261" s="5"/>
     </row>
-    <row r="262" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:2" ht="15.75" customHeight="1">
       <c r="B262" s="5"/>
     </row>
-    <row r="263" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:2" ht="15.75" customHeight="1">
       <c r="B263" s="5"/>
     </row>
-    <row r="264" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:2" ht="15.75" customHeight="1">
       <c r="B264" s="5"/>
     </row>
-    <row r="265" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:2" ht="15.75" customHeight="1">
       <c r="B265" s="5"/>
     </row>
-    <row r="266" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:2" ht="15.75" customHeight="1">
       <c r="B266" s="5"/>
     </row>
-    <row r="267" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:2" ht="15.75" customHeight="1">
       <c r="B267" s="5"/>
     </row>
-    <row r="268" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:2" ht="15.75" customHeight="1">
       <c r="B268" s="5"/>
     </row>
-    <row r="269" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:2" ht="15.75" customHeight="1">
       <c r="B269" s="5"/>
     </row>
-    <row r="270" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:2" ht="15.75" customHeight="1">
       <c r="B270" s="5"/>
     </row>
-    <row r="271" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:2" ht="15.75" customHeight="1">
       <c r="B271" s="5"/>
     </row>
-    <row r="272" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:2" ht="15.75" customHeight="1">
       <c r="B272" s="5"/>
     </row>
-    <row r="273" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:2" ht="15.75" customHeight="1">
       <c r="B273" s="5"/>
     </row>
-    <row r="274" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:2" ht="15.75" customHeight="1">
       <c r="B274" s="5"/>
     </row>
-    <row r="275" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:2" ht="15.75" customHeight="1">
       <c r="B275" s="5"/>
     </row>
-    <row r="276" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:2" ht="15.75" customHeight="1">
       <c r="B276" s="5"/>
     </row>
-    <row r="277" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:2" ht="15.75" customHeight="1">
       <c r="B277" s="5"/>
     </row>
-    <row r="278" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:2" ht="15.75" customHeight="1">
       <c r="B278" s="5"/>
     </row>
-    <row r="279" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:2" ht="15.75" customHeight="1">
       <c r="B279" s="5"/>
     </row>
-    <row r="280" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:2" ht="15.75" customHeight="1">
       <c r="B280" s="5"/>
     </row>
-    <row r="281" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:2" ht="15.75" customHeight="1">
       <c r="B281" s="5"/>
     </row>
-    <row r="282" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:2" ht="15.75" customHeight="1">
       <c r="B282" s="5"/>
     </row>
-    <row r="283" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:2" ht="15.75" customHeight="1">
       <c r="B283" s="5"/>
     </row>
-    <row r="284" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:2" ht="15.75" customHeight="1">
       <c r="B284" s="5"/>
     </row>
-    <row r="285" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:2" ht="15.75" customHeight="1">
       <c r="B285" s="5"/>
     </row>
-    <row r="286" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:2" ht="15.75" customHeight="1">
       <c r="B286" s="5"/>
     </row>
-    <row r="287" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:2" ht="15.75" customHeight="1">
       <c r="B287" s="5"/>
     </row>
-    <row r="288" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:2" ht="15.75" customHeight="1">
       <c r="B288" s="5"/>
     </row>
-    <row r="289" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:2" ht="15.75" customHeight="1">
       <c r="B289" s="5"/>
     </row>
-    <row r="290" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:2" ht="15.75" customHeight="1">
       <c r="B290" s="5"/>
     </row>
-    <row r="291" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:2" ht="15.75" customHeight="1">
       <c r="B291" s="5"/>
     </row>
-    <row r="292" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:2" ht="15.75" customHeight="1">
       <c r="B292" s="5"/>
     </row>
-    <row r="293" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:2" ht="15.75" customHeight="1">
       <c r="B293" s="5"/>
     </row>
-    <row r="294" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:2" ht="15.75" customHeight="1">
       <c r="B294" s="5"/>
     </row>
-    <row r="295" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:2" ht="15.75" customHeight="1">
       <c r="B295" s="5"/>
     </row>
-    <row r="296" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:2" ht="15.75" customHeight="1">
       <c r="B296" s="5"/>
     </row>
-    <row r="297" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:2" ht="15.75" customHeight="1">
       <c r="B297" s="5"/>
     </row>
-    <row r="298" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:2" ht="15.75" customHeight="1">
       <c r="B298" s="5"/>
     </row>
-    <row r="299" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:2" ht="15.75" customHeight="1">
       <c r="B299" s="5"/>
     </row>
-    <row r="300" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:2" ht="15.75" customHeight="1">
       <c r="B300" s="5"/>
     </row>
-    <row r="301" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:2" ht="15.75" customHeight="1">
       <c r="B301" s="5"/>
     </row>
-    <row r="302" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:2" ht="15.75" customHeight="1">
       <c r="B302" s="5"/>
     </row>
-    <row r="303" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:2" ht="15.75" customHeight="1">
       <c r="B303" s="5"/>
     </row>
-    <row r="304" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:2" ht="15.75" customHeight="1">
       <c r="B304" s="5"/>
     </row>
-    <row r="305" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:2" ht="15.75" customHeight="1">
       <c r="B305" s="5"/>
     </row>
-    <row r="306" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:2" ht="15.75" customHeight="1">
       <c r="B306" s="5"/>
     </row>
-    <row r="307" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:2" ht="15.75" customHeight="1">
       <c r="B307" s="5"/>
     </row>
-    <row r="308" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:2" ht="15.75" customHeight="1">
       <c r="B308" s="5"/>
     </row>
-    <row r="309" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:2" ht="15.75" customHeight="1">
       <c r="B309" s="5"/>
     </row>
-    <row r="310" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:2" ht="15.75" customHeight="1">
       <c r="B310" s="5"/>
     </row>
-    <row r="311" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:2" ht="15.75" customHeight="1">
       <c r="B311" s="5"/>
     </row>
-    <row r="312" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:2" ht="15.75" customHeight="1">
       <c r="B312" s="5"/>
     </row>
-    <row r="313" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:2" ht="15.75" customHeight="1">
       <c r="B313" s="5"/>
     </row>
-    <row r="314" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:2" ht="15.75" customHeight="1">
       <c r="B314" s="5"/>
     </row>
-    <row r="315" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:2" ht="15.75" customHeight="1">
       <c r="B315" s="5"/>
     </row>
-    <row r="316" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="2:2" ht="15.75" customHeight="1">
       <c r="B316" s="5"/>
     </row>
-    <row r="317" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="2:2" ht="15.75" customHeight="1">
       <c r="B317" s="5"/>
     </row>
-    <row r="318" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="2:2" ht="15.75" customHeight="1">
       <c r="B318" s="5"/>
     </row>
-    <row r="319" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="2:2" ht="15.75" customHeight="1">
       <c r="B319" s="5"/>
     </row>
-    <row r="320" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="2:2" ht="15.75" customHeight="1">
       <c r="B320" s="5"/>
     </row>
-    <row r="321" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:2" ht="15.75" customHeight="1">
       <c r="B321" s="5"/>
     </row>
-    <row r="322" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:2" ht="15.75" customHeight="1">
       <c r="B322" s="5"/>
     </row>
-    <row r="323" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:2" ht="15.75" customHeight="1">
       <c r="B323" s="5"/>
     </row>
-    <row r="324" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:2" ht="15.75" customHeight="1">
       <c r="B324" s="5"/>
     </row>
-    <row r="325" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:2" ht="15.75" customHeight="1">
       <c r="B325" s="5"/>
     </row>
-    <row r="326" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:2" ht="15.75" customHeight="1">
       <c r="B326" s="5"/>
     </row>
-    <row r="327" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:2" ht="15.75" customHeight="1">
       <c r="B327" s="5"/>
     </row>
-    <row r="328" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="2:2" ht="15.75" customHeight="1">
       <c r="B328" s="5"/>
     </row>
-    <row r="329" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="2:2" ht="15.75" customHeight="1">
       <c r="B329" s="5"/>
     </row>
-    <row r="330" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="2:2" ht="15.75" customHeight="1">
       <c r="B330" s="5"/>
     </row>
-    <row r="331" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="2:2" ht="15.75" customHeight="1">
       <c r="B331" s="5"/>
     </row>
-    <row r="332" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="2:2" ht="15.75" customHeight="1">
       <c r="B332" s="5"/>
     </row>
-    <row r="333" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="2:2" ht="15.75" customHeight="1">
       <c r="B333" s="5"/>
     </row>
-    <row r="334" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:2" ht="15.75" customHeight="1">
       <c r="B334" s="5"/>
     </row>
-    <row r="335" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="2:2" ht="15.75" customHeight="1">
       <c r="B335" s="5"/>
     </row>
-    <row r="336" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="2:2" ht="15.75" customHeight="1">
       <c r="B336" s="5"/>
     </row>
-    <row r="337" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="2:2" ht="15.75" customHeight="1">
       <c r="B337" s="5"/>
     </row>
-    <row r="338" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="2:2" ht="15.75" customHeight="1">
       <c r="B338" s="5"/>
     </row>
-    <row r="339" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="2:2" ht="15.75" customHeight="1">
       <c r="B339" s="5"/>
     </row>
-    <row r="340" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="2:2" ht="15.75" customHeight="1">
       <c r="B340" s="5"/>
     </row>
-    <row r="341" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="2:2" ht="15.75" customHeight="1">
       <c r="B341" s="5"/>
     </row>
-    <row r="342" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="2:2" ht="15.75" customHeight="1">
       <c r="B342" s="5"/>
     </row>
-    <row r="343" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="2:2" ht="15.75" customHeight="1">
       <c r="B343" s="5"/>
     </row>
-    <row r="344" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="2:2" ht="15.75" customHeight="1">
       <c r="B344" s="5"/>
     </row>
-    <row r="345" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="2:2" ht="15.75" customHeight="1">
       <c r="B345" s="5"/>
     </row>
-    <row r="346" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="2:2" ht="15.75" customHeight="1">
       <c r="B346" s="5"/>
     </row>
-    <row r="347" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="2:2" ht="15.75" customHeight="1">
       <c r="B347" s="5"/>
     </row>
-    <row r="348" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="2:2" ht="15.75" customHeight="1">
       <c r="B348" s="5"/>
     </row>
-    <row r="349" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="2:2" ht="15.75" customHeight="1">
       <c r="B349" s="5"/>
     </row>
-    <row r="350" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="2:2" ht="15.75" customHeight="1">
       <c r="B350" s="5"/>
     </row>
-    <row r="351" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="2:2" ht="15.75" customHeight="1">
       <c r="B351" s="5"/>
     </row>
-    <row r="352" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="2:2" ht="15.75" customHeight="1">
       <c r="B352" s="5"/>
     </row>
-    <row r="353" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="2:2" ht="15.75" customHeight="1">
       <c r="B353" s="5"/>
     </row>
-    <row r="354" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="2:2" ht="15.75" customHeight="1">
       <c r="B354" s="5"/>
     </row>
-    <row r="355" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="2:2" ht="15.75" customHeight="1">
       <c r="B355" s="5"/>
     </row>
-    <row r="356" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="2:2" ht="15.75" customHeight="1">
       <c r="B356" s="5"/>
     </row>
-    <row r="357" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="2:2" ht="15.75" customHeight="1">
       <c r="B357" s="5"/>
     </row>
-    <row r="358" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="2:2" ht="15.75" customHeight="1">
       <c r="B358" s="5"/>
     </row>
-    <row r="359" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="2:2" ht="15.75" customHeight="1">
       <c r="B359" s="5"/>
     </row>
-    <row r="360" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="2:2" ht="15.75" customHeight="1">
       <c r="B360" s="5"/>
     </row>
-    <row r="361" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="2:2" ht="15.75" customHeight="1">
       <c r="B361" s="5"/>
     </row>
-    <row r="362" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="2:2" ht="15.75" customHeight="1">
       <c r="B362" s="5"/>
     </row>
-    <row r="363" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="2:2" ht="15.75" customHeight="1">
       <c r="B363" s="5"/>
     </row>
-    <row r="364" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="2:2" ht="15.75" customHeight="1">
       <c r="B364" s="5"/>
     </row>
-    <row r="365" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="2:2" ht="15.75" customHeight="1">
       <c r="B365" s="5"/>
     </row>
-    <row r="366" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="2:2" ht="15.75" customHeight="1">
       <c r="B366" s="5"/>
     </row>
-    <row r="367" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="2:2" ht="15.75" customHeight="1">
       <c r="B367" s="5"/>
     </row>
-    <row r="368" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="2:2" ht="15.75" customHeight="1">
       <c r="B368" s="5"/>
     </row>
-    <row r="369" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="2:2" ht="15.75" customHeight="1">
       <c r="B369" s="5"/>
     </row>
-    <row r="370" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="2:2" ht="15.75" customHeight="1">
       <c r="B370" s="5"/>
     </row>
-    <row r="371" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="2:2" ht="15.75" customHeight="1">
       <c r="B371" s="5"/>
     </row>
-    <row r="372" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="2:2" ht="15.75" customHeight="1">
       <c r="B372" s="5"/>
     </row>
-    <row r="373" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="2:2" ht="15.75" customHeight="1">
       <c r="B373" s="5"/>
     </row>
-    <row r="374" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="2:2" ht="15.75" customHeight="1">
       <c r="B374" s="5"/>
     </row>
-    <row r="375" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="2:2" ht="15.75" customHeight="1">
       <c r="B375" s="5"/>
     </row>
-    <row r="376" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="2:2" ht="15.75" customHeight="1">
       <c r="B376" s="5"/>
     </row>
-    <row r="377" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="2:2" ht="15.75" customHeight="1">
       <c r="B377" s="5"/>
     </row>
-    <row r="378" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="2:2" ht="15.75" customHeight="1">
       <c r="B378" s="5"/>
     </row>
-    <row r="379" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="2:2" ht="15.75" customHeight="1">
       <c r="B379" s="5"/>
     </row>
-    <row r="380" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="2:2" ht="15.75" customHeight="1">
       <c r="B380" s="5"/>
     </row>
-    <row r="381" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="2:2" ht="15.75" customHeight="1">
       <c r="B381" s="5"/>
     </row>
-    <row r="382" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="2:2" ht="15.75" customHeight="1">
       <c r="B382" s="5"/>
     </row>
-    <row r="383" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="2:2" ht="15.75" customHeight="1">
       <c r="B383" s="5"/>
     </row>
-    <row r="384" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="2:2" ht="15.75" customHeight="1">
       <c r="B384" s="5"/>
     </row>
-    <row r="385" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="2:2" ht="15.75" customHeight="1">
       <c r="B385" s="5"/>
     </row>
-    <row r="386" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="2:2" ht="15.75" customHeight="1">
       <c r="B386" s="5"/>
     </row>
-    <row r="387" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="2:2" ht="15.75" customHeight="1">
       <c r="B387" s="5"/>
     </row>
-    <row r="388" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="2:2" ht="15.75" customHeight="1">
       <c r="B388" s="5"/>
     </row>
-    <row r="389" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="2:2" ht="15.75" customHeight="1">
       <c r="B389" s="5"/>
     </row>
-    <row r="390" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="2:2" ht="15.75" customHeight="1">
       <c r="B390" s="5"/>
     </row>
-    <row r="391" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="2:2" ht="15.75" customHeight="1">
       <c r="B391" s="5"/>
     </row>
-    <row r="392" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="2:2" ht="15.75" customHeight="1">
       <c r="B392" s="5"/>
     </row>
-    <row r="393" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="2:2" ht="15.75" customHeight="1">
       <c r="B393" s="5"/>
     </row>
-    <row r="394" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="2:2" ht="15.75" customHeight="1">
       <c r="B394" s="5"/>
     </row>
-    <row r="395" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="2:2" ht="15.75" customHeight="1">
       <c r="B395" s="5"/>
     </row>
-    <row r="396" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="2:2" ht="15.75" customHeight="1">
       <c r="B396" s="5"/>
     </row>
-    <row r="397" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="2:2" ht="15.75" customHeight="1">
       <c r="B397" s="5"/>
     </row>
-    <row r="398" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="2:2" ht="15.75" customHeight="1">
       <c r="B398" s="5"/>
     </row>
-    <row r="399" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="2:2" ht="15.75" customHeight="1">
       <c r="B399" s="5"/>
     </row>
-    <row r="400" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="2:2" ht="15.75" customHeight="1">
       <c r="B400" s="5"/>
     </row>
-    <row r="401" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="2:2" ht="15.75" customHeight="1">
       <c r="B401" s="5"/>
     </row>
-    <row r="402" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="2:2" ht="15.75" customHeight="1">
       <c r="B402" s="5"/>
     </row>
-    <row r="403" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="2:2" ht="15.75" customHeight="1">
       <c r="B403" s="5"/>
     </row>
-    <row r="404" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="2:2" ht="15.75" customHeight="1">
       <c r="B404" s="5"/>
     </row>
-    <row r="405" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="2:2" ht="15.75" customHeight="1">
       <c r="B405" s="5"/>
     </row>
-    <row r="406" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="2:2" ht="15.75" customHeight="1">
       <c r="B406" s="5"/>
     </row>
-    <row r="407" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="2:2" ht="15.75" customHeight="1">
       <c r="B407" s="5"/>
     </row>
-    <row r="408" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="2:2" ht="15.75" customHeight="1">
       <c r="B408" s="5"/>
     </row>
-    <row r="409" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="2:2" ht="15.75" customHeight="1">
       <c r="B409" s="5"/>
     </row>
-    <row r="410" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="2:2" ht="15.75" customHeight="1">
       <c r="B410" s="5"/>
     </row>
-    <row r="411" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="2:2" ht="15.75" customHeight="1">
       <c r="B411" s="5"/>
     </row>
-    <row r="412" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="2:2" ht="15.75" customHeight="1">
       <c r="B412" s="5"/>
     </row>
-    <row r="413" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="2:2" ht="15.75" customHeight="1">
       <c r="B413" s="5"/>
     </row>
-    <row r="414" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="2:2" ht="15.75" customHeight="1">
       <c r="B414" s="5"/>
     </row>
-    <row r="415" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="2:2" ht="15.75" customHeight="1">
       <c r="B415" s="5"/>
     </row>
-    <row r="416" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="2:2" ht="15.75" customHeight="1">
       <c r="B416" s="5"/>
     </row>
-    <row r="417" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="2:2" ht="15.75" customHeight="1">
       <c r="B417" s="5"/>
     </row>
-    <row r="418" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="2:2" ht="15.75" customHeight="1">
       <c r="B418" s="5"/>
     </row>
-    <row r="419" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="2:2" ht="15.75" customHeight="1">
       <c r="B419" s="5"/>
     </row>
-    <row r="420" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="2:2" ht="15.75" customHeight="1">
       <c r="B420" s="5"/>
     </row>
-    <row r="421" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="2:2" ht="15.75" customHeight="1">
       <c r="B421" s="5"/>
     </row>
-    <row r="422" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="2:2" ht="15.75" customHeight="1">
       <c r="B422" s="5"/>
     </row>
-    <row r="423" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="2:2" ht="15.75" customHeight="1">
       <c r="B423" s="5"/>
     </row>
-    <row r="424" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="2:2" ht="15.75" customHeight="1">
       <c r="B424" s="5"/>
     </row>
-    <row r="425" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="2:2" ht="15.75" customHeight="1">
       <c r="B425" s="5"/>
     </row>
-    <row r="426" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="2:2" ht="15.75" customHeight="1">
       <c r="B426" s="5"/>
     </row>
-    <row r="427" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="2:2" ht="15.75" customHeight="1">
       <c r="B427" s="5"/>
     </row>
-    <row r="428" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="2:2" ht="15.75" customHeight="1">
       <c r="B428" s="5"/>
     </row>
-    <row r="429" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="2:2" ht="15.75" customHeight="1">
       <c r="B429" s="5"/>
     </row>
-    <row r="430" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="2:2" ht="15.75" customHeight="1">
       <c r="B430" s="5"/>
     </row>
-    <row r="431" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="2:2" ht="15.75" customHeight="1">
       <c r="B431" s="5"/>
     </row>
-    <row r="432" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="2:2" ht="15.75" customHeight="1">
       <c r="B432" s="5"/>
     </row>
-    <row r="433" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="2:2" ht="15.75" customHeight="1">
       <c r="B433" s="5"/>
     </row>
-    <row r="434" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="2:2" ht="15.75" customHeight="1">
       <c r="B434" s="5"/>
     </row>
-    <row r="435" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="2:2" ht="15.75" customHeight="1">
       <c r="B435" s="5"/>
     </row>
-    <row r="436" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="2:2" ht="15.75" customHeight="1">
       <c r="B436" s="5"/>
     </row>
-    <row r="437" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="2:2" ht="15.75" customHeight="1">
       <c r="B437" s="5"/>
     </row>
-    <row r="438" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="2:2" ht="15.75" customHeight="1">
       <c r="B438" s="5"/>
     </row>
-    <row r="439" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="2:2" ht="15.75" customHeight="1">
       <c r="B439" s="5"/>
     </row>
-    <row r="440" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="2:2" ht="15.75" customHeight="1">
       <c r="B440" s="5"/>
     </row>
-    <row r="441" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="2:2" ht="15.75" customHeight="1">
       <c r="B441" s="5"/>
     </row>
-    <row r="442" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="2:2" ht="15.75" customHeight="1">
       <c r="B442" s="5"/>
     </row>
-    <row r="443" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="2:2" ht="15.75" customHeight="1">
       <c r="B443" s="5"/>
     </row>
-    <row r="444" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="2:2" ht="15.75" customHeight="1">
       <c r="B444" s="5"/>
     </row>
-    <row r="445" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="2:2" ht="15.75" customHeight="1">
       <c r="B445" s="5"/>
     </row>
-    <row r="446" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="2:2" ht="15.75" customHeight="1">
       <c r="B446" s="5"/>
     </row>
-    <row r="447" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="2:2" ht="15.75" customHeight="1">
       <c r="B447" s="5"/>
     </row>
-    <row r="448" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="2:2" ht="15.75" customHeight="1">
       <c r="B448" s="5"/>
     </row>
-    <row r="449" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="2:2" ht="15.75" customHeight="1">
       <c r="B449" s="5"/>
     </row>
-    <row r="450" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="2:2" ht="15.75" customHeight="1">
       <c r="B450" s="5"/>
     </row>
-    <row r="451" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="2:2" ht="15.75" customHeight="1">
       <c r="B451" s="5"/>
     </row>
-    <row r="452" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="2:2" ht="15.75" customHeight="1">
       <c r="B452" s="5"/>
     </row>
-    <row r="453" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="2:2" ht="15.75" customHeight="1">
       <c r="B453" s="5"/>
     </row>
-    <row r="454" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="2:2" ht="15.75" customHeight="1">
       <c r="B454" s="5"/>
     </row>
-    <row r="455" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="2:2" ht="15.75" customHeight="1">
       <c r="B455" s="5"/>
     </row>
-    <row r="456" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="2:2" ht="15.75" customHeight="1">
       <c r="B456" s="5"/>
     </row>
-    <row r="457" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="2:2" ht="15.75" customHeight="1">
       <c r="B457" s="5"/>
     </row>
-    <row r="458" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="2:2" ht="15.75" customHeight="1">
       <c r="B458" s="5"/>
     </row>
-    <row r="459" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="2:2" ht="15.75" customHeight="1">
       <c r="B459" s="5"/>
     </row>
-    <row r="460" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="2:2" ht="15.75" customHeight="1">
       <c r="B460" s="5"/>
     </row>
-    <row r="461" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="2:2" ht="15.75" customHeight="1">
       <c r="B461" s="5"/>
     </row>
-    <row r="462" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="2:2" ht="15.75" customHeight="1">
       <c r="B462" s="5"/>
     </row>
-    <row r="463" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="2:2" ht="15.75" customHeight="1">
       <c r="B463" s="5"/>
     </row>
-    <row r="464" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="2:2" ht="15.75" customHeight="1">
       <c r="B464" s="5"/>
     </row>
-    <row r="465" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="2:2" ht="15.75" customHeight="1">
       <c r="B465" s="5"/>
     </row>
-    <row r="466" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="2:2" ht="15.75" customHeight="1">
       <c r="B466" s="5"/>
     </row>
-    <row r="467" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="2:2" ht="15.75" customHeight="1">
       <c r="B467" s="5"/>
     </row>
-    <row r="468" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="2:2" ht="15.75" customHeight="1">
       <c r="B468" s="5"/>
     </row>
-    <row r="469" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="2:2" ht="15.75" customHeight="1">
       <c r="B469" s="5"/>
     </row>
-    <row r="470" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="2:2" ht="15.75" customHeight="1">
       <c r="B470" s="5"/>
     </row>
-    <row r="471" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="2:2" ht="15.75" customHeight="1">
       <c r="B471" s="5"/>
     </row>
-    <row r="472" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="2:2" ht="15.75" customHeight="1">
       <c r="B472" s="5"/>
     </row>
-    <row r="473" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="2:2" ht="15.75" customHeight="1">
       <c r="B473" s="5"/>
     </row>
-    <row r="474" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="2:2" ht="15.75" customHeight="1">
       <c r="B474" s="5"/>
     </row>
-    <row r="475" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="475" spans="2:2" ht="15.75" customHeight="1">
       <c r="B475" s="5"/>
     </row>
-    <row r="476" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="2:2" ht="15.75" customHeight="1">
       <c r="B476" s="5"/>
     </row>
-    <row r="477" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="477" spans="2:2" ht="15.75" customHeight="1">
       <c r="B477" s="5"/>
     </row>
-    <row r="478" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="2:2" ht="15.75" customHeight="1">
       <c r="B478" s="5"/>
     </row>
-    <row r="479" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="479" spans="2:2" ht="15.75" customHeight="1">
       <c r="B479" s="5"/>
     </row>
-    <row r="480" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="2:2" ht="15.75" customHeight="1">
       <c r="B480" s="5"/>
     </row>
-    <row r="481" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="481" spans="2:2" ht="15.75" customHeight="1">
       <c r="B481" s="5"/>
     </row>
-    <row r="482" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="482" spans="2:2" ht="15.75" customHeight="1">
       <c r="B482" s="5"/>
     </row>
-    <row r="483" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="483" spans="2:2" ht="15.75" customHeight="1">
       <c r="B483" s="5"/>
     </row>
-    <row r="484" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="484" spans="2:2" ht="15.75" customHeight="1">
       <c r="B484" s="5"/>
     </row>
-    <row r="485" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="485" spans="2:2" ht="15.75" customHeight="1">
       <c r="B485" s="5"/>
     </row>
-    <row r="486" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="486" spans="2:2" ht="15.75" customHeight="1">
       <c r="B486" s="5"/>
     </row>
-    <row r="487" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="487" spans="2:2" ht="15.75" customHeight="1">
       <c r="B487" s="5"/>
     </row>
-    <row r="488" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="488" spans="2:2" ht="15.75" customHeight="1">
       <c r="B488" s="5"/>
     </row>
-    <row r="489" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="489" spans="2:2" ht="15.75" customHeight="1">
       <c r="B489" s="5"/>
     </row>
-    <row r="490" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="490" spans="2:2" ht="15.75" customHeight="1">
       <c r="B490" s="5"/>
     </row>
-    <row r="491" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="491" spans="2:2" ht="15.75" customHeight="1">
       <c r="B491" s="5"/>
     </row>
-    <row r="492" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="492" spans="2:2" ht="15.75" customHeight="1">
       <c r="B492" s="5"/>
     </row>
-    <row r="493" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="493" spans="2:2" ht="15.75" customHeight="1">
       <c r="B493" s="5"/>
     </row>
-    <row r="494" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="494" spans="2:2" ht="15.75" customHeight="1">
       <c r="B494" s="5"/>
     </row>
-    <row r="495" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="495" spans="2:2" ht="15.75" customHeight="1">
       <c r="B495" s="5"/>
     </row>
-    <row r="496" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="496" spans="2:2" ht="15.75" customHeight="1">
       <c r="B496" s="5"/>
     </row>
-    <row r="497" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="497" spans="2:2" ht="15.75" customHeight="1">
       <c r="B497" s="5"/>
     </row>
-    <row r="498" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="498" spans="2:2" ht="15.75" customHeight="1">
       <c r="B498" s="5"/>
     </row>
-    <row r="499" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="499" spans="2:2" ht="15.75" customHeight="1">
       <c r="B499" s="5"/>
     </row>
-    <row r="500" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="500" spans="2:2" ht="15.75" customHeight="1">
       <c r="B500" s="5"/>
     </row>
-    <row r="501" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="501" spans="2:2" ht="15.75" customHeight="1">
       <c r="B501" s="5"/>
     </row>
-    <row r="502" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="502" spans="2:2" ht="15.75" customHeight="1">
       <c r="B502" s="5"/>
     </row>
-    <row r="503" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="503" spans="2:2" ht="15.75" customHeight="1">
       <c r="B503" s="5"/>
     </row>
-    <row r="504" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="504" spans="2:2" ht="15.75" customHeight="1">
       <c r="B504" s="5"/>
     </row>
-    <row r="505" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="505" spans="2:2" ht="15.75" customHeight="1">
       <c r="B505" s="5"/>
     </row>
-    <row r="506" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="506" spans="2:2" ht="15.75" customHeight="1">
       <c r="B506" s="5"/>
     </row>
-    <row r="507" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="507" spans="2:2" ht="15.75" customHeight="1">
       <c r="B507" s="5"/>
     </row>
-    <row r="508" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="508" spans="2:2" ht="15.75" customHeight="1">
       <c r="B508" s="5"/>
     </row>
-    <row r="509" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="509" spans="2:2" ht="15.75" customHeight="1">
       <c r="B509" s="5"/>
     </row>
-    <row r="510" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="510" spans="2:2" ht="15.75" customHeight="1">
       <c r="B510" s="5"/>
     </row>
-    <row r="511" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="511" spans="2:2" ht="15.75" customHeight="1">
       <c r="B511" s="5"/>
     </row>
-    <row r="512" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="512" spans="2:2" ht="15.75" customHeight="1">
       <c r="B512" s="5"/>
     </row>
-    <row r="513" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="513" spans="2:2" ht="15.75" customHeight="1">
       <c r="B513" s="5"/>
     </row>
-    <row r="514" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="514" spans="2:2" ht="15.75" customHeight="1">
       <c r="B514" s="5"/>
     </row>
-    <row r="515" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="515" spans="2:2" ht="15.75" customHeight="1">
       <c r="B515" s="5"/>
     </row>
-    <row r="516" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="516" spans="2:2" ht="15.75" customHeight="1">
       <c r="B516" s="5"/>
     </row>
-    <row r="517" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="517" spans="2:2" ht="15.75" customHeight="1">
       <c r="B517" s="5"/>
     </row>
-    <row r="518" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="518" spans="2:2" ht="15.75" customHeight="1">
       <c r="B518" s="5"/>
     </row>
-    <row r="519" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="519" spans="2:2" ht="15.75" customHeight="1">
       <c r="B519" s="5"/>
     </row>
-    <row r="520" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="520" spans="2:2" ht="15.75" customHeight="1">
       <c r="B520" s="5"/>
     </row>
-    <row r="521" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="521" spans="2:2" ht="15.75" customHeight="1">
       <c r="B521" s="5"/>
     </row>
-    <row r="522" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="522" spans="2:2" ht="15.75" customHeight="1">
       <c r="B522" s="5"/>
     </row>
-    <row r="523" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="523" spans="2:2" ht="15.75" customHeight="1">
       <c r="B523" s="5"/>
     </row>
-    <row r="524" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="524" spans="2:2" ht="15.75" customHeight="1">
       <c r="B524" s="5"/>
     </row>
-    <row r="525" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="525" spans="2:2" ht="15.75" customHeight="1">
       <c r="B525" s="5"/>
     </row>
-    <row r="526" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="526" spans="2:2" ht="15.75" customHeight="1">
       <c r="B526" s="5"/>
     </row>
-    <row r="527" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="527" spans="2:2" ht="15.75" customHeight="1">
       <c r="B527" s="5"/>
     </row>
-    <row r="528" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="528" spans="2:2" ht="15.75" customHeight="1">
       <c r="B528" s="5"/>
     </row>
-    <row r="529" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="529" spans="2:2" ht="15.75" customHeight="1">
       <c r="B529" s="5"/>
     </row>
-    <row r="530" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="530" spans="2:2" ht="15.75" customHeight="1">
       <c r="B530" s="5"/>
     </row>
-    <row r="531" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="531" spans="2:2" ht="15.75" customHeight="1">
       <c r="B531" s="5"/>
     </row>
-    <row r="532" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="532" spans="2:2" ht="15.75" customHeight="1">
       <c r="B532" s="5"/>
     </row>
-    <row r="533" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="533" spans="2:2" ht="15.75" customHeight="1">
       <c r="B533" s="5"/>
     </row>
-    <row r="534" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="534" spans="2:2" ht="15.75" customHeight="1">
       <c r="B534" s="5"/>
     </row>
-    <row r="535" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="535" spans="2:2" ht="15.75" customHeight="1">
       <c r="B535" s="5"/>
     </row>
-    <row r="536" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="536" spans="2:2" ht="15.75" customHeight="1">
       <c r="B536" s="5"/>
     </row>
-    <row r="537" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="537" spans="2:2" ht="15.75" customHeight="1">
       <c r="B537" s="5"/>
     </row>
-    <row r="538" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="538" spans="2:2" ht="15.75" customHeight="1">
       <c r="B538" s="5"/>
     </row>
-    <row r="539" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="539" spans="2:2" ht="15.75" customHeight="1">
       <c r="B539" s="5"/>
     </row>
-    <row r="540" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="540" spans="2:2" ht="15.75" customHeight="1">
       <c r="B540" s="5"/>
     </row>
-    <row r="541" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="541" spans="2:2" ht="15.75" customHeight="1">
       <c r="B541" s="5"/>
     </row>
-    <row r="542" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="542" spans="2:2" ht="15.75" customHeight="1">
       <c r="B542" s="5"/>
     </row>
-    <row r="543" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="543" spans="2:2" ht="15.75" customHeight="1">
       <c r="B543" s="5"/>
     </row>
-    <row r="544" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="544" spans="2:2" ht="15.75" customHeight="1">
       <c r="B544" s="5"/>
     </row>
-    <row r="545" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="545" spans="2:2" ht="15.75" customHeight="1">
       <c r="B545" s="5"/>
     </row>
-    <row r="546" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="546" spans="2:2" ht="15.75" customHeight="1">
       <c r="B546" s="5"/>
     </row>
-    <row r="547" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="547" spans="2:2" ht="15.75" customHeight="1">
       <c r="B547" s="5"/>
     </row>
-    <row r="548" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="548" spans="2:2" ht="15.75" customHeight="1">
       <c r="B548" s="5"/>
     </row>
-    <row r="549" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="549" spans="2:2" ht="15.75" customHeight="1">
       <c r="B549" s="5"/>
     </row>
-    <row r="550" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="550" spans="2:2" ht="15.75" customHeight="1">
       <c r="B550" s="5"/>
     </row>
-    <row r="551" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="551" spans="2:2" ht="15.75" customHeight="1">
       <c r="B551" s="5"/>
     </row>
-    <row r="552" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="552" spans="2:2" ht="15.75" customHeight="1">
       <c r="B552" s="5"/>
     </row>
-    <row r="553" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="553" spans="2:2" ht="15.75" customHeight="1">
       <c r="B553" s="5"/>
     </row>
-    <row r="554" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="554" spans="2:2" ht="15.75" customHeight="1">
       <c r="B554" s="5"/>
     </row>
-    <row r="555" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="555" spans="2:2" ht="15.75" customHeight="1">
       <c r="B555" s="5"/>
     </row>
-    <row r="556" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="556" spans="2:2" ht="15.75" customHeight="1">
       <c r="B556" s="5"/>
     </row>
-    <row r="557" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="557" spans="2:2" ht="15.75" customHeight="1">
       <c r="B557" s="5"/>
     </row>
-    <row r="558" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="558" spans="2:2" ht="15.75" customHeight="1">
       <c r="B558" s="5"/>
     </row>
-    <row r="559" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="559" spans="2:2" ht="15.75" customHeight="1">
       <c r="B559" s="5"/>
     </row>
-    <row r="560" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="560" spans="2:2" ht="15.75" customHeight="1">
       <c r="B560" s="5"/>
     </row>
-    <row r="561" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="561" spans="2:2" ht="15.75" customHeight="1">
       <c r="B561" s="5"/>
     </row>
-    <row r="562" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="562" spans="2:2" ht="15.75" customHeight="1">
       <c r="B562" s="5"/>
     </row>
-    <row r="563" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="563" spans="2:2" ht="15.75" customHeight="1">
       <c r="B563" s="5"/>
     </row>
-    <row r="564" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="564" spans="2:2" ht="15.75" customHeight="1">
       <c r="B564" s="5"/>
     </row>
-    <row r="565" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="565" spans="2:2" ht="15.75" customHeight="1">
       <c r="B565" s="5"/>
     </row>
-    <row r="566" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="566" spans="2:2" ht="15.75" customHeight="1">
       <c r="B566" s="5"/>
     </row>
-    <row r="567" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="567" spans="2:2" ht="15.75" customHeight="1">
       <c r="B567" s="5"/>
     </row>
-    <row r="568" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="568" spans="2:2" ht="15.75" customHeight="1">
       <c r="B568" s="5"/>
     </row>
-    <row r="569" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="569" spans="2:2" ht="15.75" customHeight="1">
       <c r="B569" s="5"/>
     </row>
-    <row r="570" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="570" spans="2:2" ht="15.75" customHeight="1">
       <c r="B570" s="5"/>
     </row>
-    <row r="571" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="571" spans="2:2" ht="15.75" customHeight="1">
       <c r="B571" s="5"/>
     </row>
-    <row r="572" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="572" spans="2:2" ht="15.75" customHeight="1">
       <c r="B572" s="5"/>
     </row>
-    <row r="573" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="573" spans="2:2" ht="15.75" customHeight="1">
       <c r="B573" s="5"/>
     </row>
-    <row r="574" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="574" spans="2:2" ht="15.75" customHeight="1">
       <c r="B574" s="5"/>
     </row>
-    <row r="575" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="575" spans="2:2" ht="15.75" customHeight="1">
       <c r="B575" s="5"/>
     </row>
-    <row r="576" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="576" spans="2:2" ht="15.75" customHeight="1">
       <c r="B576" s="5"/>
     </row>
-    <row r="577" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="577" spans="2:2" ht="15.75" customHeight="1">
       <c r="B577" s="5"/>
     </row>
-    <row r="578" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="578" spans="2:2" ht="15.75" customHeight="1">
       <c r="B578" s="5"/>
     </row>
-    <row r="579" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="579" spans="2:2" ht="15.75" customHeight="1">
       <c r="B579" s="5"/>
     </row>
-    <row r="580" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="580" spans="2:2" ht="15.75" customHeight="1">
       <c r="B580" s="5"/>
     </row>
-    <row r="581" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="581" spans="2:2" ht="15.75" customHeight="1">
       <c r="B581" s="5"/>
     </row>
-    <row r="582" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="582" spans="2:2" ht="15.75" customHeight="1">
       <c r="B582" s="5"/>
     </row>
-    <row r="583" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="583" spans="2:2" ht="15.75" customHeight="1">
       <c r="B583" s="5"/>
     </row>
-    <row r="584" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="584" spans="2:2" ht="15.75" customHeight="1">
       <c r="B584" s="5"/>
     </row>
-    <row r="585" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="585" spans="2:2" ht="15.75" customHeight="1">
       <c r="B585" s="5"/>
     </row>
-    <row r="586" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="586" spans="2:2" ht="15.75" customHeight="1">
       <c r="B586" s="5"/>
     </row>
-    <row r="587" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="587" spans="2:2" ht="15.75" customHeight="1">
       <c r="B587" s="5"/>
     </row>
-    <row r="588" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="588" spans="2:2" ht="15.75" customHeight="1">
       <c r="B588" s="5"/>
     </row>
-    <row r="589" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="589" spans="2:2" ht="15.75" customHeight="1">
       <c r="B589" s="5"/>
     </row>
-    <row r="590" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="590" spans="2:2" ht="15.75" customHeight="1">
       <c r="B590" s="5"/>
     </row>
-    <row r="591" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="591" spans="2:2" ht="15.75" customHeight="1">
       <c r="B591" s="5"/>
     </row>
-    <row r="592" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="592" spans="2:2" ht="15.75" customHeight="1">
       <c r="B592" s="5"/>
     </row>
-    <row r="593" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="593" spans="2:2" ht="15.75" customHeight="1">
       <c r="B593" s="5"/>
     </row>
-    <row r="594" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="594" spans="2:2" ht="15.75" customHeight="1">
       <c r="B594" s="5"/>
     </row>
-    <row r="595" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="595" spans="2:2" ht="15.75" customHeight="1">
       <c r="B595" s="5"/>
     </row>
-    <row r="596" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="596" spans="2:2" ht="15.75" customHeight="1">
       <c r="B596" s="5"/>
     </row>
-    <row r="597" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="597" spans="2:2" ht="15.75" customHeight="1">
       <c r="B597" s="5"/>
     </row>
-    <row r="598" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="598" spans="2:2" ht="15.75" customHeight="1">
       <c r="B598" s="5"/>
     </row>
-    <row r="599" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="599" spans="2:2" ht="15.75" customHeight="1">
       <c r="B599" s="5"/>
     </row>
-    <row r="600" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="600" spans="2:2" ht="15.75" customHeight="1">
       <c r="B600" s="5"/>
     </row>
-    <row r="601" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="601" spans="2:2" ht="15.75" customHeight="1">
       <c r="B601" s="5"/>
     </row>
-    <row r="602" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="602" spans="2:2" ht="15.75" customHeight="1">
       <c r="B602" s="5"/>
     </row>
-    <row r="603" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="603" spans="2:2" ht="15.75" customHeight="1">
       <c r="B603" s="5"/>
     </row>
-    <row r="604" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="604" spans="2:2" ht="15.75" customHeight="1">
       <c r="B604" s="5"/>
     </row>
-    <row r="605" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="605" spans="2:2" ht="15.75" customHeight="1">
       <c r="B605" s="5"/>
     </row>
-    <row r="606" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="606" spans="2:2" ht="15.75" customHeight="1">
       <c r="B606" s="5"/>
     </row>
-    <row r="607" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="607" spans="2:2" ht="15.75" customHeight="1">
       <c r="B607" s="5"/>
     </row>
-    <row r="608" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="608" spans="2:2" ht="15.75" customHeight="1">
       <c r="B608" s="5"/>
     </row>
-    <row r="609" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="609" spans="2:2" ht="15.75" customHeight="1">
       <c r="B609" s="5"/>
     </row>
-    <row r="610" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="610" spans="2:2" ht="15.75" customHeight="1">
       <c r="B610" s="5"/>
     </row>
-    <row r="611" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="611" spans="2:2" ht="15.75" customHeight="1">
       <c r="B611" s="5"/>
     </row>
-    <row r="612" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="612" spans="2:2" ht="15.75" customHeight="1">
       <c r="B612" s="5"/>
     </row>
-    <row r="613" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="613" spans="2:2" ht="15.75" customHeight="1">
       <c r="B613" s="5"/>
     </row>
-    <row r="614" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="614" spans="2:2" ht="15.75" customHeight="1">
       <c r="B614" s="5"/>
     </row>
-    <row r="615" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="615" spans="2:2" ht="15.75" customHeight="1">
       <c r="B615" s="5"/>
     </row>
-    <row r="616" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="616" spans="2:2" ht="15.75" customHeight="1">
       <c r="B616" s="5"/>
     </row>
-    <row r="617" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="617" spans="2:2" ht="15.75" customHeight="1">
       <c r="B617" s="5"/>
     </row>
-    <row r="618" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="618" spans="2:2" ht="15.75" customHeight="1">
       <c r="B618" s="5"/>
     </row>
-    <row r="619" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="619" spans="2:2" ht="15.75" customHeight="1">
       <c r="B619" s="5"/>
     </row>
-    <row r="620" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="620" spans="2:2" ht="15.75" customHeight="1">
       <c r="B620" s="5"/>
     </row>
-    <row r="621" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="621" spans="2:2" ht="15.75" customHeight="1">
       <c r="B621" s="5"/>
     </row>
-    <row r="622" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="622" spans="2:2" ht="15.75" customHeight="1">
       <c r="B622" s="5"/>
     </row>
-    <row r="623" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="623" spans="2:2" ht="15.75" customHeight="1">
       <c r="B623" s="5"/>
     </row>
-    <row r="624" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="624" spans="2:2" ht="15.75" customHeight="1">
       <c r="B624" s="5"/>
     </row>
-    <row r="625" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="625" spans="2:2" ht="15.75" customHeight="1">
       <c r="B625" s="5"/>
     </row>
-    <row r="626" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="626" spans="2:2" ht="15.75" customHeight="1">
       <c r="B626" s="5"/>
     </row>
-    <row r="627" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="627" spans="2:2" ht="15.75" customHeight="1">
       <c r="B627" s="5"/>
     </row>
-    <row r="628" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="628" spans="2:2" ht="15.75" customHeight="1">
       <c r="B628" s="5"/>
     </row>
-    <row r="629" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="629" spans="2:2" ht="15.75" customHeight="1">
       <c r="B629" s="5"/>
     </row>
-    <row r="630" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="630" spans="2:2" ht="15.75" customHeight="1">
       <c r="B630" s="5"/>
     </row>
-    <row r="631" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="631" spans="2:2" ht="15.75" customHeight="1">
       <c r="B631" s="5"/>
     </row>
-    <row r="632" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="632" spans="2:2" ht="15.75" customHeight="1">
       <c r="B632" s="5"/>
     </row>
-    <row r="633" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="633" spans="2:2" ht="15.75" customHeight="1">
       <c r="B633" s="5"/>
     </row>
-    <row r="634" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="634" spans="2:2" ht="15.75" customHeight="1">
       <c r="B634" s="5"/>
     </row>
-    <row r="635" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="635" spans="2:2" ht="15.75" customHeight="1">
       <c r="B635" s="5"/>
     </row>
-    <row r="636" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="636" spans="2:2" ht="15.75" customHeight="1">
       <c r="B636" s="5"/>
     </row>
-    <row r="637" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="637" spans="2:2" ht="15.75" customHeight="1">
       <c r="B637" s="5"/>
     </row>
-    <row r="638" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="638" spans="2:2" ht="15.75" customHeight="1">
       <c r="B638" s="5"/>
     </row>
-    <row r="639" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="639" spans="2:2" ht="15.75" customHeight="1">
       <c r="B639" s="5"/>
     </row>
-    <row r="640" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="640" spans="2:2" ht="15.75" customHeight="1">
       <c r="B640" s="5"/>
     </row>
-    <row r="641" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="641" spans="2:2" ht="15.75" customHeight="1">
       <c r="B641" s="5"/>
     </row>
-    <row r="642" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="642" spans="2:2" ht="15.75" customHeight="1">
       <c r="B642" s="5"/>
     </row>
-    <row r="643" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="643" spans="2:2" ht="15.75" customHeight="1">
       <c r="B643" s="5"/>
     </row>
-    <row r="644" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="644" spans="2:2" ht="15.75" customHeight="1">
       <c r="B644" s="5"/>
     </row>
-    <row r="645" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="645" spans="2:2" ht="15.75" customHeight="1">
       <c r="B645" s="5"/>
     </row>
-    <row r="646" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="646" spans="2:2" ht="15.75" customHeight="1">
       <c r="B646" s="5"/>
     </row>
-    <row r="647" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="647" spans="2:2" ht="15.75" customHeight="1">
       <c r="B647" s="5"/>
     </row>
-    <row r="648" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="648" spans="2:2" ht="15.75" customHeight="1">
       <c r="B648" s="5"/>
     </row>
-    <row r="649" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="649" spans="2:2" ht="15.75" customHeight="1">
       <c r="B649" s="5"/>
     </row>
-    <row r="650" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="650" spans="2:2" ht="15.75" customHeight="1">
       <c r="B650" s="5"/>
     </row>
-    <row r="651" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="651" spans="2:2" ht="15.75" customHeight="1">
       <c r="B651" s="5"/>
     </row>
-    <row r="652" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="652" spans="2:2" ht="15.75" customHeight="1">
       <c r="B652" s="5"/>
     </row>
-    <row r="653" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="653" spans="2:2" ht="15.75" customHeight="1">
       <c r="B653" s="5"/>
     </row>
-    <row r="654" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="654" spans="2:2" ht="15.75" customHeight="1">
       <c r="B654" s="5"/>
     </row>
-    <row r="655" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="655" spans="2:2" ht="15.75" customHeight="1">
       <c r="B655" s="5"/>
     </row>
-    <row r="656" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="656" spans="2:2" ht="15.75" customHeight="1">
       <c r="B656" s="5"/>
     </row>
-    <row r="657" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="657" spans="2:2" ht="15.75" customHeight="1">
       <c r="B657" s="5"/>
     </row>
-    <row r="658" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="658" spans="2:2" ht="15.75" customHeight="1">
       <c r="B658" s="5"/>
     </row>
-    <row r="659" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="659" spans="2:2" ht="15.75" customHeight="1">
       <c r="B659" s="5"/>
     </row>
-    <row r="660" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="660" spans="2:2" ht="15.75" customHeight="1">
       <c r="B660" s="5"/>
     </row>
-    <row r="661" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="661" spans="2:2" ht="15.75" customHeight="1">
       <c r="B661" s="5"/>
     </row>
-    <row r="662" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="662" spans="2:2" ht="15.75" customHeight="1">
       <c r="B662" s="5"/>
     </row>
-    <row r="663" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="663" spans="2:2" ht="15.75" customHeight="1">
       <c r="B663" s="5"/>
     </row>
-    <row r="664" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="664" spans="2:2" ht="15.75" customHeight="1">
       <c r="B664" s="5"/>
     </row>
-    <row r="665" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="665" spans="2:2" ht="15.75" customHeight="1">
       <c r="B665" s="5"/>
     </row>
-    <row r="666" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="666" spans="2:2" ht="15.75" customHeight="1">
       <c r="B666" s="5"/>
     </row>
-    <row r="667" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="667" spans="2:2" ht="15.75" customHeight="1">
       <c r="B667" s="5"/>
     </row>
-    <row r="668" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="668" spans="2:2" ht="15.75" customHeight="1">
       <c r="B668" s="5"/>
     </row>
-    <row r="669" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="669" spans="2:2" ht="15.75" customHeight="1">
       <c r="B669" s="5"/>
     </row>
-    <row r="670" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="670" spans="2:2" ht="15.75" customHeight="1">
       <c r="B670" s="5"/>
     </row>
-    <row r="671" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="671" spans="2:2" ht="15.75" customHeight="1">
       <c r="B671" s="5"/>
     </row>
-    <row r="672" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="672" spans="2:2" ht="15.75" customHeight="1">
       <c r="B672" s="5"/>
     </row>
-    <row r="673" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="673" spans="2:2" ht="15.75" customHeight="1">
       <c r="B673" s="5"/>
     </row>
-    <row r="674" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="674" spans="2:2" ht="15.75" customHeight="1">
       <c r="B674" s="5"/>
     </row>
-    <row r="675" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="675" spans="2:2" ht="15.75" customHeight="1">
       <c r="B675" s="5"/>
     </row>
-    <row r="676" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="676" spans="2:2" ht="15.75" customHeight="1">
       <c r="B676" s="5"/>
     </row>
-    <row r="677" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="677" spans="2:2" ht="15.75" customHeight="1">
       <c r="B677" s="5"/>
     </row>
-    <row r="678" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="678" spans="2:2" ht="15.75" customHeight="1">
       <c r="B678" s="5"/>
     </row>
-    <row r="679" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="679" spans="2:2" ht="15.75" customHeight="1">
       <c r="B679" s="5"/>
     </row>
-    <row r="680" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="680" spans="2:2" ht="15.75" customHeight="1">
       <c r="B680" s="5"/>
     </row>
-    <row r="681" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="681" spans="2:2" ht="15.75" customHeight="1">
       <c r="B681" s="5"/>
     </row>
-    <row r="682" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="682" spans="2:2" ht="15.75" customHeight="1">
       <c r="B682" s="5"/>
     </row>
-    <row r="683" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="683" spans="2:2" ht="15.75" customHeight="1">
       <c r="B683" s="5"/>
     </row>
-    <row r="684" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="684" spans="2:2" ht="15.75" customHeight="1">
       <c r="B684" s="5"/>
     </row>
-    <row r="685" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="685" spans="2:2" ht="15.75" customHeight="1">
       <c r="B685" s="5"/>
     </row>
-    <row r="686" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="686" spans="2:2" ht="15.75" customHeight="1">
       <c r="B686" s="5"/>
     </row>
-    <row r="687" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="687" spans="2:2" ht="15.75" customHeight="1">
       <c r="B687" s="5"/>
     </row>
-    <row r="688" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="688" spans="2:2" ht="15.75" customHeight="1">
       <c r="B688" s="5"/>
     </row>
-    <row r="689" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="689" spans="2:2" ht="15.75" customHeight="1">
       <c r="B689" s="5"/>
     </row>
-    <row r="690" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="690" spans="2:2" ht="15.75" customHeight="1">
       <c r="B690" s="5"/>
     </row>
-    <row r="691" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="691" spans="2:2" ht="15.75" customHeight="1">
       <c r="B691" s="5"/>
     </row>
-    <row r="692" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="692" spans="2:2" ht="15.75" customHeight="1">
       <c r="B692" s="5"/>
     </row>
-    <row r="693" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="693" spans="2:2" ht="15.75" customHeight="1">
       <c r="B693" s="5"/>
     </row>
-    <row r="694" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="694" spans="2:2" ht="15.75" customHeight="1">
       <c r="B694" s="5"/>
     </row>
-    <row r="695" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="695" spans="2:2" ht="15.75" customHeight="1">
       <c r="B695" s="5"/>
     </row>
-    <row r="696" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="696" spans="2:2" ht="15.75" customHeight="1">
       <c r="B696" s="5"/>
     </row>
-    <row r="697" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="697" spans="2:2" ht="15.75" customHeight="1">
       <c r="B697" s="5"/>
     </row>
-    <row r="698" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="698" spans="2:2" ht="15.75" customHeight="1">
       <c r="B698" s="5"/>
     </row>
-    <row r="699" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="699" spans="2:2" ht="15.75" customHeight="1">
       <c r="B699" s="5"/>
     </row>
-    <row r="700" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="700" spans="2:2" ht="15.75" customHeight="1">
       <c r="B700" s="5"/>
     </row>
-    <row r="701" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="701" spans="2:2" ht="15.75" customHeight="1">
       <c r="B701" s="5"/>
     </row>
-    <row r="702" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="702" spans="2:2" ht="15.75" customHeight="1">
       <c r="B702" s="5"/>
     </row>
-    <row r="703" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="703" spans="2:2" ht="15.75" customHeight="1">
       <c r="B703" s="5"/>
     </row>
-    <row r="704" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="704" spans="2:2" ht="15.75" customHeight="1">
       <c r="B704" s="5"/>
     </row>
-    <row r="705" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="705" spans="2:2" ht="15.75" customHeight="1">
       <c r="B705" s="5"/>
     </row>
-    <row r="706" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="706" spans="2:2" ht="15.75" customHeight="1">
       <c r="B706" s="5"/>
     </row>
-    <row r="707" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="707" spans="2:2" ht="15.75" customHeight="1">
       <c r="B707" s="5"/>
     </row>
-    <row r="708" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="708" spans="2:2" ht="15.75" customHeight="1">
       <c r="B708" s="5"/>
     </row>
-    <row r="709" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="709" spans="2:2" ht="15.75" customHeight="1">
       <c r="B709" s="5"/>
     </row>
-    <row r="710" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="710" spans="2:2" ht="15.75" customHeight="1">
       <c r="B710" s="5"/>
     </row>
-    <row r="711" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="711" spans="2:2" ht="15.75" customHeight="1">
       <c r="B711" s="5"/>
     </row>
-    <row r="712" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="712" spans="2:2" ht="15.75" customHeight="1">
       <c r="B712" s="5"/>
     </row>
-    <row r="713" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="713" spans="2:2" ht="15.75" customHeight="1">
       <c r="B713" s="5"/>
     </row>
-    <row r="714" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="714" spans="2:2" ht="15.75" customHeight="1">
       <c r="B714" s="5"/>
     </row>
-    <row r="715" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="715" spans="2:2" ht="15.75" customHeight="1">
       <c r="B715" s="5"/>
     </row>
-    <row r="716" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="716" spans="2:2" ht="15.75" customHeight="1">
       <c r="B716" s="5"/>
     </row>
-    <row r="717" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="717" spans="2:2" ht="15.75" customHeight="1">
       <c r="B717" s="5"/>
     </row>
-    <row r="718" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="718" spans="2:2" ht="15.75" customHeight="1">
       <c r="B718" s="5"/>
     </row>
-    <row r="719" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="719" spans="2:2" ht="15.75" customHeight="1">
       <c r="B719" s="5"/>
     </row>
-    <row r="720" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="720" spans="2:2" ht="15.75" customHeight="1">
       <c r="B720" s="5"/>
     </row>
-    <row r="721" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="721" spans="2:2" ht="15.75" customHeight="1">
       <c r="B721" s="5"/>
     </row>
-    <row r="722" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="722" spans="2:2" ht="15.75" customHeight="1">
       <c r="B722" s="5"/>
     </row>
-    <row r="723" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="723" spans="2:2" ht="15.75" customHeight="1">
       <c r="B723" s="5"/>
     </row>
-    <row r="724" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="724" spans="2:2" ht="15.75" customHeight="1">
       <c r="B724" s="5"/>
     </row>
-    <row r="725" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="725" spans="2:2" ht="15.75" customHeight="1">
       <c r="B725" s="5"/>
     </row>
-    <row r="726" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="726" spans="2:2" ht="15.75" customHeight="1">
       <c r="B726" s="5"/>
     </row>
-    <row r="727" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="727" spans="2:2" ht="15.75" customHeight="1">
       <c r="B727" s="5"/>
     </row>
-    <row r="728" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="728" spans="2:2" ht="15.75" customHeight="1">
       <c r="B728" s="5"/>
     </row>
-    <row r="729" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="729" spans="2:2" ht="15.75" customHeight="1">
       <c r="B729" s="5"/>
     </row>
-    <row r="730" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="730" spans="2:2" ht="15.75" customHeight="1">
       <c r="B730" s="5"/>
     </row>
-    <row r="731" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="731" spans="2:2" ht="15.75" customHeight="1">
       <c r="B731" s="5"/>
     </row>
-    <row r="732" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="732" spans="2:2" ht="15.75" customHeight="1">
       <c r="B732" s="5"/>
     </row>
-    <row r="733" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="733" spans="2:2" ht="15.75" customHeight="1">
       <c r="B733" s="5"/>
     </row>
-    <row r="734" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="734" spans="2:2" ht="15.75" customHeight="1">
       <c r="B734" s="5"/>
     </row>
-    <row r="735" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="735" spans="2:2" ht="15.75" customHeight="1">
       <c r="B735" s="5"/>
     </row>
-    <row r="736" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="736" spans="2:2" ht="15.75" customHeight="1">
       <c r="B736" s="5"/>
     </row>
-    <row r="737" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="737" spans="2:2" ht="15.75" customHeight="1">
       <c r="B737" s="5"/>
     </row>
-    <row r="738" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="738" spans="2:2" ht="15.75" customHeight="1">
       <c r="B738" s="5"/>
     </row>
-    <row r="739" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="739" spans="2:2" ht="15.75" customHeight="1">
       <c r="B739" s="5"/>
     </row>
-    <row r="740" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="740" spans="2:2" ht="15.75" customHeight="1">
       <c r="B740" s="5"/>
     </row>
-    <row r="741" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="741" spans="2:2" ht="15.75" customHeight="1">
       <c r="B741" s="5"/>
     </row>
-    <row r="742" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="742" spans="2:2" ht="15.75" customHeight="1">
       <c r="B742" s="5"/>
     </row>
-    <row r="743" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="743" spans="2:2" ht="15.75" customHeight="1">
       <c r="B743" s="5"/>
     </row>
-    <row r="744" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="744" spans="2:2" ht="15.75" customHeight="1">
       <c r="B744" s="5"/>
     </row>
-    <row r="745" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="745" spans="2:2" ht="15.75" customHeight="1">
       <c r="B745" s="5"/>
     </row>
-    <row r="746" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="746" spans="2:2" ht="15.75" customHeight="1">
       <c r="B746" s="5"/>
     </row>
-    <row r="747" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="747" spans="2:2" ht="15.75" customHeight="1">
       <c r="B747" s="5"/>
     </row>
-    <row r="748" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="748" spans="2:2" ht="15.75" customHeight="1">
       <c r="B748" s="5"/>
     </row>
-    <row r="749" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="749" spans="2:2" ht="15.75" customHeight="1">
       <c r="B749" s="5"/>
     </row>
-    <row r="750" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="750" spans="2:2" ht="15.75" customHeight="1">
       <c r="B750" s="5"/>
     </row>
-    <row r="751" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="751" spans="2:2" ht="15.75" customHeight="1">
       <c r="B751" s="5"/>
     </row>
-    <row r="752" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="752" spans="2:2" ht="15.75" customHeight="1">
       <c r="B752" s="5"/>
     </row>
-    <row r="753" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="753" spans="2:2" ht="15.75" customHeight="1">
       <c r="B753" s="5"/>
     </row>
-    <row r="754" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="754" spans="2:2" ht="15.75" customHeight="1">
       <c r="B754" s="5"/>
     </row>
-    <row r="755" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="755" spans="2:2" ht="15.75" customHeight="1">
       <c r="B755" s="5"/>
     </row>
-    <row r="756" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="756" spans="2:2" ht="15.75" customHeight="1">
       <c r="B756" s="5"/>
     </row>
-    <row r="757" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="757" spans="2:2" ht="15.75" customHeight="1">
       <c r="B757" s="5"/>
     </row>
-    <row r="758" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="758" spans="2:2" ht="15.75" customHeight="1">
       <c r="B758" s="5"/>
     </row>
-    <row r="759" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="759" spans="2:2" ht="15.75" customHeight="1">
       <c r="B759" s="5"/>
     </row>
-    <row r="760" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="760" spans="2:2" ht="15.75" customHeight="1">
       <c r="B760" s="5"/>
     </row>
-    <row r="761" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="761" spans="2:2" ht="15.75" customHeight="1">
       <c r="B761" s="5"/>
     </row>
-    <row r="762" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="762" spans="2:2" ht="15.75" customHeight="1">
       <c r="B762" s="5"/>
     </row>
-    <row r="763" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="763" spans="2:2" ht="15.75" customHeight="1">
       <c r="B763" s="5"/>
     </row>
-    <row r="764" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="764" spans="2:2" ht="15.75" customHeight="1">
       <c r="B764" s="5"/>
     </row>
-    <row r="765" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="765" spans="2:2" ht="15.75" customHeight="1">
       <c r="B765" s="5"/>
     </row>
-    <row r="766" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="766" spans="2:2" ht="15.75" customHeight="1">
       <c r="B766" s="5"/>
     </row>
-    <row r="767" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="767" spans="2:2" ht="15.75" customHeight="1">
       <c r="B767" s="5"/>
     </row>
-    <row r="768" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="768" spans="2:2" ht="15.75" customHeight="1">
       <c r="B768" s="5"/>
     </row>
-    <row r="769" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="769" spans="2:2" ht="15.75" customHeight="1">
       <c r="B769" s="5"/>
     </row>
-    <row r="770" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="770" spans="2:2" ht="15.75" customHeight="1">
       <c r="B770" s="5"/>
     </row>
-    <row r="771" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="771" spans="2:2" ht="15.75" customHeight="1">
       <c r="B771" s="5"/>
     </row>
-    <row r="772" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="772" spans="2:2" ht="15.75" customHeight="1">
       <c r="B772" s="5"/>
     </row>
-    <row r="773" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="773" spans="2:2" ht="15.75" customHeight="1">
       <c r="B773" s="5"/>
     </row>
-    <row r="774" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="774" spans="2:2" ht="15.75" customHeight="1">
       <c r="B774" s="5"/>
     </row>
-    <row r="775" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="775" spans="2:2" ht="15.75" customHeight="1">
       <c r="B775" s="5"/>
     </row>
-    <row r="776" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="776" spans="2:2" ht="15.75" customHeight="1">
       <c r="B776" s="5"/>
     </row>
-    <row r="777" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="777" spans="2:2" ht="15.75" customHeight="1">
       <c r="B777" s="5"/>
     </row>
-    <row r="778" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="778" spans="2:2" ht="15.75" customHeight="1">
       <c r="B778" s="5"/>
     </row>
-    <row r="779" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="779" spans="2:2" ht="15.75" customHeight="1">
       <c r="B779" s="5"/>
     </row>
-    <row r="780" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="780" spans="2:2" ht="15.75" customHeight="1">
       <c r="B780" s="5"/>
     </row>
-    <row r="781" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="781" spans="2:2" ht="15.75" customHeight="1">
       <c r="B781" s="5"/>
     </row>
-    <row r="782" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="782" spans="2:2" ht="15.75" customHeight="1">
       <c r="B782" s="5"/>
     </row>
-    <row r="783" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="783" spans="2:2" ht="15.75" customHeight="1">
       <c r="B783" s="5"/>
     </row>
-    <row r="784" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="784" spans="2:2" ht="15.75" customHeight="1">
       <c r="B784" s="5"/>
     </row>
-    <row r="785" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="785" spans="2:2" ht="15.75" customHeight="1">
       <c r="B785" s="5"/>
     </row>
-    <row r="786" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="786" spans="2:2" ht="15.75" customHeight="1">
       <c r="B786" s="5"/>
     </row>
-    <row r="787" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="787" spans="2:2" ht="15.75" customHeight="1">
       <c r="B787" s="5"/>
     </row>
-    <row r="788" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="788" spans="2:2" ht="15.75" customHeight="1">
       <c r="B788" s="5"/>
     </row>
-    <row r="789" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="789" spans="2:2" ht="15.75" customHeight="1">
       <c r="B789" s="5"/>
     </row>
-    <row r="790" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="790" spans="2:2" ht="15.75" customHeight="1">
       <c r="B790" s="5"/>
     </row>
-    <row r="791" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="791" spans="2:2" ht="15.75" customHeight="1">
       <c r="B791" s="5"/>
     </row>
-    <row r="792" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="792" spans="2:2" ht="15.75" customHeight="1">
       <c r="B792" s="5"/>
     </row>
-    <row r="793" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="793" spans="2:2" ht="15.75" customHeight="1">
       <c r="B793" s="5"/>
     </row>
-    <row r="794" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="794" spans="2:2" ht="15.75" customHeight="1">
       <c r="B794" s="5"/>
     </row>
-    <row r="795" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="795" spans="2:2" ht="15.75" customHeight="1">
       <c r="B795" s="5"/>
     </row>
-    <row r="796" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="796" spans="2:2" ht="15.75" customHeight="1">
       <c r="B796" s="5"/>
     </row>
-    <row r="797" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="797" spans="2:2" ht="15.75" customHeight="1">
       <c r="B797" s="5"/>
     </row>
-    <row r="798" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="798" spans="2:2" ht="15.75" customHeight="1">
       <c r="B798" s="5"/>
     </row>
-    <row r="799" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="799" spans="2:2" ht="15.75" customHeight="1">
       <c r="B799" s="5"/>
     </row>
-    <row r="800" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="800" spans="2:2" ht="15.75" customHeight="1">
       <c r="B800" s="5"/>
     </row>
-    <row r="801" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="801" spans="2:2" ht="15.75" customHeight="1">
       <c r="B801" s="5"/>
     </row>
-    <row r="802" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="802" spans="2:2" ht="15.75" customHeight="1">
       <c r="B802" s="5"/>
     </row>
-    <row r="803" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="803" spans="2:2" ht="15.75" customHeight="1">
       <c r="B803" s="5"/>
     </row>
-    <row r="804" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="804" spans="2:2" ht="15.75" customHeight="1">
       <c r="B804" s="5"/>
     </row>
-    <row r="805" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="805" spans="2:2" ht="15.75" customHeight="1">
       <c r="B805" s="5"/>
     </row>
-    <row r="806" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="806" spans="2:2" ht="15.75" customHeight="1">
       <c r="B806" s="5"/>
     </row>
-    <row r="807" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="807" spans="2:2" ht="15.75" customHeight="1">
       <c r="B807" s="5"/>
     </row>
-    <row r="808" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="808" spans="2:2" ht="15.75" customHeight="1">
       <c r="B808" s="5"/>
     </row>
-    <row r="809" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="809" spans="2:2" ht="15.75" customHeight="1">
       <c r="B809" s="5"/>
     </row>
-    <row r="810" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="810" spans="2:2" ht="15.75" customHeight="1">
       <c r="B810" s="5"/>
     </row>
-    <row r="811" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="811" spans="2:2" ht="15.75" customHeight="1">
       <c r="B811" s="5"/>
     </row>
-    <row r="812" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="812" spans="2:2" ht="15.75" customHeight="1">
       <c r="B812" s="5"/>
     </row>
-    <row r="813" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="813" spans="2:2" ht="15.75" customHeight="1">
       <c r="B813" s="5"/>
     </row>
-    <row r="814" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="814" spans="2:2" ht="15.75" customHeight="1">
       <c r="B814" s="5"/>
     </row>
-    <row r="815" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="815" spans="2:2" ht="15.75" customHeight="1">
       <c r="B815" s="5"/>
     </row>
-    <row r="816" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="816" spans="2:2" ht="15.75" customHeight="1">
       <c r="B816" s="5"/>
     </row>
-    <row r="817" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="817" spans="2:2" ht="15.75" customHeight="1">
       <c r="B817" s="5"/>
     </row>
-    <row r="818" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="818" spans="2:2" ht="15.75" customHeight="1">
       <c r="B818" s="5"/>
     </row>
-    <row r="819" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="819" spans="2:2" ht="15.75" customHeight="1">
       <c r="B819" s="5"/>
     </row>
-    <row r="820" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="820" spans="2:2" ht="15.75" customHeight="1">
       <c r="B820" s="5"/>
     </row>
-    <row r="821" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="821" spans="2:2" ht="15.75" customHeight="1">
       <c r="B821" s="5"/>
     </row>
-    <row r="822" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="822" spans="2:2" ht="15.75" customHeight="1">
       <c r="B822" s="5"/>
     </row>
-    <row r="823" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="823" spans="2:2" ht="15.75" customHeight="1">
       <c r="B823" s="5"/>
     </row>
-    <row r="824" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="824" spans="2:2" ht="15.75" customHeight="1">
       <c r="B824" s="5"/>
     </row>
-    <row r="825" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="825" spans="2:2" ht="15.75" customHeight="1">
       <c r="B825" s="5"/>
     </row>
-    <row r="826" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="826" spans="2:2" ht="15.75" customHeight="1">
       <c r="B826" s="5"/>
     </row>
-    <row r="827" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="827" spans="2:2" ht="15.75" customHeight="1">
       <c r="B827" s="5"/>
     </row>
-    <row r="828" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="828" spans="2:2" ht="15.75" customHeight="1">
       <c r="B828" s="5"/>
     </row>
-    <row r="829" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="829" spans="2:2" ht="15.75" customHeight="1">
       <c r="B829" s="5"/>
     </row>
-    <row r="830" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="830" spans="2:2" ht="15.75" customHeight="1">
       <c r="B830" s="5"/>
     </row>
-    <row r="831" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="831" spans="2:2" ht="15.75" customHeight="1">
       <c r="B831" s="5"/>
     </row>
-    <row r="832" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="832" spans="2:2" ht="15.75" customHeight="1">
       <c r="B832" s="5"/>
     </row>
-    <row r="833" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="833" spans="2:2" ht="15.75" customHeight="1">
       <c r="B833" s="5"/>
     </row>
-    <row r="834" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="834" spans="2:2" ht="15.75" customHeight="1">
       <c r="B834" s="5"/>
     </row>
-    <row r="835" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="835" spans="2:2" ht="15.75" customHeight="1">
       <c r="B835" s="5"/>
     </row>
-    <row r="836" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="836" spans="2:2" ht="15.75" customHeight="1">
       <c r="B836" s="5"/>
     </row>
-    <row r="837" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="837" spans="2:2" ht="15.75" customHeight="1">
       <c r="B837" s="5"/>
     </row>
-    <row r="838" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="838" spans="2:2" ht="15.75" customHeight="1">
       <c r="B838" s="5"/>
     </row>
-    <row r="839" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="839" spans="2:2" ht="15.75" customHeight="1">
       <c r="B839" s="5"/>
     </row>
-    <row r="840" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="840" spans="2:2" ht="15.75" customHeight="1">
       <c r="B840" s="5"/>
     </row>
-    <row r="841" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="841" spans="2:2" ht="15.75" customHeight="1">
       <c r="B841" s="5"/>
     </row>
-    <row r="842" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="842" spans="2:2" ht="15.75" customHeight="1">
       <c r="B842" s="5"/>
     </row>
-    <row r="843" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="843" spans="2:2" ht="15.75" customHeight="1">
       <c r="B843" s="5"/>
     </row>
-    <row r="844" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="844" spans="2:2" ht="15.75" customHeight="1">
       <c r="B844" s="5"/>
     </row>
-    <row r="845" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="845" spans="2:2" ht="15.75" customHeight="1">
       <c r="B845" s="5"/>
     </row>
-    <row r="846" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="846" spans="2:2" ht="15.75" customHeight="1">
       <c r="B846" s="5"/>
     </row>
-    <row r="847" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="847" spans="2:2" ht="15.75" customHeight="1">
       <c r="B847" s="5"/>
     </row>
-    <row r="848" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="848" spans="2:2" ht="15.75" customHeight="1">
       <c r="B848" s="5"/>
     </row>
-    <row r="849" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="849" spans="2:2" ht="15.75" customHeight="1">
       <c r="B849" s="5"/>
     </row>
-    <row r="850" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="850" spans="2:2" ht="15.75" customHeight="1">
       <c r="B850" s="5"/>
     </row>
-    <row r="851" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="851" spans="2:2" ht="15.75" customHeight="1">
       <c r="B851" s="5"/>
     </row>
-    <row r="852" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="852" spans="2:2" ht="15.75" customHeight="1">
       <c r="B852" s="5"/>
     </row>
-    <row r="853" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="853" spans="2:2" ht="15.75" customHeight="1">
       <c r="B853" s="5"/>
     </row>
-    <row r="854" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="854" spans="2:2" ht="15.75" customHeight="1">
       <c r="B854" s="5"/>
     </row>
-    <row r="855" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="855" spans="2:2" ht="15.75" customHeight="1">
       <c r="B855" s="5"/>
     </row>
-    <row r="856" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="856" spans="2:2" ht="15.75" customHeight="1">
       <c r="B856" s="5"/>
     </row>
-    <row r="857" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="857" spans="2:2" ht="15.75" customHeight="1">
       <c r="B857" s="5"/>
     </row>
-    <row r="858" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="858" spans="2:2" ht="15.75" customHeight="1">
       <c r="B858" s="5"/>
     </row>
-    <row r="859" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="859" spans="2:2" ht="15.75" customHeight="1">
       <c r="B859" s="5"/>
     </row>
-    <row r="860" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="860" spans="2:2" ht="15.75" customHeight="1">
       <c r="B860" s="5"/>
     </row>
-    <row r="861" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="861" spans="2:2" ht="15.75" customHeight="1">
       <c r="B861" s="5"/>
     </row>
-    <row r="862" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="862" spans="2:2" ht="15.75" customHeight="1">
       <c r="B862" s="5"/>
     </row>
-    <row r="863" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="863" spans="2:2" ht="15.75" customHeight="1">
       <c r="B863" s="5"/>
     </row>
-    <row r="864" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="864" spans="2:2" ht="15.75" customHeight="1">
       <c r="B864" s="5"/>
     </row>
-    <row r="865" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="865" spans="2:2" ht="15.75" customHeight="1">
       <c r="B865" s="5"/>
     </row>
-    <row r="866" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="866" spans="2:2" ht="15.75" customHeight="1">
       <c r="B866" s="5"/>
     </row>
-    <row r="867" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="867" spans="2:2" ht="15.75" customHeight="1">
       <c r="B867" s="5"/>
     </row>
-    <row r="868" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="868" spans="2:2" ht="15.75" customHeight="1">
       <c r="B868" s="5"/>
     </row>
-    <row r="869" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="869" spans="2:2" ht="15.75" customHeight="1">
       <c r="B869" s="5"/>
     </row>
-    <row r="870" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="870" spans="2:2" ht="15.75" customHeight="1">
       <c r="B870" s="5"/>
     </row>
-    <row r="871" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="871" spans="2:2" ht="15.75" customHeight="1">
       <c r="B871" s="5"/>
     </row>
-    <row r="872" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="872" spans="2:2" ht="15.75" customHeight="1">
       <c r="B872" s="5"/>
     </row>
-    <row r="873" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="873" spans="2:2" ht="15.75" customHeight="1">
       <c r="B873" s="5"/>
     </row>
-    <row r="874" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="874" spans="2:2" ht="15.75" customHeight="1">
       <c r="B874" s="5"/>
     </row>
-    <row r="875" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="875" spans="2:2" ht="15.75" customHeight="1">
       <c r="B875" s="5"/>
     </row>
-    <row r="876" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="876" spans="2:2" ht="15.75" customHeight="1">
       <c r="B876" s="5"/>
     </row>
-    <row r="877" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="877" spans="2:2" ht="15.75" customHeight="1">
       <c r="B877" s="5"/>
     </row>
-    <row r="878" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="878" spans="2:2" ht="15.75" customHeight="1">
       <c r="B878" s="5"/>
     </row>
-    <row r="879" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="879" spans="2:2" ht="15.75" customHeight="1">
       <c r="B879" s="5"/>
     </row>
-    <row r="880" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="880" spans="2:2" ht="15.75" customHeight="1">
       <c r="B880" s="5"/>
     </row>
-    <row r="881" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="881" spans="2:2" ht="15.75" customHeight="1">
       <c r="B881" s="5"/>
     </row>
-    <row r="882" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="882" spans="2:2" ht="15.75" customHeight="1">
       <c r="B882" s="5"/>
     </row>
-    <row r="883" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="883" spans="2:2" ht="15.75" customHeight="1">
       <c r="B883" s="5"/>
     </row>
-    <row r="884" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="884" spans="2:2" ht="15.75" customHeight="1">
       <c r="B884" s="5"/>
     </row>
-    <row r="885" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="885" spans="2:2" ht="15.75" customHeight="1">
       <c r="B885" s="5"/>
     </row>
-    <row r="886" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="886" spans="2:2" ht="15.75" customHeight="1">
       <c r="B886" s="5"/>
     </row>
-    <row r="887" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="887" spans="2:2" ht="15.75" customHeight="1">
       <c r="B887" s="5"/>
     </row>
-    <row r="888" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="888" spans="2:2" ht="15.75" customHeight="1">
       <c r="B888" s="5"/>
     </row>
-    <row r="889" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="889" spans="2:2" ht="15.75" customHeight="1">
       <c r="B889" s="5"/>
     </row>
-    <row r="890" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="890" spans="2:2" ht="15.75" customHeight="1">
       <c r="B890" s="5"/>
     </row>
-    <row r="891" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="891" spans="2:2" ht="15.75" customHeight="1">
       <c r="B891" s="5"/>
     </row>
-    <row r="892" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="892" spans="2:2" ht="15.75" customHeight="1">
       <c r="B892" s="5"/>
     </row>
-    <row r="893" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="893" spans="2:2" ht="15.75" customHeight="1">
       <c r="B893" s="5"/>
     </row>
-    <row r="894" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="894" spans="2:2" ht="15.75" customHeight="1">
       <c r="B894" s="5"/>
     </row>
-    <row r="895" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="895" spans="2:2" ht="15.75" customHeight="1">
       <c r="B895" s="5"/>
     </row>
-    <row r="896" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="896" spans="2:2" ht="15.75" customHeight="1">
       <c r="B896" s="5"/>
     </row>
-    <row r="897" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="897" spans="2:2" ht="15.75" customHeight="1">
       <c r="B897" s="5"/>
     </row>
-    <row r="898" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="898" spans="2:2" ht="15.75" customHeight="1">
       <c r="B898" s="5"/>
     </row>
-    <row r="899" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="899" spans="2:2" ht="15.75" customHeight="1">
       <c r="B899" s="5"/>
     </row>
-    <row r="900" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="900" spans="2:2" ht="15.75" customHeight="1">
       <c r="B900" s="5"/>
     </row>
-    <row r="901" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="901" spans="2:2" ht="15.75" customHeight="1">
       <c r="B901" s="5"/>
     </row>
-    <row r="902" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="902" spans="2:2" ht="15.75" customHeight="1">
       <c r="B902" s="5"/>
     </row>
-    <row r="903" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="903" spans="2:2" ht="15.75" customHeight="1">
       <c r="B903" s="5"/>
     </row>
-    <row r="904" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="904" spans="2:2" ht="15.75" customHeight="1">
       <c r="B904" s="5"/>
     </row>
-    <row r="905" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="905" spans="2:2" ht="15.75" customHeight="1">
       <c r="B905" s="5"/>
     </row>
-    <row r="906" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="906" spans="2:2" ht="15.75" customHeight="1">
       <c r="B906" s="5"/>
     </row>
-    <row r="907" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="907" spans="2:2" ht="15.75" customHeight="1">
       <c r="B907" s="5"/>
     </row>
-    <row r="908" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="908" spans="2:2" ht="15.75" customHeight="1">
       <c r="B908" s="5"/>
     </row>
-    <row r="909" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="909" spans="2:2" ht="15.75" customHeight="1">
       <c r="B909" s="5"/>
     </row>
-    <row r="910" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="910" spans="2:2" ht="15.75" customHeight="1">
       <c r="B910" s="5"/>
     </row>
-    <row r="911" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="911" spans="2:2" ht="15.75" customHeight="1">
       <c r="B911" s="5"/>
     </row>
-    <row r="912" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="912" spans="2:2" ht="15.75" customHeight="1">
       <c r="B912" s="5"/>
     </row>
-    <row r="913" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="913" spans="2:2" ht="15.75" customHeight="1">
       <c r="B913" s="5"/>
     </row>
-    <row r="914" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="914" spans="2:2" ht="15.75" customHeight="1">
       <c r="B914" s="5"/>
     </row>
-    <row r="915" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="915" spans="2:2" ht="15.75" customHeight="1">
       <c r="B915" s="5"/>
     </row>
-    <row r="916" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="916" spans="2:2" ht="15.75" customHeight="1">
       <c r="B916" s="5"/>
     </row>
-    <row r="917" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="917" spans="2:2" ht="15.75" customHeight="1">
       <c r="B917" s="5"/>
     </row>
-    <row r="918" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="918" spans="2:2" ht="15.75" customHeight="1">
       <c r="B918" s="5"/>
     </row>
-    <row r="919" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="919" spans="2:2" ht="15.75" customHeight="1">
       <c r="B919" s="5"/>
     </row>
-    <row r="920" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="920" spans="2:2" ht="15.75" customHeight="1">
       <c r="B920" s="5"/>
     </row>
-    <row r="921" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="921" spans="2:2" ht="15.75" customHeight="1">
       <c r="B921" s="5"/>
     </row>
-    <row r="922" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="922" spans="2:2" ht="15.75" customHeight="1">
       <c r="B922" s="5"/>
     </row>
-    <row r="923" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="923" spans="2:2" ht="15.75" customHeight="1">
       <c r="B923" s="5"/>
     </row>
-    <row r="924" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="924" spans="2:2" ht="15.75" customHeight="1">
       <c r="B924" s="5"/>
     </row>
-    <row r="925" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="925" spans="2:2" ht="15.75" customHeight="1">
       <c r="B925" s="5"/>
     </row>
-    <row r="926" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="926" spans="2:2" ht="15.75" customHeight="1">
       <c r="B926" s="5"/>
     </row>
-    <row r="927" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="927" spans="2:2" ht="15.75" customHeight="1">
       <c r="B927" s="5"/>
     </row>
-    <row r="928" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="928" spans="2:2" ht="15.75" customHeight="1">
       <c r="B928" s="5"/>
     </row>
-    <row r="929" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="929" spans="2:2" ht="15.75" customHeight="1">
       <c r="B929" s="5"/>
     </row>
-    <row r="930" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="930" spans="2:2" ht="15.75" customHeight="1">
       <c r="B930" s="5"/>
     </row>
-    <row r="931" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="931" spans="2:2" ht="15.75" customHeight="1">
       <c r="B931" s="5"/>
     </row>
-    <row r="932" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="932" spans="2:2" ht="15.75" customHeight="1">
       <c r="B932" s="5"/>
     </row>
-    <row r="933" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="933" spans="2:2" ht="15.75" customHeight="1">
       <c r="B933" s="5"/>
     </row>
-    <row r="934" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="934" spans="2:2" ht="15.75" customHeight="1">
       <c r="B934" s="5"/>
     </row>
-    <row r="935" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="935" spans="2:2" ht="15.75" customHeight="1">
       <c r="B935" s="5"/>
     </row>
-    <row r="936" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="936" spans="2:2" ht="15.75" customHeight="1">
       <c r="B936" s="5"/>
     </row>
-    <row r="937" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="937" spans="2:2" ht="15.75" customHeight="1">
       <c r="B937" s="5"/>
     </row>
-    <row r="938" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="938" spans="2:2" ht="15.75" customHeight="1">
       <c r="B938" s="5"/>
     </row>
-    <row r="939" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="939" spans="2:2" ht="15.75" customHeight="1">
       <c r="B939" s="5"/>
     </row>
-    <row r="940" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="940" spans="2:2" ht="15.75" customHeight="1">
       <c r="B940" s="5"/>
     </row>
-    <row r="941" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="941" spans="2:2" ht="15.75" customHeight="1">
       <c r="B941" s="5"/>
     </row>
-    <row r="942" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="942" spans="2:2" ht="15.75" customHeight="1">
       <c r="B942" s="5"/>
     </row>
-    <row r="943" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="943" spans="2:2" ht="15.75" customHeight="1">
       <c r="B943" s="5"/>
     </row>
-    <row r="944" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="944" spans="2:2" ht="15.75" customHeight="1">
       <c r="B944" s="5"/>
     </row>
-    <row r="945" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="945" spans="2:2" ht="15.75" customHeight="1">
       <c r="B945" s="5"/>
     </row>
-    <row r="946" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="946" spans="2:2" ht="15.75" customHeight="1">
       <c r="B946" s="5"/>
     </row>
-    <row r="947" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="947" spans="2:2" ht="15.75" customHeight="1">
       <c r="B947" s="5"/>
     </row>
-    <row r="948" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="948" spans="2:2" ht="15.75" customHeight="1">
       <c r="B948" s="5"/>
     </row>
-    <row r="949" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="949" spans="2:2" ht="15.75" customHeight="1">
       <c r="B949" s="5"/>
     </row>
-    <row r="950" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="950" spans="2:2" ht="15.75" customHeight="1">
       <c r="B950" s="5"/>
     </row>
-    <row r="951" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="951" spans="2:2" ht="15.75" customHeight="1">
       <c r="B951" s="5"/>
     </row>
-    <row r="952" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="952" spans="2:2" ht="15.75" customHeight="1">
       <c r="B952" s="5"/>
     </row>
-    <row r="953" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="953" spans="2:2" ht="15.75" customHeight="1">
       <c r="B953" s="5"/>
     </row>
-    <row r="954" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="954" spans="2:2" ht="15.75" customHeight="1">
       <c r="B954" s="5"/>
     </row>
-    <row r="955" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="955" spans="2:2" ht="15.75" customHeight="1">
       <c r="B955" s="5"/>
     </row>
-    <row r="956" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="956" spans="2:2" ht="15.75" customHeight="1">
       <c r="B956" s="5"/>
     </row>
-    <row r="957" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="957" spans="2:2" ht="15.75" customHeight="1">
       <c r="B957" s="5"/>
     </row>
-    <row r="958" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="958" spans="2:2" ht="15.75" customHeight="1">
       <c r="B958" s="5"/>
     </row>
-    <row r="959" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="959" spans="2:2" ht="15.75" customHeight="1">
       <c r="B959" s="5"/>
     </row>
-    <row r="960" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="960" spans="2:2" ht="15.75" customHeight="1">
       <c r="B960" s="5"/>
     </row>
-    <row r="961" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="961" spans="2:2" ht="15.75" customHeight="1">
       <c r="B961" s="5"/>
     </row>
-    <row r="962" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="962" spans="2:2" ht="15.75" customHeight="1">
       <c r="B962" s="5"/>
     </row>
-    <row r="963" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="963" spans="2:2" ht="15.75" customHeight="1">
       <c r="B963" s="5"/>
     </row>
-    <row r="964" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="964" spans="2:2" ht="15.75" customHeight="1">
       <c r="B964" s="5"/>
     </row>
-    <row r="965" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="965" spans="2:2" ht="15.75" customHeight="1">
       <c r="B965" s="5"/>
     </row>
-    <row r="966" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="966" spans="2:2" ht="15.75" customHeight="1">
       <c r="B966" s="5"/>
     </row>
-    <row r="967" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="967" spans="2:2" ht="15.75" customHeight="1">
       <c r="B967" s="5"/>
     </row>
-    <row r="968" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="968" spans="2:2" ht="15.75" customHeight="1">
       <c r="B968" s="5"/>
     </row>
-    <row r="969" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="969" spans="2:2" ht="15.75" customHeight="1">
       <c r="B969" s="5"/>
     </row>
-    <row r="970" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="970" spans="2:2" ht="15.75" customHeight="1">
       <c r="B970" s="5"/>
     </row>
-    <row r="971" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="971" spans="2:2" ht="15.75" customHeight="1">
       <c r="B971" s="5"/>
     </row>
-    <row r="972" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="972" spans="2:2" ht="15.75" customHeight="1">
       <c r="B972" s="5"/>
     </row>
-    <row r="973" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="973" spans="2:2" ht="15.75" customHeight="1">
       <c r="B973" s="5"/>
     </row>
-    <row r="974" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="974" spans="2:2" ht="15.75" customHeight="1">
       <c r="B974" s="5"/>
     </row>
-    <row r="975" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="975" spans="2:2" ht="15.75" customHeight="1">
       <c r="B975" s="5"/>
     </row>
-    <row r="976" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="976" spans="2:2" ht="15.75" customHeight="1">
       <c r="B976" s="5"/>
     </row>
-    <row r="977" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="977" spans="2:2" ht="15.75" customHeight="1">
       <c r="B977" s="5"/>
     </row>
-    <row r="978" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="978" spans="2:2" ht="15.75" customHeight="1">
       <c r="B978" s="5"/>
     </row>
-    <row r="979" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="979" spans="2:2" ht="15.75" customHeight="1">
       <c r="B979" s="5"/>
     </row>
-    <row r="980" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="980" spans="2:2" ht="15.75" customHeight="1">
       <c r="B980" s="5"/>
     </row>
-    <row r="981" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="981" spans="2:2" ht="15.75" customHeight="1">
       <c r="B981" s="5"/>
     </row>
-    <row r="982" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="982" spans="2:2" ht="15.75" customHeight="1">
       <c r="B982" s="5"/>
     </row>
-    <row r="983" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="983" spans="2:2" ht="15.75" customHeight="1">
       <c r="B983" s="5"/>
     </row>
-    <row r="984" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="984" spans="2:2" ht="15.75" customHeight="1">
       <c r="B984" s="5"/>
     </row>
-    <row r="985" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="985" spans="2:2" ht="15.75" customHeight="1">
       <c r="B985" s="5"/>
     </row>
-    <row r="986" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="986" spans="2:2" ht="15.75" customHeight="1">
       <c r="B986" s="5"/>
     </row>
-    <row r="987" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="987" spans="2:2" ht="15.75" customHeight="1">
       <c r="B987" s="5"/>
     </row>
-    <row r="988" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="988" spans="2:2" ht="15.75" customHeight="1">
       <c r="B988" s="5"/>
     </row>
-    <row r="989" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="989" spans="2:2" ht="15.75" customHeight="1">
       <c r="B989" s="5"/>
     </row>
-    <row r="990" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="990" spans="2:2" ht="15.75" customHeight="1">
       <c r="B990" s="5"/>
     </row>
-    <row r="991" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="991" spans="2:2" ht="15.75" customHeight="1">
       <c r="B991" s="5"/>
     </row>
-    <row r="992" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="992" spans="2:2" ht="15.75" customHeight="1">
       <c r="B992" s="5"/>
     </row>
-    <row r="993" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="993" spans="2:2" ht="15.75" customHeight="1">
       <c r="B993" s="5"/>
     </row>
-    <row r="994" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="994" spans="2:2" ht="15.75" customHeight="1">
       <c r="B994" s="5"/>
     </row>
-    <row r="995" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="995" spans="2:2" ht="15.75" customHeight="1">
       <c r="B995" s="5"/>
     </row>
-    <row r="996" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="996" spans="2:2" ht="15.75" customHeight="1">
       <c r="B996" s="5"/>
     </row>
-    <row r="997" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="997" spans="2:2" ht="15.75" customHeight="1">
       <c r="B997" s="5"/>
     </row>
-    <row r="998" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="998" spans="2:2" ht="15.75" customHeight="1">
       <c r="B998" s="5"/>
     </row>
-    <row r="999" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="999" spans="2:2" ht="15.75" customHeight="1">
       <c r="B999" s="5"/>
     </row>
-    <row r="1000" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1000" spans="2:2" ht="15.75" customHeight="1">
       <c r="B1000" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IH-260 Update excel column names
</commit_message>
<xml_diff>
--- a/src/main/resources/법인 회원 업로드.xlsx
+++ b/src/main/resources/법인 회원 업로드.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A8A33E91-5CFA-48AA-82A6-E2052996E08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03391784-857C-4799-918B-B9E94EA43427}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A8A33E91-5CFA-48AA-82A6-E2052996E08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7332485F-8103-48E4-BC7E-FE34B9D689A0}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <t>가격</t>
   </si>
   <si>
-    <t>지불 날짜 (YYYY-MM-DD)</t>
+    <t>결제일자 (YYYY-MM-DD)</t>
   </si>
   <si>
     <t>이름</t>
@@ -342,7 +342,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>

</xml_diff>